<commit_message>
Removed "Transcript URL" header
</commit_message>
<xml_diff>
--- a/data/transcripts_urls.xlsx
+++ b/data/transcripts_urls.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stuti\Desktop\Northeastern University\Academics\Semesters\Sem-4\NLP\NLP_Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Proton Drive\My files\NEU Documents\Projects (Personal)\Projects\Humor-Analysis---NLP\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C565F046-2CFA-418B-A63B-2045FD962857}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD020A48-EB28-431D-8CB6-749D03702DF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{85CC9304-FA11-446F-BB0A-C4F1A4670BA4}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="475">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="474">
   <si>
     <t>PETE HOLMES: I AM NOT FOR EVERYONE (2023) | TRANSCRIPT</t>
   </si>
@@ -1444,9 +1444,6 @@
   </si>
   <si>
     <t>GEORGE CARLIN: IT’S BAD FOR YA (2008) FULL TRANSCRIPT</t>
-  </si>
-  <si>
-    <t>Transcript Links</t>
   </si>
   <si>
     <t>URL</t>
@@ -1518,9 +1515,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1558,7 +1555,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1664,7 +1661,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1806,7 +1803,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1814,13 +1811,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A5831E2-CEA7-4E89-A4AD-342BF57F2E79}">
-  <dimension ref="A1:A475"/>
+  <dimension ref="A1:A474"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="21.21875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -1828,2850 +1828,2845 @@
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>474</v>
+      <c r="A2" s="1" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A102" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A103" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A104" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A105" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A106" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A107" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A108" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A109" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A110" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A111" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A112" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A113" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A114" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A115" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A116" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A117" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A118" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A119" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A120" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A121" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A122" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A123" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A124" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A125" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A126" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A127" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A128" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A129" s="1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A130" s="1" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A131" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A132" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A133" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A134" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A135" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A136" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A137" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A138" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A139" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A140" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A141" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A142" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A143" s="1" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A144" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A145" s="1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A146" s="1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A147" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A148" s="1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A149" s="1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A150" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A151" s="1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A152" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A153" s="1" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A154" s="1" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A155" s="1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A156" s="1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A157" s="1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A158" s="1" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A159" s="1" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A160" s="1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A161" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A162" s="1" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A163" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A164" s="1" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A165" s="1" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A166" s="1" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A167" s="1" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A168" s="1" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A169" s="1" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A170" s="1" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A171" s="1" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A172" s="1" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A173" s="1" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A174" s="1" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A175" s="1" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A176" s="1" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A177" s="1" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A178" s="1" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A179" s="1" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A180" s="1" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A181" s="1" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A182" s="1" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A183" s="1" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A184" s="1" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A185" s="1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A186" s="1" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A187" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A188" s="1" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A189" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A190" s="1" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A191" s="1" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A192" s="1" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A193" s="1" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A194" s="1" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A195" s="1" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A196" s="1" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A197" s="1" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A198" s="1" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A199" s="1" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A200" s="1" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="201" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A201" s="1" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="202" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A202" s="1" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="203" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A203" s="1" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="204" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A204" s="1" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="205" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A205" s="1" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="206" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A206" s="1" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="207" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A207" s="1" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row r="208" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A208" s="1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="209" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A209" s="1" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="210" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A210" s="1" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="211" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A211" s="1" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="212" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A212" s="1" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="213" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A213" s="1" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="214" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A214" s="1" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="215" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A215" s="1" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="216" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A216" s="1" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="217" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A217" s="1" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="218" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A218" s="1" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="219" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A219" s="1" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="220" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A220" s="1" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="221" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A221" s="1" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="222" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A222" s="1" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
     </row>
     <row r="223" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A223" s="1" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="224" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A224" s="1" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
     <row r="225" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A225" s="1" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
     </row>
     <row r="226" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A226" s="1" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="227" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A227" s="1" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="228" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A228" s="1" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
     </row>
     <row r="229" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A229" s="1" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="230" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A230" s="1" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
     </row>
     <row r="231" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A231" s="1" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="232" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A232" s="1" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="233" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A233" s="1" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="234" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A234" s="1" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="235" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A235" s="1" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="236" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A236" s="1" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
     </row>
     <row r="237" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A237" s="1" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="238" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A238" s="1" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="239" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A239" s="1" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="240" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A240" s="1" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="241" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A241" s="1" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="242" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A242" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
     </row>
     <row r="243" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A243" s="1" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="244" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A244" s="1" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="245" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A245" s="1" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="246" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A246" s="1" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="247" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A247" s="1" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="248" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A248" s="1" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="249" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A249" s="1" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="250" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A250" s="1" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="251" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A251" s="1" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="252" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A252" s="1" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="253" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A253" s="1" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
     </row>
     <row r="254" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A254" s="1" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
     </row>
     <row r="255" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A255" s="1" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
     </row>
     <row r="256" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A256" s="1" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="257" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A257" s="1" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
     <row r="258" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A258" s="1" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="259" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A259" s="1" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
     </row>
     <row r="260" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A260" s="1" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="261" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A261" s="1" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="262" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A262" s="1" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="263" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A263" s="1" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="264" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A264" s="1" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="265" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A265" s="1" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="266" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A266" s="1" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="267" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A267" s="1" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="268" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A268" s="1" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="269" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A269" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="270" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A270" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="271" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A271" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="272" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A272" s="1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="273" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A273" s="1" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="274" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A274" s="1" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="275" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A275" s="1" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="276" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A276" s="1" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="277" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A277" s="1" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="278" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A278" s="1" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="279" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A279" s="1" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="280" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A280" s="1" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="281" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A281" s="1" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="282" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A282" s="1" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="283" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A283" s="1" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
     </row>
     <row r="284" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A284" s="1" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="285" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A285" s="1" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
     </row>
     <row r="286" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A286" s="1" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
     <row r="287" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A287" s="1" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="288" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A288" s="1" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
     </row>
     <row r="289" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A289" s="1" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="290" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A290" s="1" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="291" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A291" s="1" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
     <row r="292" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A292" s="1" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
     </row>
     <row r="293" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A293" s="1" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
     </row>
     <row r="294" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A294" s="1" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="295" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A295" s="1" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
     </row>
     <row r="296" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A296" s="1" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
     </row>
     <row r="297" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A297" s="1" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
     </row>
     <row r="298" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A298" s="1" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="299" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A299" s="1" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
     </row>
     <row r="300" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A300" s="1" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
     </row>
     <row r="301" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A301" s="1" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
     </row>
     <row r="302" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A302" s="1" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
     </row>
     <row r="303" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A303" s="1" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
     </row>
     <row r="304" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A304" s="1" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="305" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A305" s="1" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
     </row>
     <row r="306" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A306" s="1" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
     </row>
     <row r="307" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A307" s="1" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
     </row>
     <row r="308" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A308" s="1" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
     </row>
     <row r="309" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A309" s="1" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
     </row>
     <row r="310" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A310" s="1" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
     </row>
     <row r="311" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A311" s="1" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
     </row>
     <row r="312" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A312" s="1" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
     </row>
     <row r="313" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A313" s="1" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
     </row>
     <row r="314" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A314" s="1" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="315" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A315" s="1" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
     </row>
     <row r="316" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A316" s="1" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
     </row>
     <row r="317" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A317" s="1" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
     </row>
     <row r="318" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A318" s="1" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
     </row>
     <row r="319" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A319" s="1" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="320" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A320" s="1" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
     </row>
     <row r="321" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A321" s="1" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
     </row>
     <row r="322" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A322" s="1" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
     </row>
     <row r="323" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A323" s="1" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
     </row>
     <row r="324" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A324" s="1" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
     </row>
     <row r="325" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A325" s="1" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
     </row>
     <row r="326" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A326" s="1" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
     </row>
     <row r="327" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A327" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
     </row>
     <row r="328" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A328" s="1" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
     <row r="329" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A329" s="1" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
     </row>
     <row r="330" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A330" s="1" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
     </row>
     <row r="331" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A331" s="1" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
     </row>
     <row r="332" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A332" s="1" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
     </row>
     <row r="333" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A333" s="1" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
     </row>
     <row r="334" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A334" s="1" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
     </row>
     <row r="335" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A335" s="1" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
     </row>
     <row r="336" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A336" s="1" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
     </row>
     <row r="337" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A337" s="1" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
     </row>
     <row r="338" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A338" s="1" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
     </row>
     <row r="339" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A339" s="1" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
     </row>
     <row r="340" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A340" s="1" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
     </row>
     <row r="341" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A341" s="1" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
     </row>
     <row r="342" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A342" s="1" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
     </row>
     <row r="343" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A343" s="1" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
     </row>
     <row r="344" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A344" s="1" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
     </row>
     <row r="345" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A345" s="1" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
     </row>
     <row r="346" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A346" s="1" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="347" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A347" s="1" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
     </row>
     <row r="348" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A348" s="1" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
     </row>
     <row r="349" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A349" s="1" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
     </row>
     <row r="350" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A350" s="1" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="351" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A351" s="1" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
     </row>
     <row r="352" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A352" s="1" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="353" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A353" s="1" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
     </row>
     <row r="354" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A354" s="1" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
     </row>
     <row r="355" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A355" s="1" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
     </row>
     <row r="356" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A356" s="1" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
     </row>
     <row r="357" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A357" s="1" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
     </row>
     <row r="358" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A358" s="1" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
     </row>
     <row r="359" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A359" s="1" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
     </row>
     <row r="360" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A360" s="1" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
     </row>
     <row r="361" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A361" s="1" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
     </row>
     <row r="362" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A362" s="1" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
     </row>
     <row r="363" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A363" s="1" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
     </row>
     <row r="364" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A364" s="1" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
     </row>
     <row r="365" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A365" s="1" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
     </row>
     <row r="366" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A366" s="1" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
     </row>
     <row r="367" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A367" s="1" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
     </row>
     <row r="368" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A368" s="1" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
     </row>
     <row r="369" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A369" s="1" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
     </row>
     <row r="370" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A370" s="1" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
     </row>
     <row r="371" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A371" s="1" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
     </row>
     <row r="372" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A372" s="1" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
     </row>
     <row r="373" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A373" s="1" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
     </row>
     <row r="374" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A374" s="1" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
     </row>
     <row r="375" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A375" s="1" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
     </row>
     <row r="376" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A376" s="1" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
     </row>
     <row r="377" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A377" s="1" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
     </row>
     <row r="378" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A378" s="1" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
     </row>
     <row r="379" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A379" s="1" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
     </row>
     <row r="380" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A380" s="1" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
     </row>
     <row r="381" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A381" s="1" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
     </row>
     <row r="382" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A382" s="1" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
     </row>
     <row r="383" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A383" s="1" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
     </row>
     <row r="384" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A384" s="1" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
     </row>
     <row r="385" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A385" s="1" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
     </row>
     <row r="386" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A386" s="1" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="387" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A387" s="1" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
     </row>
     <row r="388" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A388" s="1" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
     </row>
     <row r="389" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A389" s="1" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
     </row>
     <row r="390" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A390" s="1" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
     </row>
     <row r="391" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A391" s="1" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
     </row>
     <row r="392" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A392" s="1" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
     </row>
     <row r="393" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A393" s="1" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
     </row>
     <row r="394" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A394" s="1" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
     </row>
     <row r="395" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A395" s="1" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
     </row>
     <row r="396" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A396" s="1" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
     </row>
     <row r="397" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A397" s="1" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
     </row>
     <row r="398" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A398" s="1" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="399" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A399" s="1" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
     </row>
     <row r="400" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A400" s="1" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
     </row>
     <row r="401" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A401" s="1" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
     </row>
     <row r="402" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A402" s="1" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
     </row>
     <row r="403" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A403" s="1" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
     </row>
     <row r="404" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A404" s="1" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
     </row>
     <row r="405" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A405" s="1" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
     </row>
     <row r="406" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A406" s="1" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
     </row>
     <row r="407" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A407" s="1" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
     </row>
     <row r="408" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A408" s="1" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
     </row>
     <row r="409" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A409" s="1" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
     </row>
     <row r="410" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A410" s="1" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
     </row>
     <row r="411" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A411" s="1" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
     </row>
     <row r="412" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A412" s="1" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="413" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A413" s="1" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
     </row>
     <row r="414" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A414" s="1" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
     </row>
     <row r="415" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A415" s="1" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
     </row>
     <row r="416" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A416" s="1" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
     </row>
     <row r="417" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A417" s="1" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
     </row>
     <row r="418" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A418" s="1" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
     </row>
     <row r="419" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A419" s="1" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
     </row>
     <row r="420" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A420" s="1" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
     </row>
     <row r="421" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A421" s="1" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
     </row>
     <row r="422" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A422" s="1" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="423" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A423" s="1" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
     </row>
     <row r="424" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A424" s="1" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
     </row>
     <row r="425" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A425" s="1" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
     </row>
     <row r="426" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A426" s="1" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
     </row>
     <row r="427" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A427" s="1" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
     </row>
     <row r="428" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A428" s="1" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
     </row>
     <row r="429" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A429" s="1" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
     </row>
     <row r="430" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A430" s="1" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
     </row>
     <row r="431" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A431" s="1" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
     </row>
     <row r="432" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A432" s="1" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
     </row>
     <row r="433" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A433" s="1" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
     </row>
     <row r="434" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A434" s="1" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
     </row>
     <row r="435" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A435" s="1" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
     </row>
     <row r="436" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A436" s="1" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
     </row>
     <row r="437" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A437" s="1" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
     </row>
     <row r="438" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A438" s="1" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
     </row>
     <row r="439" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A439" s="1" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
     </row>
     <row r="440" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A440" s="1" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
     </row>
     <row r="441" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A441" s="1" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
     </row>
     <row r="442" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A442" s="1" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
     </row>
     <row r="443" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A443" s="1" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
     </row>
     <row r="444" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A444" s="1" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
     </row>
     <row r="445" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A445" s="1" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
     </row>
     <row r="446" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A446" s="1" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
     </row>
     <row r="447" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A447" s="1" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
     </row>
     <row r="448" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A448" s="1" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
     </row>
     <row r="449" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A449" s="1" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
     </row>
     <row r="450" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A450" s="1" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
     </row>
     <row r="451" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A451" s="1" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
     </row>
     <row r="452" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A452" s="1" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
     </row>
     <row r="453" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A453" s="1" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
     </row>
     <row r="454" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A454" s="1" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
     </row>
     <row r="455" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A455" s="1" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
     </row>
     <row r="456" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A456" s="1" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
     </row>
     <row r="457" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A457" s="1" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
     </row>
     <row r="458" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A458" s="1" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
     </row>
     <row r="459" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A459" s="1" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
     </row>
     <row r="460" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A460" s="1" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="461" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A461" s="1" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
     </row>
     <row r="462" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A462" s="1" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
     </row>
     <row r="463" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A463" s="1" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
     </row>
     <row r="464" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A464" s="1" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
     </row>
     <row r="465" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A465" s="1" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
     </row>
     <row r="466" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A466" s="1" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
     </row>
     <row r="467" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A467" s="1" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
     </row>
     <row r="468" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A468" s="1" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
     </row>
     <row r="469" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A469" s="1" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
     </row>
     <row r="470" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A470" s="1" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
     </row>
     <row r="471" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A471" s="1" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
     </row>
     <row r="472" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A472" s="1" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
     </row>
     <row r="473" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A473" s="1" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
     </row>
     <row r="474" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A474" s="1" t="s">
-        <v>471</v>
-      </c>
-    </row>
-    <row r="475" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A475" s="1" t="s">
         <v>472</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A3" r:id="rId1" display="https://scrapsfromtheloft.com/comedy/pete-holmes-i-am-not-for-everyone-transcript/" xr:uid="{5A1D765B-06A2-49FE-BDA4-2A5B993608A1}"/>
-    <hyperlink ref="A4" r:id="rId2" display="https://scrapsfromtheloft.com/comedy/jeff-dunham-im-with-cupid-transcript/" xr:uid="{B0B29DFB-ABDE-4008-8EA5-1D27FE82B09B}"/>
-    <hyperlink ref="A5" r:id="rId3" display="https://scrapsfromtheloft.com/comedy/taylor-tomlinson-have-it-all-transcript/" xr:uid="{103F827F-24EC-4689-9102-48B055EF2FDD}"/>
-    <hyperlink ref="A6" r:id="rId4" display="https://scrapsfromtheloft.com/comedy/kevin-bridges-overdue-catch-up-transcript/" xr:uid="{A7F568A5-11B6-46D3-B2D9-7C87DA717B0A}"/>
-    <hyperlink ref="A7" r:id="rId5" display="https://scrapsfromtheloft.com/comedy/jacqueline-novak-get-on-your-knees-transcript/" xr:uid="{7692E464-8943-4D84-BA2B-5363B730D1C1}"/>
-    <hyperlink ref="A8" r:id="rId6" display="https://scrapsfromtheloft.com/comedy/kelsey-cook-the-hustler-transcript/" xr:uid="{9693B817-5A06-444C-82D3-BBAC48918F51}"/>
-    <hyperlink ref="A9" r:id="rId7" display="https://scrapsfromtheloft.com/comedy/dylan-moran-yeah-yeah-2011-transcript/" xr:uid="{51C0208E-82FD-4991-8787-A7270417625A}"/>
-    <hyperlink ref="A10" r:id="rId8" display="https://scrapsfromtheloft.com/comedy/dusty-slay-workin-man-transcript/" xr:uid="{B6E212AE-B1D2-45ED-A04A-3FCB565E9B1A}"/>
-    <hyperlink ref="A11" r:id="rId9" display="https://scrapsfromtheloft.com/comedy/jack-whitehall-settle-down-transcript/" xr:uid="{26C5255C-0209-41E5-B84E-FB020AE7AB14}"/>
-    <hyperlink ref="A12" r:id="rId10" display="https://scrapsfromtheloft.com/comedy/dylan-moran-what-it-is-transcript/" xr:uid="{99F33C3C-7B79-42F9-B96E-7A881B9E13F8}"/>
-    <hyperlink ref="A13" r:id="rId11" display="https://scrapsfromtheloft.com/comedy/kevin-james-irregardless-transcript/" xr:uid="{F48C2FB9-816C-40EC-97C0-279F70009A5C}"/>
-    <hyperlink ref="A14" r:id="rId12" display="https://scrapsfromtheloft.com/comedy/pete-davidson-turbo-fonzarelli-transcript/" xr:uid="{5CE31BAE-8266-47A7-945A-9514347478FE}"/>
-    <hyperlink ref="A15" r:id="rId13" display="https://scrapsfromtheloft.com/comedy/david-nihill-cultural-appreciation-transcript/" xr:uid="{1940523D-A103-423C-982F-4408D8A68B61}"/>
-    <hyperlink ref="A16" r:id="rId14" display="https://scrapsfromtheloft.com/comedy/matt-rife-matthew-steven-rife-transcript/" xr:uid="{D51A4658-261A-46B4-9F25-46142BEF6822}"/>
-    <hyperlink ref="A17" r:id="rId15" display="https://scrapsfromtheloft.com/comedy/shane-gillis-live-in-austin-transcript/" xr:uid="{1D73F476-BE79-4BC3-92AF-9A8F66F2A4FF}"/>
-    <hyperlink ref="A18" r:id="rId16" display="https://scrapsfromtheloft.com/comedy/lewis-black-tragically-i-need-you-transcript/" xr:uid="{EA61EA08-68B7-46DD-83B7-7D4B1F3E4B7B}"/>
-    <hyperlink ref="A19" r:id="rId17" display="https://scrapsfromtheloft.com/comedy/stavros-halkias-live-at-the-lodge-room-transcript/" xr:uid="{582622BF-6C06-4DBC-A8B0-37B7F6C2CE3C}"/>
-    <hyperlink ref="A20" r:id="rId18" display="https://scrapsfromtheloft.com/comedy/george-carlin-im-glad-im-dead-transcript/" xr:uid="{02F33CE5-BA29-4A86-B762-870B1F6EEF9F}"/>
-    <hyperlink ref="A21" r:id="rId19" display="https://scrapsfromtheloft.com/comedy/leanne-morgan-im-every-woman-transcript/" xr:uid="{4427E684-5AD4-4694-BF68-0AEE8840C6E9}"/>
-    <hyperlink ref="A22" r:id="rId20" display="https://scrapsfromtheloft.com/comedy/louis-ck-at-the-dolby-transcript/" xr:uid="{6FA7854F-995C-4C0C-983E-1A1D07543902}"/>
-    <hyperlink ref="A23" r:id="rId21" display="https://scrapsfromtheloft.com/comedy/roseanne-barr-cancel-this-transcript/" xr:uid="{B56BFF6C-BC17-4945-9A51-407389636B4F}"/>
-    <hyperlink ref="A24" r:id="rId22" display="https://scrapsfromtheloft.com/comedy/sammy-obeid-martyr-in-safe-space-transcript/" xr:uid="{E053EB31-A7E0-4BAC-94BC-CFA67D54C679}"/>
-    <hyperlink ref="A25" r:id="rId23" display="https://scrapsfromtheloft.com/comedy/sammy-obeid-where-is-bethlehem-transcript/" xr:uid="{0781BE37-A90C-4EFF-B6AB-BD942D928BE1}"/>
-    <hyperlink ref="A26" r:id="rId24" display="https://scrapsfromtheloft.com/comedy/sammy-obeid-palestine-censorship/" xr:uid="{A0E040FC-4C5A-42B1-92EE-E14DFA88EA17}"/>
-    <hyperlink ref="A27" r:id="rId25" display="https://scrapsfromtheloft.com/comedy/sammy-obeid-on-palestine-transcript/" xr:uid="{569C38DA-EC81-45C9-9D13-5D49CD798BA6}"/>
-    <hyperlink ref="A28" r:id="rId26" display="https://scrapsfromtheloft.com/comedy/dave-chappelle-the-dreamer-transcript/" xr:uid="{27D0EDF7-371E-4081-8012-1149BC40FD17}"/>
-    <hyperlink ref="A29" r:id="rId27" display="https://scrapsfromtheloft.com/comedy/gary-gulman-the-great-depresh-transcript/" xr:uid="{AB838C74-6B13-4A97-8594-550D7EC88590}"/>
-    <hyperlink ref="A30" r:id="rId28" display="https://scrapsfromtheloft.com/comedy/ricky-gervais-armageddon-transcript/" xr:uid="{CF928857-29C4-448A-89DB-6DDF81E06B1F}"/>
-    <hyperlink ref="A31" r:id="rId29" display="https://scrapsfromtheloft.com/comedy/gary-gulman-its-about-time-transcript/" xr:uid="{E589B5B6-FA85-42C2-8699-5091A348A3D4}"/>
-    <hyperlink ref="A32" r:id="rId30" display="https://scrapsfromtheloft.com/comedy/gary-gulman-born-on-3rd-base-transcript/" xr:uid="{CC303E0C-EBB7-4052-896A-EC5BFBF5EBC6}"/>
-    <hyperlink ref="A33" r:id="rId31" display="https://scrapsfromtheloft.com/comedy/trevor-noah-where-was-i-transcript/" xr:uid="{33A79624-DC03-411A-97C5-17B2085CF5B8}"/>
-    <hyperlink ref="A34" r:id="rId32" display="https://scrapsfromtheloft.com/comedy/maria-bamford-special-special-special-transcript/" xr:uid="{B9DAB39D-FD11-4D40-AD2D-32D6127E1EC4}"/>
-    <hyperlink ref="A35" r:id="rId33" display="https://scrapsfromtheloft.com/comedy/david-cross-making-america-great-again-transcript/" xr:uid="{EF0290DD-065D-4037-B470-2160A6C12B3B}"/>
-    <hyperlink ref="A36" r:id="rId34" display="https://scrapsfromtheloft.com/comedy/matt-rife-natural-selection-transcript/" xr:uid="{320771BD-7579-4BF6-9F7F-979102D48CA1}"/>
-    <hyperlink ref="A37" r:id="rId35" display="https://scrapsfromtheloft.com/comedy/mike-birbiglia-old-man-and-pool-transcript/" xr:uid="{E99853AA-59BE-4441-A5B0-C320A0FDABF5}"/>
-    <hyperlink ref="A38" r:id="rId36" display="https://scrapsfromtheloft.com/comedy/beth-stelling-girl-daddy-transcript/" xr:uid="{275BD693-9A5A-4FB9-B2B9-537E1F490AD1}"/>
-    <hyperlink ref="A39" r:id="rId37" display="https://scrapsfromtheloft.com/comedy/beth-stelling-if-you-didnt-want-me-then-transcript/" xr:uid="{72F3D415-3E9A-4990-BDA5-181C8D678160}"/>
-    <hyperlink ref="A40" r:id="rId38" display="https://scrapsfromtheloft.com/comedy/michelle-wolf-its-great-to-be-here-transcript/" xr:uid="{44AB3F1A-BBB5-4C8B-94D4-815367BC2688}"/>
-    <hyperlink ref="A41" r:id="rId39" display="https://scrapsfromtheloft.com/comedy/andrew-santino-home-field-advantage-transcript/" xr:uid="{0270D451-5285-49E4-8C4B-837684C2EC71}"/>
-    <hyperlink ref="A42" r:id="rId40" display="https://scrapsfromtheloft.com/comedy/shane-gillis-beautiful-dogs-transcript/" xr:uid="{56ACA4F0-CFA1-497D-834C-901B1AF627D2}"/>
-    <hyperlink ref="A43" r:id="rId41" display="https://scrapsfromtheloft.com/comedy/andrew-santino-cheeseburger-transcript/" xr:uid="{A43D24A2-35FA-407F-B732-16F165F13022}"/>
-    <hyperlink ref="A44" r:id="rId42" display="https://scrapsfromtheloft.com/comedy/jared-freid-37-and-single-transcript/" xr:uid="{3EECE32C-5C51-42C4-85D7-D886F0D7959D}"/>
-    <hyperlink ref="A45" r:id="rId43" display="https://scrapsfromtheloft.com/comedy/jim-gaffigan-dark-pale-transcript/" xr:uid="{95D28C6D-D32C-465C-AB48-B07BB786CE3C}"/>
-    <hyperlink ref="A46" r:id="rId44" display="https://scrapsfromtheloft.com/comedy/jim-gaffigan-obsessed-transcript/" xr:uid="{71868F17-B803-43BD-BC70-C708FEB639E3}"/>
-    <hyperlink ref="A47" r:id="rId45" display="https://scrapsfromtheloft.com/comedy/mark-normand-soup-to-nuts-transcript/" xr:uid="{658766F7-447D-4C30-8CF9-11BC39E4A0F0}"/>
-    <hyperlink ref="A48" r:id="rId46" display="https://scrapsfromtheloft.com/comedy/tom-segura-sledgehammer-transcript/" xr:uid="{130B2024-145A-451E-97A1-0802F0C7956D}"/>
-    <hyperlink ref="A49" r:id="rId47" display="https://scrapsfromtheloft.com/comedy/eddie-izzard-force-majeure-live-transcript/" xr:uid="{F3441139-8832-4351-AA7E-9D2B0DD5FFDC}"/>
-    <hyperlink ref="A50" r:id="rId48" display="https://scrapsfromtheloft.com/comedy/marlon-wayans-you-know-what-it-is-transcript/" xr:uid="{138144C1-6447-4473-BECA-FD472F1189AC}"/>
-    <hyperlink ref="A51" r:id="rId49" display="https://scrapsfromtheloft.com/comedy/kyle-kinane-whiskey-icarus-transcript/" xr:uid="{E7270BCC-027B-4611-8931-FCF01FF6C861}"/>
-    <hyperlink ref="A52" r:id="rId50" display="https://scrapsfromtheloft.com/comedy/kyle-kinane-loose-in-chicago-transcript/" xr:uid="{20A7F931-8E28-4282-BC06-AC6144F259DC}"/>
-    <hyperlink ref="A53" r:id="rId51" display="https://scrapsfromtheloft.com/comedy/mae-martin-sap-transcript/" xr:uid="{8CB7D3C9-4EA1-41C0-B0B7-1CEBE17E1B66}"/>
-    <hyperlink ref="A54" r:id="rId52" display="https://scrapsfromtheloft.com/comedy/amy-schumer-emergency-contact-transcript/" xr:uid="{23C89BD9-C383-4ED2-8C5A-B4EF9E232564}"/>
-    <hyperlink ref="A55" r:id="rId53" display="https://scrapsfromtheloft.com/comedy/wanda-sykes-im-an-entertainer-transcript/" xr:uid="{5879064C-47CD-43B0-91C1-EA1F1B1DCB19}"/>
-    <hyperlink ref="A56" r:id="rId54" display="https://scrapsfromtheloft.com/comedy/john-mulaney-baby-j-transcript/" xr:uid="{01979D08-EE3E-4054-B8DD-E0C091F9300F}"/>
-    <hyperlink ref="A57" r:id="rId55" display="https://scrapsfromtheloft.com/comedy/kathleen-madigan-hunting-bigfoot-transcript/" xr:uid="{5241BA9A-2293-48AF-8CC0-49D7E9C26709}"/>
-    <hyperlink ref="A58" r:id="rId56" display="https://scrapsfromtheloft.com/comedy/marc-maron-from-bleak-to-dark-transcript/" xr:uid="{003AD07F-770F-45EF-8F2F-643268147328}"/>
-    <hyperlink ref="A59" r:id="rId57" display="https://scrapsfromtheloft.com/comedy/bert-kreischer-razzle-dazzle-transcript/" xr:uid="{A0DC67F6-22C8-42CF-80BA-CBC6A2A5DD78}"/>
-    <hyperlink ref="A60" r:id="rId58" display="https://scrapsfromtheloft.com/comedy/chris-rock-selective-outrage-transcript/" xr:uid="{E76CD361-0D9B-4D87-88FC-C28102BDA6D7}"/>
-    <hyperlink ref="A61" r:id="rId59" display="https://scrapsfromtheloft.com/comedy/marc-maron-thinky-pain-transcript/" xr:uid="{B7C6A84F-1BC8-46ED-9505-768A8411E813}"/>
-    <hyperlink ref="A62" r:id="rId60" display="https://scrapsfromtheloft.com/comedy/chelsea-handler-evolution-transcript/" xr:uid="{119F2563-F9C6-4204-9AF9-750553FA1FDE}"/>
-    <hyperlink ref="A63" r:id="rId61" display="https://scrapsfromtheloft.com/comedy/tom-papa-what-a-day-transcript/" xr:uid="{F588BA02-5EBF-4767-84C4-94B8C2AF9983}"/>
-    <hyperlink ref="A64" r:id="rId62" display="https://scrapsfromtheloft.com/comedy/jim-jefferies-high-n-dry-transcript/" xr:uid="{7B8E60CD-6566-4020-A48C-0BF3A94DC8C1}"/>
-    <hyperlink ref="A65" r:id="rId63" display="https://scrapsfromtheloft.com/comedy/dave-chappelle-monologue-snl-2022-transcript/" xr:uid="{1434AA6F-7A8D-4AB9-94EC-8938E743419F}"/>
-    <hyperlink ref="A66" r:id="rId64" display="https://scrapsfromtheloft.com/comedy/dave-chappelle-whats-in-a-name-transcript/" xr:uid="{4A67C691-3641-4E69-B582-E07CE3B96A42}"/>
-    <hyperlink ref="A67" r:id="rId65" display="https://scrapsfromtheloft.com/comedy/iliza-shlesinger-hot-forever-transcript/" xr:uid="{4C4E5619-DCCB-46B3-9AF3-F32F199A27BB}"/>
-    <hyperlink ref="A68" r:id="rId66" display="https://scrapsfromtheloft.com/comedy/gabriel-iglesias-stadium-fluffy-transcript/" xr:uid="{2CC29002-1846-4602-8A65-DF109AA92D44}"/>
-    <hyperlink ref="A69" r:id="rId67" display="https://scrapsfromtheloft.com/comedy/fortune-feimster-good-fortune-transcript/" xr:uid="{43348BEB-168B-4CF2-9EE5-7A9B05FB23AB}"/>
-    <hyperlink ref="A70" r:id="rId68" display="https://scrapsfromtheloft.com/comedy/deon-cole-charleens-boy-transcript/" xr:uid="{0E3EEF81-2D90-4CC4-8DFA-1B2B2658E1EE}"/>
-    <hyperlink ref="A71" r:id="rId69" display="https://scrapsfromtheloft.com/comedy/neal-brennan-blocks-transcript/" xr:uid="{2F0E5B77-96E9-4B57-A570-1FA3CFF70D15}"/>
-    <hyperlink ref="A72" r:id="rId70" display="https://scrapsfromtheloft.com/comedy/trevor-noah-i-wish-you-would-transcript/" xr:uid="{C9E739FB-B0D0-43AF-AC88-FF5CDA6E8E6A}"/>
-    <hyperlink ref="A73" r:id="rId71" display="https://scrapsfromtheloft.com/comedy/whitney-cummings-jokes-transcript/" xr:uid="{398274B3-82FC-4F71-82F7-31B73230A375}"/>
-    <hyperlink ref="A74" r:id="rId72" display="https://scrapsfromtheloft.com/comedy/kate-berlant-cinnamon-in-the-wind-transcript/" xr:uid="{01A6C34F-B8F2-4224-849B-4836DC21374E}"/>
-    <hyperlink ref="A75" r:id="rId73" display="https://scrapsfromtheloft.com/comedy/patton-oswalt-we-all-scream-transcript/" xr:uid="{8659D14A-3BFC-49B1-BAB4-C9FD2B303DDD}"/>
-    <hyperlink ref="A76" r:id="rId74" display="https://scrapsfromtheloft.com/comedy/orny-adams-more-than-loud-transcript/" xr:uid="{458CF1FB-F993-4CE5-AA95-A166A91CC5D6}"/>
-    <hyperlink ref="A77" r:id="rId75" display="https://scrapsfromtheloft.com/comedy/bill-burr-live-at-red-rocks-transcript/" xr:uid="{EAE8F4AB-FC97-4213-A775-0AF1FB9B8881}"/>
-    <hyperlink ref="A78" r:id="rId76" display="https://scrapsfromtheloft.com/comedy/jon-stewart-acceptance-speech-2022-mark-twain-prize/" xr:uid="{5C98BD8C-D047-45A7-9CFF-2A8502F7FEBE}"/>
-    <hyperlink ref="A79" r:id="rId77" display="https://scrapsfromtheloft.com/comedy/pete-davidson-presents-the-best-friends-transcript/" xr:uid="{0DB4D68D-4E58-4780-850C-08264CEDE938}"/>
-    <hyperlink ref="A80" r:id="rId78" display="https://scrapsfromtheloft.com/comedy/amy-schumer-presents-parental-advisory-transcript/" xr:uid="{2F5F84A9-0A0B-416B-9002-CAF9DCE1ECA7}"/>
-    <hyperlink ref="A81" r:id="rId79" display="https://scrapsfromtheloft.com/comedy/bill-burr-presents-friends-who-kill-transcript/" xr:uid="{52452733-0AE7-4A32-9594-A28586828AA9}"/>
-    <hyperlink ref="A82" r:id="rId80" display="https://scrapsfromtheloft.com/comedy/norm-macdonald-nothing-special-transcript/" xr:uid="{0706AF62-2CB6-4A95-B943-0EC5B22DD9EA}"/>
-    <hyperlink ref="A83" r:id="rId81" display="https://scrapsfromtheloft.com/comedy/ricky-gervais-supernature-transcript/" xr:uid="{E3A2A904-F047-46D8-9396-9DCD252020B5}"/>
-    <hyperlink ref="A84" r:id="rId82" display="https://scrapsfromtheloft.com/comedy/mike-epps-under-rated-never-faded-x-rated-transcript/" xr:uid="{A9C7B963-8628-454B-B657-FE4AEC724CF9}"/>
-    <hyperlink ref="A85" r:id="rId83" display="https://scrapsfromtheloft.com/comedy/mike-epps-dont-take-it-personal-transcript/" xr:uid="{0B25DD54-D623-405B-B02B-47A2F2A5E75D}"/>
-    <hyperlink ref="A86" r:id="rId84" display="https://scrapsfromtheloft.com/comedy/catherine-cohen-the-twist-she-gorgeous-transcript/" xr:uid="{5DDA4DEF-1630-4A86-A0A3-7C94EF765733}"/>
-    <hyperlink ref="A87" r:id="rId85" display="https://scrapsfromtheloft.com/comedy/mike-epps-indiana-mike-transcript/" xr:uid="{313AEE6C-EEA2-4ECF-B028-CF35244A44C6}"/>
-    <hyperlink ref="A88" r:id="rId86" display="https://scrapsfromtheloft.com/comedy/jerrod-carmichael-rothaniel-transcript/" xr:uid="{1B68785C-E27A-4DCA-8883-654EF9D3E358}"/>
-    <hyperlink ref="A89" r:id="rId87" display="https://scrapsfromtheloft.com/comedy/taylor-tomlinson-look-at-you-transcript/" xr:uid="{19633DE2-5841-4790-BA8C-17E6FAD75ADF}"/>
-    <hyperlink ref="A90" r:id="rId88" display="https://scrapsfromtheloft.com/comedy/taylor-tomlinson-quarter-life-crisis-transcript/" xr:uid="{CC3384BF-D97D-4D34-899F-678F1EF333CB}"/>
-    <hyperlink ref="A91" r:id="rId89" display="https://scrapsfromtheloft.com/comedy/moses-storm-trash-white-transcript/" xr:uid="{BCDC121A-FF2F-481C-9B92-7AD0FD7BA71D}"/>
-    <hyperlink ref="A92" r:id="rId90" display="https://scrapsfromtheloft.com/comedy/trevor-noah-white-house-correspondents-dinner-2022-transcript/" xr:uid="{9D20C3B0-17BB-4BC9-8993-53A8A1DA84DE}"/>
-    <hyperlink ref="A93" r:id="rId91" display="https://scrapsfromtheloft.com/comedy/ali-wong-don-wong-transcript/" xr:uid="{56987CA9-BC60-4B45-A639-835DDBE72193}"/>
-    <hyperlink ref="A94" r:id="rId92" display="https://scrapsfromtheloft.com/comedy/aziz-ansari-nightclub-comedian-transcript/" xr:uid="{620C4C02-D013-4B79-B80C-455B2F224801}"/>
-    <hyperlink ref="A95" r:id="rId93" display="https://scrapsfromtheloft.com/comedy/jim-gaffigan-comedy-monster-transcript/" xr:uid="{0804EE60-73FF-4C1E-9C60-53F788C57527}"/>
-    <hyperlink ref="A96" r:id="rId94" display="https://scrapsfromtheloft.com/comedy/louis-c-k-sorry-transcript/" xr:uid="{8D8A75CD-2960-4788-A201-CD7447A9CD8F}"/>
-    <hyperlink ref="A97" r:id="rId95" display="https://scrapsfromtheloft.com/comedy/drew-michael-drew-michael-2018-transcript/" xr:uid="{4E30AA5B-9642-4AF8-AEB1-C8951B3CBB72}"/>
-    <hyperlink ref="A98" r:id="rId96" display="https://scrapsfromtheloft.com/comedy/drew-michael-red-blue-green-transcript/" xr:uid="{A2C28084-BED3-4165-9E9B-2925D053355D}"/>
-    <hyperlink ref="A99" r:id="rId97" display="https://scrapsfromtheloft.com/comedy/mo-amer-mohammed-in-texas-transcript/" xr:uid="{3B8B17E7-1A29-4A30-A30F-A9CF54157D33}"/>
-    <hyperlink ref="A100" r:id="rId98" display="https://scrapsfromtheloft.com/comedy/dave-chappelle-the-closer-transcript/" xr:uid="{6FB89A96-DB6D-4D0A-9D11-346EB139A59C}"/>
-    <hyperlink ref="A101" r:id="rId99" display="https://scrapsfromtheloft.com/comedy/kathleen-madigan-bothering-jesus-transcript/" xr:uid="{D0801BB9-5BCC-435F-A99A-9ABB068695F2}"/>
-    <hyperlink ref="A102" r:id="rId100" display="https://scrapsfromtheloft.com/comedy/kathleen-madigan-madigan-again-transcript/" xr:uid="{5C618F8D-BEC1-479B-AE27-E83EAFAB95A0}"/>
-    <hyperlink ref="A103" r:id="rId101" display="https://scrapsfromtheloft.com/comedy/phil-wang-philly-philly-wang-wang-transcript/" xr:uid="{635ED003-0DDA-4E5F-B1D7-D896AD1E1C45}"/>
-    <hyperlink ref="A104" r:id="rId102" display="https://scrapsfromtheloft.com/comedy/dave-chappelle-846-transcript/" xr:uid="{C32677AD-48A3-43C4-B4F2-63EC1DB51B60}"/>
-    <hyperlink ref="A105" r:id="rId103" display="https://scrapsfromtheloft.com/comedy/tom-papa-youre-doing-great-transcript/" xr:uid="{4E7B839C-41F1-4FDA-AC46-504B073D9084}"/>
-    <hyperlink ref="A106" r:id="rId104" display="https://scrapsfromtheloft.com/comedy/tom-papa-human-mule-transcript/" xr:uid="{66275D45-FD4E-4902-8FA9-AD456D2D8A9F}"/>
-    <hyperlink ref="A107" r:id="rId105" display="https://scrapsfromtheloft.com/comedy/tom-papa-freaked-out-transcript/" xr:uid="{AD8A8B62-366D-4448-84FC-E735BB187BE4}"/>
-    <hyperlink ref="A108" r:id="rId106" display="https://scrapsfromtheloft.com/comedy/bo-burnham-inside-transcript/" xr:uid="{2C64B8C6-4EFA-46E4-87EF-0BC25CFB5C36}"/>
-    <hyperlink ref="A109" r:id="rId107" display="https://scrapsfromtheloft.com/comedy/tig-notaro-boyish-girl-interrupted-transcript/" xr:uid="{9F74A07F-BCCB-488B-A6FA-6AE219CE3DDD}"/>
-    <hyperlink ref="A110" r:id="rId108" display="https://scrapsfromtheloft.com/comedy/joe-list-i-hate-myself-transcript/" xr:uid="{4A517A92-43EA-4378-856F-8823824B9454}"/>
-    <hyperlink ref="A111" r:id="rId109" display="https://scrapsfromtheloft.com/comedy/nate-bargatze-greatest-average-american-transcript/" xr:uid="{808DE029-55A6-496A-B3E1-37E70E354777}"/>
-    <hyperlink ref="A112" r:id="rId110" display="https://scrapsfromtheloft.com/comedy/brian-regan-on-the-rocks-transcript/" xr:uid="{143C3DFB-426C-4F4F-A8F1-B8796327CD77}"/>
-    <hyperlink ref="A113" r:id="rId111" display="https://scrapsfromtheloft.com/comedy/george-carlin-politically-correct-language/" xr:uid="{6D7B449C-8EC2-493D-83E9-1CC0B3A40661}"/>
-    <hyperlink ref="A114" r:id="rId112" display="https://scrapsfromtheloft.com/comedy/doug-stanhope-beer-hall-putsch-transcript/" xr:uid="{903A1195-357E-4307-A44B-38CF6A47EAF0}"/>
-    <hyperlink ref="A115" r:id="rId113" display="https://scrapsfromtheloft.com/comedy/chris-rock-total-blackout-the-tamborine-extended-cut-transcript/" xr:uid="{0AAED6DC-BC35-49BB-AB60-59E767B7F9D8}"/>
-    <hyperlink ref="A116" r:id="rId114" display="https://scrapsfromtheloft.com/comedy/george-carlin-life-worth-losing-transcript/" xr:uid="{61A8D5B7-44AA-473D-85F6-F7666220CC0A}"/>
-    <hyperlink ref="A117" r:id="rId115" display="https://scrapsfromtheloft.com/comedy/sarah-cooper-everythings-fine-transcript/" xr:uid="{58DF5534-8D8C-4558-9DEE-5EA3E08A70A8}"/>
-    <hyperlink ref="A118" r:id="rId116" display="https://scrapsfromtheloft.com/comedy/bo-burnham-words-words-words-transcript/" xr:uid="{4F62E633-E1A8-40EA-8945-63F6054122FE}"/>
-    <hyperlink ref="A119" r:id="rId117" display="https://scrapsfromtheloft.com/comedy/vir-das-outside-in-the-lockdown-special-transcript/" xr:uid="{3D63A592-1E13-42CC-B427-F21C20AE678C}"/>
-    <hyperlink ref="A120" r:id="rId118" display="https://scrapsfromtheloft.com/comedy/larry-the-cable-guy-remain-seated-transcript/" xr:uid="{A38CE093-B7CA-4776-896A-C505283E53E6}"/>
-    <hyperlink ref="A121" r:id="rId119" display="https://scrapsfromtheloft.com/comedy/craig-ferguson-just-being-honest-transcript/" xr:uid="{3C3F8D19-FF85-43BF-9D50-75D654EFBC33}"/>
-    <hyperlink ref="A122" r:id="rId120" display="https://scrapsfromtheloft.com/comedy/kevin-hart-zero-fks-given-2020-transcript/" xr:uid="{2662A13A-09C0-4000-A057-74A9E1942F5E}"/>
-    <hyperlink ref="A123" r:id="rId121" display="https://scrapsfromtheloft.com/comedy/sam-morril-i-got-this-2020-transcript/" xr:uid="{E2C4D97E-8D52-4FA7-89C7-093232B6E00A}"/>
-    <hyperlink ref="A124" r:id="rId122" display="https://scrapsfromtheloft.com/comedy/dave-chappelle-snl-monologue-2020-transcript/" xr:uid="{D3215B21-C8F6-4FF0-8FA9-306D44A360AA}"/>
-    <hyperlink ref="A125" r:id="rId123" display="https://scrapsfromtheloft.com/comedy/chris-rock-snl-monologue-2020-transcript/" xr:uid="{C6E9E2F5-6BE0-42AE-BF4A-09C9B4DBAF0B}"/>
-    <hyperlink ref="A126" r:id="rId124" display="https://scrapsfromtheloft.com/comedy/bill-burr-snl-monologue-2020-transcript/" xr:uid="{57E57DDF-3C15-46ED-945A-393A6BE85F66}"/>
-    <hyperlink ref="A127" r:id="rId125" display="https://scrapsfromtheloft.com/comedy/john-mulaney-snl-monologue-2020-transcript/" xr:uid="{E1A1DC93-219F-49FC-871D-F7FB8CD66980}"/>
-    <hyperlink ref="A128" r:id="rId126" display="https://scrapsfromtheloft.com/comedy/ronny-chieng-asian-comedian-destroys-america-transcript/" xr:uid="{79E6A364-575E-4B13-9A0C-AC977AD8FBB6}"/>
-    <hyperlink ref="A129" r:id="rId127" display="https://scrapsfromtheloft.com/comedy/craig-ferguson-a-wee-bit-o-revolution-transcript/" xr:uid="{A33111DD-B534-4938-B617-DEEAB3312E8A}"/>
-    <hyperlink ref="A130" r:id="rId128" display="https://scrapsfromtheloft.com/comedy/michael-mcintyre-showman-transcript/" xr:uid="{46EF93DF-25B1-467A-9CDA-EE85B73271F2}"/>
-    <hyperlink ref="A131" r:id="rId129" display="https://scrapsfromtheloft.com/comedy/rob-schneider-asian-momma-mexican-kids-transcript/" xr:uid="{69DE029C-2DC8-4EA0-AA94-105521863FC5}"/>
-    <hyperlink ref="A132" r:id="rId130" display="https://scrapsfromtheloft.com/comedy/sam-jay-3-in-the-morning-transcript/" xr:uid="{D3A50ECE-A607-4DCC-8C23-48F472C3AE4D}"/>
-    <hyperlink ref="A133" r:id="rId131" display="https://scrapsfromtheloft.com/comedy/jack-whitehall-im-only-joking-transcript/" xr:uid="{02167311-F9B8-4B2C-9697-2F0CBB595180}"/>
-    <hyperlink ref="A134" r:id="rId132" display="https://scrapsfromtheloft.com/comedy/urzila-carlson-overqualified-loser-transcript/" xr:uid="{77F892BA-0DB3-444B-AD36-69602E309037}"/>
-    <hyperlink ref="A135" r:id="rId133" display="https://scrapsfromtheloft.com/comedy/george-lopez-well-do-it-for-half-transcript/" xr:uid="{04142243-8610-447A-A81A-67C99FE7D179}"/>
-    <hyperlink ref="A136" r:id="rId134" display="https://scrapsfromtheloft.com/comedy/jim-jefferies-intolerant-transcript/" xr:uid="{2403AEF5-D047-4F8E-9CB0-924A31826541}"/>
-    <hyperlink ref="A137" r:id="rId135" display="https://scrapsfromtheloft.com/comedy/bill-hicks-censored-david-letterman-transcript/" xr:uid="{E92E9AA6-A596-4131-BE29-7A8F022E1BD7}"/>
-    <hyperlink ref="A138" r:id="rId136" display="https://scrapsfromtheloft.com/comedy/george-carlin-doin-it-again-transcript/" xr:uid="{A2052C3A-68A7-4B9B-8617-18D6A6E99DCA}"/>
-    <hyperlink ref="A139" r:id="rId137" display="https://scrapsfromtheloft.com/comedy/eric-andre-legalize-everything-transcript/" xr:uid="{B349E504-7C7D-4255-9E5B-18D896F3B398}"/>
-    <hyperlink ref="A140" r:id="rId138" display="https://scrapsfromtheloft.com/comedy/roy-wood-jr-father-figure-transcript/" xr:uid="{F745C385-DA3C-4EB7-B472-F4E649884604}"/>
-    <hyperlink ref="A141" r:id="rId139" display="https://scrapsfromtheloft.com/comedy/dave-chappelle-hbo-comedy-half-hour-1998-transcript/" xr:uid="{02B0E273-9452-46D8-94E2-5515DE66D468}"/>
-    <hyperlink ref="A142" r:id="rId140" display="https://scrapsfromtheloft.com/comedy/mark-normand-dont-be-yourself-transcript/" xr:uid="{874620AA-BD19-4AFB-99CA-CB640B258141}"/>
-    <hyperlink ref="A143" r:id="rId141" display="https://scrapsfromtheloft.com/comedy/doug-stanhope-fear-of-an-empty-bed-transcript/" xr:uid="{89849FAA-F300-4B65-8139-BC9AC20D3BAC}"/>
-    <hyperlink ref="A144" r:id="rId142" display="https://scrapsfromtheloft.com/comedy/chris-gethard-career-suicide-transcript/" xr:uid="{9CF34735-48EA-4D73-90C2-E365CB7D864D}"/>
-    <hyperlink ref="A145" r:id="rId143" display="https://scrapsfromtheloft.com/comedy/ramy-youssef-feelings-transcript/" xr:uid="{D881A39D-B5D5-451E-BF49-D46E4CD6DF75}"/>
-    <hyperlink ref="A146" r:id="rId144" display="https://scrapsfromtheloft.com/comedy/kenny-sebastian-dont-be-that-guy-transcript/" xr:uid="{6402D41B-646C-4121-B52F-457DEB584E88}"/>
-    <hyperlink ref="A147" r:id="rId145" display="https://scrapsfromtheloft.com/comedy/billy-connolly-high-horse-tour-live-transcript/" xr:uid="{83A0F7DD-5E4D-496F-89DF-879261A2A76F}"/>
-    <hyperlink ref="A148" r:id="rId146" display="https://scrapsfromtheloft.com/comedy/hannah-gadsby-douglas-transcript/" xr:uid="{2A98E731-9133-4944-840E-496E5F5EA1B5}"/>
-    <hyperlink ref="A149" r:id="rId147" display="https://scrapsfromtheloft.com/comedy/hasan-minhaj-homecoming-king-transcript/" xr:uid="{853BBDA7-3BB3-4E00-8C5B-7515E742E665}"/>
-    <hyperlink ref="A150" r:id="rId148" display="https://scrapsfromtheloft.com/comedy/patton-oswalt-i-love-everything-transcript/" xr:uid="{B2439BB0-C739-4D83-9362-EE928DCDC194}"/>
-    <hyperlink ref="A151" r:id="rId149" display="https://scrapsfromtheloft.com/comedy/russell-peters-deported-transcript/" xr:uid="{6769E7C2-76D7-4C5C-811F-A0E8B15ADA69}"/>
-    <hyperlink ref="A152" r:id="rId150" display="https://scrapsfromtheloft.com/comedy/jimmy-o-yang-good-deal-transcript/" xr:uid="{4ABC56B4-64DD-4C7D-A2B6-C4B52021DD64}"/>
-    <hyperlink ref="A153" r:id="rId151" display="https://scrapsfromtheloft.com/comedy/jo-koy-lights-out-2012-full-transcript/" xr:uid="{0F75CFB1-80D6-4E65-9D2B-99EFA2107AAA}"/>
-    <hyperlink ref="A154" r:id="rId152" display="https://scrapsfromtheloft.com/comedy/lee-mack-going-out-live-transcript/" xr:uid="{93DA4351-9905-4F94-8183-657C2D92938E}"/>
-    <hyperlink ref="A155" r:id="rId153" display="https://scrapsfromtheloft.com/comedy/lee-mack-live-transcript/" xr:uid="{6E707677-42DA-41AE-9581-F477FC63DE1D}"/>
-    <hyperlink ref="A156" r:id="rId154" display="https://scrapsfromtheloft.com/comedy/t-j-miller-no-real-reason-transcript/" xr:uid="{B32D671A-7170-4BBB-8206-3073709D1EA3}"/>
-    <hyperlink ref="A157" r:id="rId155" display="https://scrapsfromtheloft.com/comedy/jerry-seinfeld-23-hours-to-kill-transcript/" xr:uid="{48231A52-58A3-4CD4-BDCC-1C8BDE6FAFD0}"/>
-    <hyperlink ref="A158" r:id="rId156" display="https://scrapsfromtheloft.com/comedy/bill-burr-late-show-with-david-letterman-2010/" xr:uid="{D06B706C-B279-40FF-81C3-02C7ED2FC9B1}"/>
-    <hyperlink ref="A159" r:id="rId157" display="https://scrapsfromtheloft.com/comedy/sincerely-louis-ck-transcript/" xr:uid="{24C12A27-C13E-440A-8D4B-4690AF28F35F}"/>
-    <hyperlink ref="A160" r:id="rId158" display="https://scrapsfromtheloft.com/comedy/jim-norton-american-degenerate-transcript/" xr:uid="{3A62081B-BD0B-4DDA-A7ED-F33649777CE0}"/>
-    <hyperlink ref="A161" r:id="rId159" display="https://scrapsfromtheloft.com/comedy/jim-norton-monster-rain-transcript/" xr:uid="{A14B89C2-19C9-4329-9BEF-26EF09BAAE07}"/>
-    <hyperlink ref="A162" r:id="rId160" display="https://scrapsfromtheloft.com/comedy/maria-bamford-weakness-is-the-brand-transcript/" xr:uid="{FFDD023F-D592-4A42-B0AC-C551414ACCF1}"/>
-    <hyperlink ref="A163" r:id="rId161" display="https://scrapsfromtheloft.com/comedy/dave-allen-first-day-at-school-transcript/" xr:uid="{525AFA60-60AC-4B16-B9D3-906AD7990B63}"/>
-    <hyperlink ref="A164" r:id="rId162" display="https://scrapsfromtheloft.com/comedy/chris-d-elia-white-male-black-comic-transcript/" xr:uid="{48325F99-6C3E-4992-B977-3E1503986B50}"/>
-    <hyperlink ref="A165" r:id="rId163" display="https://scrapsfromtheloft.com/comedy/chris-d-elia-man-on-fire-transcript/" xr:uid="{8D5C7C1C-1F52-4922-8E5F-599ED344139A}"/>
-    <hyperlink ref="A166" r:id="rId164" display="https://scrapsfromtheloft.com/comedy/george-carlin-indian-drill-sergeant-transcript/" xr:uid="{428637A9-12B3-47D0-9E05-C6BD2984E4C0}"/>
-    <hyperlink ref="A167" r:id="rId165" display="https://scrapsfromtheloft.com/comedy/tom-segura-ball-hog-transcript/" xr:uid="{3DF8548C-5E87-4A37-BC5A-16E3107CE840}"/>
-    <hyperlink ref="A168" r:id="rId166" display="https://scrapsfromtheloft.com/comedy/bert-kreischer-hey-big-boy-transcript/" xr:uid="{6BC8D29B-3490-40CD-9E06-B1724F2C6818}"/>
-    <hyperlink ref="A169" r:id="rId167" display="https://scrapsfromtheloft.com/comedy/bert-kreischer-fighting-a-bear-transcript/" xr:uid="{DABAFA02-E493-48C8-9CC8-3BA9582AE0D0}"/>
-    <hyperlink ref="A170" r:id="rId168" display="https://scrapsfromtheloft.com/comedy/marc-maron-end-times-fun-transcript/" xr:uid="{60E40130-2DD6-47D2-91E8-669BCC6D489A}"/>
-    <hyperlink ref="A171" r:id="rId169" display="https://scrapsfromtheloft.com/comedy/pete-davidson-smd-transcript/" xr:uid="{0E71D953-8185-40C5-B70C-6EBCCCB6FB51}"/>
-    <hyperlink ref="A172" r:id="rId170" display="https://scrapsfromtheloft.com/comedy/pete-davidson-alive-from-new-york-transcript/" xr:uid="{A6EF7B36-CA7F-4FEB-B1C1-5352C9113941}"/>
-    <hyperlink ref="A173" r:id="rId171" display="https://scrapsfromtheloft.com/comedy/amanda-seales-i-be-knowin-transcript/" xr:uid="{C2E35E00-738E-4FA1-99A3-F2BE812250E7}"/>
-    <hyperlink ref="A174" r:id="rId172" display="https://scrapsfromtheloft.com/comedy/stewart-lee-carpet-remnant-world-transcript/" xr:uid="{32143994-4CEA-416F-9AF2-E67C478EC48B}"/>
-    <hyperlink ref="A175" r:id="rId173" display="https://scrapsfromtheloft.com/comedy/stewart-lee-content-provider-transcript/" xr:uid="{ECAC06A7-7766-44B4-BE13-1BC276D79FF7}"/>
-    <hyperlink ref="A176" r:id="rId174" display="https://scrapsfromtheloft.com/comedy/sara-pascoe-ladsladslads-2019-full-transcript/" xr:uid="{9F5930FE-603D-41BB-AD15-ED29C17B22A9}"/>
-    <hyperlink ref="A177" r:id="rId175" display="https://scrapsfromtheloft.com/comedy/dan-soder-son-of-a-gary-transcript/" xr:uid="{E8FC0CEF-0EA6-4431-A525-4A10A7198501}"/>
-    <hyperlink ref="A178" r:id="rId176" display="https://scrapsfromtheloft.com/comedy/jim-gaffigan-quality-time-transcript/" xr:uid="{8371EE7A-6B57-4BC1-9980-C605E4DE5237}"/>
-    <hyperlink ref="A179" r:id="rId177" display="https://scrapsfromtheloft.com/comedy/dave-chappelle-acceptance-speech-2019-mark-twain-prize/" xr:uid="{FFC097E6-0790-4272-8817-49ABC04C1F59}"/>
-    <hyperlink ref="A180" r:id="rId178" display="https://scrapsfromtheloft.com/comedy/ricky-gervais-2020-golden-globes-monologue-transcript/" xr:uid="{A20AA465-EB98-455A-9462-1ED6F1C5AF13}"/>
-    <hyperlink ref="A181" r:id="rId179" display="https://scrapsfromtheloft.com/comedy/kevin-bridges-whole-different-story-transcript/" xr:uid="{F69CDC9E-520D-4D78-9CD8-AFFB155DA0D9}"/>
-    <hyperlink ref="A182" r:id="rId180" display="https://scrapsfromtheloft.com/comedy/kevin-bridges-story-so-far-live-glasgow-transcript/" xr:uid="{65FE2A4C-7DB8-421F-AD57-B0BD3A1D6C55}"/>
-    <hyperlink ref="A183" r:id="rId181" display="https://scrapsfromtheloft.com/comedy/kevin-bridges-the-story-continues-transcript/" xr:uid="{386A9112-D3F8-4C1D-8C4D-703CCD1A11BC}"/>
-    <hyperlink ref="A184" r:id="rId182" display="https://scrapsfromtheloft.com/comedy/andy-woodhull-youll-always-be-late-transcript/" xr:uid="{0B40AAC3-70CA-48A6-9591-272F99E0F057}"/>
-    <hyperlink ref="A185" r:id="rId183" display="https://scrapsfromtheloft.com/comedy/michelle-wolf-joke-show-transcript/" xr:uid="{CA12813D-E949-486A-A186-267FB683E3F1}"/>
-    <hyperlink ref="A186" r:id="rId184" display="https://scrapsfromtheloft.com/comedy/tiffany-haddish-black-mitzvah-transcript/" xr:uid="{669178C5-F85A-4BDE-9915-7FD09E85E865}"/>
-    <hyperlink ref="A187" r:id="rId185" display="https://scrapsfromtheloft.com/comedy/mike-birbiglia-the-new-one-transcript/" xr:uid="{D01E8F51-586D-4C80-94E8-DD207F1F851E}"/>
-    <hyperlink ref="A188" r:id="rId186" display="https://scrapsfromtheloft.com/comedy/iliza-shlesinger-unveiled-transcript/" xr:uid="{7B02D1D5-C8EC-46D8-8A3E-DA506B513204}"/>
-    <hyperlink ref="A189" r:id="rId187" display="https://scrapsfromtheloft.com/comedy/seth-meyers-lobby-baby-transcript/" xr:uid="{FDAC246E-7F9E-4D3D-8859-83840D7DC992}"/>
-    <hyperlink ref="A190" r:id="rId188" display="https://scrapsfromtheloft.com/comedy/arsenio-hall-smart-and-classy-transcript/" xr:uid="{B96D4084-124A-4A0C-BA78-EAB12E3D5BA0}"/>
-    <hyperlink ref="A191" r:id="rId189" display="https://scrapsfromtheloft.com/comedy/sebastian-maniscalco-tonight-show-starring-jimmy-fallon-transcript/" xr:uid="{32829CD6-F948-47CB-9D73-2838E402B0D2}"/>
-    <hyperlink ref="A192" r:id="rId190" display="https://scrapsfromtheloft.com/comedy/nikki-glaser-bangin-transcript/" xr:uid="{06B477EE-CD33-4E59-B806-AE6D84EE8169}"/>
-    <hyperlink ref="A193" r:id="rId191" display="https://scrapsfromtheloft.com/comedy/ryan-hamilton-stand-up-the-tonight-show-starring-jimmy-fallon-transcript/" xr:uid="{2ABE238D-E04E-4A99-8BA2-5B76306DBA42}"/>
-    <hyperlink ref="A194" r:id="rId192" display="https://scrapsfromtheloft.com/comedy/mark-normand-stand-up-tonight-show-starring-jimmy-fallon/" xr:uid="{FC723AB0-2B6E-4332-9A31-1960C9203EC7}"/>
-    <hyperlink ref="A195" r:id="rId193" display="https://scrapsfromtheloft.com/comedy/george-carlin-dumb-americans-transcript/" xr:uid="{BC20C34D-9791-41DB-A64E-E34A2AC9CE79}"/>
-    <hyperlink ref="A196" r:id="rId194" display="https://scrapsfromtheloft.com/comedy/bill-burr-paper-tiger-transcript/" xr:uid="{F31FD261-2770-4AE9-8114-48EF34A99559}"/>
-    <hyperlink ref="A197" r:id="rId195" display="https://scrapsfromtheloft.com/comedy/dave-chappelle-sticks-stones-epilogue-punchline-transcript/" xr:uid="{9587C9E8-1B85-4766-9E5B-595A53BAE814}"/>
-    <hyperlink ref="A198" r:id="rId196" display="https://scrapsfromtheloft.com/comedy/brazil-corruption-amazon-hasan-minhaj/" xr:uid="{42730A73-8E69-43AD-B0FC-45B84227C65B}"/>
-    <hyperlink ref="A199" r:id="rId197" display="https://scrapsfromtheloft.com/comedy/dave-chappelle-sticks-stones-transcript/" xr:uid="{E96C77B4-E21E-4270-8126-6210DEE0F843}"/>
-    <hyperlink ref="A200" r:id="rId198" display="https://scrapsfromtheloft.com/comedy/emily-heller-ice-thickeners-transcript/" xr:uid="{84B7CFA5-AE2C-43E2-B87E-494593BC0F00}"/>
-    <hyperlink ref="A201" r:id="rId199" display="https://scrapsfromtheloft.com/comedy/david-cross-oh-come-on-transcript/" xr:uid="{5E9F50A2-B89A-476A-94F8-8B4930879449}"/>
-    <hyperlink ref="A202" r:id="rId200" display="https://scrapsfromtheloft.com/comedy/kevin-hart-gun-compartment-transcript/" xr:uid="{63B59384-DF87-4DF6-954E-96F71B98044F}"/>
-    <hyperlink ref="A203" r:id="rId201" display="https://scrapsfromtheloft.com/comedy/whitney-cummings-can-i-touch-it-transcript/" xr:uid="{27387D58-FFE9-4BAE-B223-57DAE6F99B15}"/>
-    <hyperlink ref="A204" r:id="rId202" display="https://scrapsfromtheloft.com/comedy/eddie-griffin-bible-negro-version-transcript/" xr:uid="{6A4A76CD-0777-4ADC-A9FF-C7AF3F6496C1}"/>
-    <hyperlink ref="A205" r:id="rId203" display="https://scrapsfromtheloft.com/comedy/tom-segura-overdoses-this-is-not-happening-transcript/" xr:uid="{57F57310-AD30-4AE4-AAC3-2F99929FE243}"/>
-    <hyperlink ref="A206" r:id="rId204" display="https://scrapsfromtheloft.com/comedy/aziz-ansari-right-now-transcript/" xr:uid="{FC3D1EFC-18F9-4D8E-8577-B1A7BF87E5F3}"/>
-    <hyperlink ref="A207" r:id="rId205" display="https://scrapsfromtheloft.com/comedy/ralphie-may-filthy-animal-tour-transcript/" xr:uid="{426E5086-58EC-433A-8F66-501025AEE4CE}"/>
-    <hyperlink ref="A208" r:id="rId206" display="https://scrapsfromtheloft.com/comedy/mike-epps-only-one-mike-transcript/" xr:uid="{D84672F7-727D-4ADD-BDF8-820FAA54F96D}"/>
-    <hyperlink ref="A209" r:id="rId207" display="https://scrapsfromtheloft.com/comedy/adam-devine-best-time-of-our-lives-transcript/" xr:uid="{3D84A67A-FBFD-4B2A-948A-309D2B26AF1C}"/>
-    <hyperlink ref="A210" r:id="rId208" display="https://scrapsfromtheloft.com/comedy/jo-koy-live-from-seattle-transcript/" xr:uid="{AB071FC9-B7D1-49F5-A658-94E2FA0A274B}"/>
-    <hyperlink ref="A211" r:id="rId209" display="https://scrapsfromtheloft.com/comedy/jo-ko-comin-in-hot-transcript/" xr:uid="{F5864EAC-0F41-42CA-83C8-46064E4AD8B9}"/>
-    <hyperlink ref="A212" r:id="rId210" display="https://scrapsfromtheloft.com/comedy/the-standups-gina-yashere-2018-transcript/" xr:uid="{1BACB788-FA07-48B1-BDDE-788713F13F96}"/>
-    <hyperlink ref="A213" r:id="rId211" display="https://scrapsfromtheloft.com/comedy/wanda-sykes-not-normal-transcript/" xr:uid="{27227C81-1FAA-460A-8C05-B40B4209FABE}"/>
-    <hyperlink ref="A214" r:id="rId212" display="https://scrapsfromtheloft.com/comedy/doug-stanhope-babies-and-abortion/" xr:uid="{B1145A4A-62C5-4F54-9CC2-035B01DA816B}"/>
-    <hyperlink ref="A215" r:id="rId213" display="https://scrapsfromtheloft.com/comedy/cedric-the-entertainer-live-from-the-ville-transcript/" xr:uid="{AEBEF49F-5CB8-48C0-B204-7A72DFFC0217}"/>
-    <hyperlink ref="A216" r:id="rId214" display="https://scrapsfromtheloft.com/comedy/eddie-murphy-raw-transcript/" xr:uid="{D5BCD62D-A493-4FBA-85D6-CDAA64A62D12}"/>
-    <hyperlink ref="A217" r:id="rId215" display="https://scrapsfromtheloft.com/comedy/colin-quinn-the-new-york-story-transcript/" xr:uid="{79C2D788-C5F9-486F-AB3D-092E77D1BD69}"/>
-    <hyperlink ref="A218" r:id="rId216" display="https://scrapsfromtheloft.com/comedy/demetri-martin-live-at-the-time-transcript/" xr:uid="{A13A0B01-455B-46F5-90B7-609A01773337}"/>
-    <hyperlink ref="A219" r:id="rId217" display="https://scrapsfromtheloft.com/comedy/george-carlin-what-am-i-doing-in-new-jersey-transcript/" xr:uid="{34AA16DC-314C-4424-8515-AAC49D1418E2}"/>
-    <hyperlink ref="A220" r:id="rId218" display="https://scrapsfromtheloft.com/comedy/chelsea-peretti-one-of-the-greats-transcript/" xr:uid="{63206FEE-EBD0-4D61-A526-4D03243B0AA1}"/>
-    <hyperlink ref="A221" r:id="rId219" display="https://scrapsfromtheloft.com/comedy/anthony-jeselnik-fire-in-the-maternity-ward-transcript/" xr:uid="{E010D904-CDB7-4A28-9282-6866A1A012CD}"/>
-    <hyperlink ref="A222" r:id="rId220" display="https://scrapsfromtheloft.com/comedy/roy-wood-jr-no-one-loves-you-transcript/" xr:uid="{0673BC99-1DB8-44AF-B75A-3CB30177BF23}"/>
-    <hyperlink ref="A223" r:id="rId221" display="https://scrapsfromtheloft.com/comedy/robin-williams-weapons-of-self-destruction-transcript/" xr:uid="{2790B4EC-7544-42CC-B32A-FB805A4460B8}"/>
-    <hyperlink ref="A224" r:id="rId222" display="https://scrapsfromtheloft.com/comedy/robin-williams-live-on-broadway-2002-full-transcript/" xr:uid="{CA143D91-3D85-4995-994C-1F89AFC229D2}"/>
-    <hyperlink ref="A225" r:id="rId223" display="https://scrapsfromtheloft.com/comedy/jimmy-carr-the-best-of-ultimate-gold-greatest-hits-transcript/" xr:uid="{C6E45C70-8BC1-4ADF-881C-350C421F9EC6}"/>
-    <hyperlink ref="A226" r:id="rId224" display="https://scrapsfromtheloft.com/comedy/nate-bargatze-the-tennessee-kid-transcript/" xr:uid="{2303AF80-BE3B-4A66-8266-45FF547E7605}"/>
-    <hyperlink ref="A227" r:id="rId225" display="https://scrapsfromtheloft.com/comedy/w-kamau-bell-private-school-negro-transcript/" xr:uid="{B1D664E6-C631-4E44-8E88-8333BD10D74F}"/>
-    <hyperlink ref="A228" r:id="rId226" display="https://scrapsfromtheloft.com/comedy/kevin-hart-irresponsible-transcript/" xr:uid="{FAF7CA67-39DD-4FF2-AF5C-2DC41FA3B3DF}"/>
-    <hyperlink ref="A229" r:id="rId227" display="https://scrapsfromtheloft.com/comedy/nate-bargatze-full-time-magic-transcript/" xr:uid="{F1865610-16FF-4C38-8825-3E81AA17E28F}"/>
-    <hyperlink ref="A230" r:id="rId228" display="https://scrapsfromtheloft.com/comedy/amy-schumer-growing-transcript/" xr:uid="{10824422-A151-4B41-95F5-2F4A7BE40864}"/>
-    <hyperlink ref="A231" r:id="rId229" display="https://scrapsfromtheloft.com/comedy/ricky-gervais-2011-golden-globes-opening-monologue/" xr:uid="{226632C0-A2AD-444C-A9E6-50F40784F47E}"/>
-    <hyperlink ref="A232" r:id="rId230" display="https://scrapsfromtheloft.com/comedy/ricky-gervais-2016-golden-globes-opening-monologue/" xr:uid="{9CFC712A-D11B-46D9-B19B-E113D314747E}"/>
-    <hyperlink ref="A233" r:id="rId231" display="https://scrapsfromtheloft.com/comedy/enissa-amani-ehrenwort-2018-full-transcript/" xr:uid="{4297CB80-4999-4CB8-80F9-46443EAC890B}"/>
-    <hyperlink ref="A234" r:id="rId232" display="https://scrapsfromtheloft.com/comedy/ken-jeong-you-complete-me-ho-transcript/" xr:uid="{43A04EDA-2169-4F8E-91B9-17936FBFEA22}"/>
-    <hyperlink ref="A235" r:id="rId233" display="https://scrapsfromtheloft.com/comedy/ray-romano-right-here-around-the-corner-transcript/" xr:uid="{ACE60299-EB0B-4B9C-B22F-5D62DB6A630D}"/>
-    <hyperlink ref="A236" r:id="rId234" display="https://scrapsfromtheloft.com/comedy/gabriel-fluffy-iglesias-one-show-fits-all-transcript/" xr:uid="{54FC58CE-3E94-4E97-8D3A-A634B7F301C4}"/>
-    <hyperlink ref="A237" r:id="rId235" display="https://scrapsfromtheloft.com/comedy/sebastian-maniscalco-stay-hungry-transcript/" xr:uid="{E2148CF7-A2BF-43C3-8724-A55BDDAE46B0}"/>
-    <hyperlink ref="A238" r:id="rId236" display="https://scrapsfromtheloft.com/comedy/latin-history-for-morons-john-leguizamo-transcript/" xr:uid="{A69E4AF9-43D1-4197-BEA6-4A0D7563A557}"/>
-    <hyperlink ref="A239" r:id="rId237" display="https://scrapsfromtheloft.com/comedy/sebastian-maniscalco-arent-you-embarrassed-transcript/" xr:uid="{8A8DD5E8-B4B3-48CC-927D-51986E41212A}"/>
-    <hyperlink ref="A240" r:id="rId238" display="https://scrapsfromtheloft.com/comedy/sebastian-maniscalco-whats-wrong-with-people-transcript/" xr:uid="{211FEBB0-AC42-4859-8F78-60FEF7FAF4EB}"/>
-    <hyperlink ref="A241" r:id="rId239" display="https://scrapsfromtheloft.com/comedy/oh-hello-on-broadway-transcript/" xr:uid="{E2E30995-FA6F-4665-BE81-9EF0C6B14326}"/>
-    <hyperlink ref="A242" r:id="rId240" display="https://scrapsfromtheloft.com/comedy/ellen-degeneres-relatable-transcript/" xr:uid="{2CA97D97-35B7-4837-BE20-BBBD4C21D463}"/>
-    <hyperlink ref="A243" r:id="rId241" display="https://scrapsfromtheloft.com/comedy/pete-holmes-dirty-clean-transcript/" xr:uid="{21E9B9E3-10E6-4E6D-84C1-B5A96D3B76D0}"/>
-    <hyperlink ref="A244" r:id="rId242" display="https://scrapsfromtheloft.com/comedy/vir-das-losing-it-transcript/" xr:uid="{339B00D9-82B3-4EE9-98E4-521AAF275D4A}"/>
-    <hyperlink ref="A245" r:id="rId243" display="https://scrapsfromtheloft.com/comedy/volker-pispers-about-usa-2004-transcript/" xr:uid="{9117F30F-0DC9-4095-B63A-214A112EB80A}"/>
-    <hyperlink ref="A246" r:id="rId244" display="https://scrapsfromtheloft.com/comedy/trevor-noah-son-of-patricia-transcript/" xr:uid="{47C2271A-DF16-46F3-8F2A-CCCBA3FCCBE5}"/>
-    <hyperlink ref="A247" r:id="rId245" display="https://scrapsfromtheloft.com/comedy/jeff-foxworthy-larry-the-cable-guy-weve-been-thinking-transcript/" xr:uid="{9FB458B3-A488-4B6A-9C5E-EE0AC6189A5C}"/>
-    <hyperlink ref="A248" r:id="rId246" display="https://scrapsfromtheloft.com/comedy/adam-sandler-100-fresh-transcript/" xr:uid="{C95AE3F6-49BE-4978-B286-EA8BB44A1445}"/>
-    <hyperlink ref="A249" r:id="rId247" display="https://scrapsfromtheloft.com/comedy/jeff-foxworthy-totally-committed-transcript/" xr:uid="{48DB69AE-831D-4337-BB08-CD92563F5D03}"/>
-    <hyperlink ref="A250" r:id="rId248" display="https://scrapsfromtheloft.com/comedy/ron-white-if-you-quit-listening-ill-shutup-transcript/" xr:uid="{597AEA37-E878-4B8C-BE73-C028EFA61242}"/>
-    <hyperlink ref="A251" r:id="rId249" display="https://scrapsfromtheloft.com/comedy/carlin-at-carnegie-transcript/" xr:uid="{78B51715-B2FA-46BB-8DC7-E59115D57905}"/>
-    <hyperlink ref="A252" r:id="rId250" display="https://scrapsfromtheloft.com/comedy/comedy-central-presents-tom-segura-s15e01-transcript/" xr:uid="{3D354D13-C56D-4517-B827-9C71C0282184}"/>
-    <hyperlink ref="A253" r:id="rId251" display="https://scrapsfromtheloft.com/comedy/mo-amer-the-vagabond-transcript/" xr:uid="{2BD833F7-C400-4801-B94E-0A3D98145D34}"/>
-    <hyperlink ref="A254" r:id="rId252" display="https://scrapsfromtheloft.com/comedy/joe-mandes-award-winning-comedy-special-transcript/" xr:uid="{895BC373-F9B5-4D5B-B664-1D3DD6C3BE96}"/>
-    <hyperlink ref="A255" r:id="rId253" display="https://scrapsfromtheloft.com/comedy/henry-rollins-keep-talking-pal-transcript/" xr:uid="{BB3D6EED-8405-4795-956A-F4B208D7853A}"/>
-    <hyperlink ref="A256" r:id="rId254" display="https://scrapsfromtheloft.com/comedy/george-carlin-saturday-night-live-monologue1975-s01e01/" xr:uid="{EB500B4D-8FDC-4DA4-85E9-4153AEA33B03}"/>
-    <hyperlink ref="A257" r:id="rId255" display="https://scrapsfromtheloft.com/comedy/joe-rogan-strange-times-transcript/" xr:uid="{99621B67-D273-40C3-84E5-A9245AC1798A}"/>
-    <hyperlink ref="A258" r:id="rId256" display="https://scrapsfromtheloft.com/comedy/louis-ck-snl-monologue-s38e06-2012-transcript/" xr:uid="{476D347E-E860-423E-8D17-173F311370D2}"/>
-    <hyperlink ref="A259" r:id="rId257" display="https://scrapsfromtheloft.com/comedy/louis-c-k-snl-monologue-march-29-2014-full-transcript/" xr:uid="{ABE33F0E-67B0-42AE-8BE7-281F12985544}"/>
-    <hyperlink ref="A260" r:id="rId258" display="https://scrapsfromtheloft.com/comedy/sarah-silvermans-monologue-saturday-night-live-2014-transcript/" xr:uid="{77825692-807E-464B-82AD-4D0732B2F304}"/>
-    <hyperlink ref="A261" r:id="rId259" display="https://scrapsfromtheloft.com/comedy/louis-c-k-snl-monologue-2015-transcript/" xr:uid="{CAD2B358-1A2D-47EA-B9DD-EE584A7ECF66}"/>
-    <hyperlink ref="A262" r:id="rId260" display="https://scrapsfromtheloft.com/comedy/john-mulaney-snl-monologue-2018-transcript/" xr:uid="{4943C0D0-9651-4679-83DD-610D8E261A90}"/>
-    <hyperlink ref="A263" r:id="rId261" display="https://scrapsfromtheloft.com/comedy/david-chappelles-snl-monologue-2016-transcript/" xr:uid="{292497D1-C8EF-43BF-9B0A-42F006CDD67F}"/>
-    <hyperlink ref="A264" r:id="rId262" display="https://scrapsfromtheloft.com/comedy/d-l-hughley-contrarian-transcript/" xr:uid="{47488665-E446-4F0B-9333-93029992429E}"/>
-    <hyperlink ref="A265" r:id="rId263" display="https://scrapsfromtheloft.com/comedy/iliza-shlesinger-freezing-hot-transcript/" xr:uid="{31D9CF2B-827D-41EF-A342-A3C61724E59F}"/>
-    <hyperlink ref="A266" r:id="rId264" display="https://scrapsfromtheloft.com/comedy/iliza-shlesinger-war-paint-transcript/" xr:uid="{E98F38BC-7D70-4A11-860E-665EABB01DE0}"/>
-    <hyperlink ref="A267" r:id="rId265" display="https://scrapsfromtheloft.com/comedy/bert-kreischer-secret-time-transcript/" xr:uid="{760D9FF4-DC5E-475C-8B6C-65B53BA5E670}"/>
-    <hyperlink ref="A268" r:id="rId266" display="https://scrapsfromtheloft.com/comedy/dick-gregory-speech-st-johns-baptist-church-may-20-1963/" xr:uid="{0E70A489-CA2C-45B6-9FAE-0F3DE552C425}"/>
-    <hyperlink ref="A269" r:id="rId267" display="https://scrapsfromtheloft.com/comedy/demetri-martin-overthinker-transcript/" xr:uid="{DF1B4884-EB2E-4935-B154-6D71D4DBF99F}"/>
-    <hyperlink ref="A270" r:id="rId268" display="https://scrapsfromtheloft.com/comedy/bill-maher-live-from-oklahoma-2018-full-transcript/" xr:uid="{AFA939A5-26EF-4AD3-825F-12445DB20EE4}"/>
-    <hyperlink ref="A271" r:id="rId269" display="https://scrapsfromtheloft.com/comedy/rowan-atkinson-live-1992-transcript/" xr:uid="{4924B6CD-7377-46EF-A4A6-26F450D2CB10}"/>
-    <hyperlink ref="A272" r:id="rId270" display="https://scrapsfromtheloft.com/comedy/iliza-shlesinger-confirmed-kills-transcript/" xr:uid="{40236CFB-E00E-4266-AA15-CDDBFBDD63B9}"/>
-    <hyperlink ref="A273" r:id="rId271" display="https://scrapsfromtheloft.com/comedy/iliza-shlesinger-elder-millennial-2018-full-transcript/" xr:uid="{3C2F2AB5-8935-42AB-B33E-2D982E4B5B37}"/>
-    <hyperlink ref="A274" r:id="rId272" display="https://scrapsfromtheloft.com/comedy/jim-gaffigan-noble-ape-full-transcript/" xr:uid="{05266F29-6721-4909-912C-5A0EBCAAAFD6}"/>
-    <hyperlink ref="A275" r:id="rId273" display="https://scrapsfromtheloft.com/comedy/jim-norton-contextually-inadequate-full-transcript/" xr:uid="{090AC489-A932-4F8D-9C04-AD0D2C808BD9}"/>
-    <hyperlink ref="A276" r:id="rId274" display="https://scrapsfromtheloft.com/comedy/hannah-gadsby-nanette-transcript/" xr:uid="{7CF8ECCD-62DC-4134-8EF1-811B83073365}"/>
-    <hyperlink ref="A277" r:id="rId275" display="https://scrapsfromtheloft.com/comedy/brad-williams-daddy-issues-transcript/" xr:uid="{0A70C933-C92A-420E-B28B-02C90EBA660E}"/>
-    <hyperlink ref="A278" r:id="rId276" display="https://scrapsfromtheloft.com/comedy/deray-davis-how-to-act-black-transcript/" xr:uid="{0BA44745-4B42-4312-AE4C-8100547A4245}"/>
-    <hyperlink ref="A279" r:id="rId277" display="https://scrapsfromtheloft.com/comedy/ricky-gervais-live-iv-science-transcript/" xr:uid="{FDE2B252-1119-437E-80BC-8194BCEB841B}"/>
-    <hyperlink ref="A280" r:id="rId278" display="https://scrapsfromtheloft.com/comedy/jim-jefferies-this-is-me-now-transcript/" xr:uid="{2A5F4BEE-4CC7-4CCE-8592-844931E30759}"/>
-    <hyperlink ref="A281" r:id="rId279" display="https://scrapsfromtheloft.com/comedy/louis-c-k-chewed-up-transcript/" xr:uid="{D6E0180B-B898-4B06-BE4B-BDCBFB8C5F08}"/>
-    <hyperlink ref="A282" r:id="rId280" display="https://scrapsfromtheloft.com/comedy/bill-burr-the-philadelphia-incident-2006-transcript/" xr:uid="{DD662BF0-A782-4222-8C19-A2D52C8C6875}"/>
-    <hyperlink ref="A283" r:id="rId281" display="https://scrapsfromtheloft.com/comedy/russell-peters-outsourced-transcript/" xr:uid="{C4961752-EBBF-4FC8-A91F-DE472B532001}"/>
-    <hyperlink ref="A284" r:id="rId282" display="https://scrapsfromtheloft.com/comedy/russell-peters-almost-famous-2016-full-transcript/" xr:uid="{F6CE82C2-A3DD-428D-A7B5-D4473023CBF4}"/>
-    <hyperlink ref="A285" r:id="rId283" display="https://scrapsfromtheloft.com/comedy/ron-white-a-little-unprofessional-transcript/" xr:uid="{B46CFEAC-040B-4D79-B6CF-BA6996F96121}"/>
-    <hyperlink ref="A286" r:id="rId284" display="https://scrapsfromtheloft.com/comedy/michael-mcintyre-hello-wembley-transcript/" xr:uid="{B322ADAD-DEF5-43E4-A93A-D3F58F5E310F}"/>
-    <hyperlink ref="A287" r:id="rId285" display="https://scrapsfromtheloft.com/comedy/kevin-smith-silent-but-deadly-transcript/" xr:uid="{3B0992C5-0459-4209-A125-98056290AD31}"/>
-    <hyperlink ref="A288" r:id="rId286" display="https://scrapsfromtheloft.com/comedy/kevin-james-never-dont-give-up-full-transcript/" xr:uid="{EFCDA39C-7770-4080-82E5-1F5E0C9F9443}"/>
-    <hyperlink ref="A289" r:id="rId287" display="https://scrapsfromtheloft.com/comedy/trevor-noah-royal-wedding-2018/" xr:uid="{EC9866D0-6A33-416D-AC69-2DF5A851C015}"/>
-    <hyperlink ref="A290" r:id="rId288" display="https://scrapsfromtheloft.com/comedy/brent-morin-im-brent-morin-2015-full-transcript/" xr:uid="{7EB78E10-DC27-4707-AF18-CC3C0E8AD169}"/>
-    <hyperlink ref="A291" r:id="rId289" display="https://scrapsfromtheloft.com/comedy/nikki-glaser-perfect-2016-full-transcript/" xr:uid="{C539AB73-4C65-4970-AA45-52FAF851DD2A}"/>
-    <hyperlink ref="A292" r:id="rId290" display="https://scrapsfromtheloft.com/comedy/doug-stanhope-on-nationalism/" xr:uid="{F71E6699-A49B-42E7-B408-3C3653276008}"/>
-    <hyperlink ref="A293" r:id="rId291" display="https://scrapsfromtheloft.com/comedy/ali-wong-hard-knock-wife-transcript/" xr:uid="{50634716-CAFF-4807-A6D0-EF245604B58D}"/>
-    <hyperlink ref="A294" r:id="rId292" display="https://scrapsfromtheloft.com/comedy/kavin-jay-everybody-calm-down-full-transcript/" xr:uid="{2C25A5FA-58C1-4651-814F-0159D2F64E4D}"/>
-    <hyperlink ref="A295" r:id="rId293" display="https://scrapsfromtheloft.com/comedy/john-mulaney-kid-gorgeous-at-radio-city-full-transcript/" xr:uid="{5382F369-01E1-4321-B1A4-F88303F47DEC}"/>
-    <hyperlink ref="A296" r:id="rId294" display="https://scrapsfromtheloft.com/comedy/eddie-griffin-undeniable-2018-full-transcript/" xr:uid="{DED80B03-C04A-4C09-AAA0-323928B641FB}"/>
-    <hyperlink ref="A297" r:id="rId295" display="https://scrapsfromtheloft.com/comedy/greg-davies-you-magnificent-beast-full-transcript/" xr:uid="{EDB7394E-FDFC-4BBD-8604-E0E295F2C157}"/>
-    <hyperlink ref="A298" r:id="rId296" display="https://scrapsfromtheloft.com/comedy/comedy-central-patton-oswalt-1999-full-transcript/" xr:uid="{44E93FDA-F210-4D6C-B5A3-C147671A11EA}"/>
-    <hyperlink ref="A299" r:id="rId297" display="https://scrapsfromtheloft.com/comedy/george-carlin-you-are-all-diseased-transcript/" xr:uid="{E353F09A-7803-4746-B3FF-E52D97711899}"/>
-    <hyperlink ref="A300" r:id="rId298" display="https://scrapsfromtheloft.com/comedy/ricky-gervais-2012-golden-globes-opening-monologue/" xr:uid="{4895119E-D2C7-49E7-8AD6-EB8628111A92}"/>
-    <hyperlink ref="A301" r:id="rId299" display="https://scrapsfromtheloft.com/comedy/marlon-wayans-wokeish-transcript/" xr:uid="{A409FB5A-6E2F-40DF-988A-EAC8A61AE25C}"/>
-    <hyperlink ref="A302" r:id="rId300" display="https://scrapsfromtheloft.com/comedy/ricky-gervais-humanity-transcript/" xr:uid="{BCEF0668-5422-43AE-9A93-DFBA261BB4BA}"/>
-    <hyperlink ref="A303" r:id="rId301" display="https://scrapsfromtheloft.com/comedy/adel-karam-live-from-beirut-transcript/" xr:uid="{33C407C0-D8CF-41A6-A5BD-425F15E25416}"/>
-    <hyperlink ref="A304" r:id="rId302" display="https://scrapsfromtheloft.com/comedy/stewart-lee-90s-comedian-2006-full-transcript/" xr:uid="{5F52CD72-8715-4897-A842-C813A3867A45}"/>
-    <hyperlink ref="A305" r:id="rId303" display="https://scrapsfromtheloft.com/comedy/mike-birbiglia-my-girlfriends-boyfriend-2013-full-transcript/" xr:uid="{039A4450-5DC2-4887-BD39-6C1E4D02BED1}"/>
-    <hyperlink ref="A306" r:id="rId304" display="https://scrapsfromtheloft.com/comedy/dave-attell-road-work-transcript/" xr:uid="{6FFA399A-4F3F-4519-91A6-DC7B5409CAB9}"/>
-    <hyperlink ref="A307" r:id="rId305" display="https://scrapsfromtheloft.com/comedy/eddie-izzard-glorious-1997-full-transcript/" xr:uid="{EB503DCF-7F44-4657-A3D5-A6BFE1B27BE5}"/>
-    <hyperlink ref="A308" r:id="rId306" display="https://scrapsfromtheloft.com/comedy/chris-rock-bring-pain-transcript/" xr:uid="{04FA5472-9842-4A8C-9395-EBA7557AF5A7}"/>
-    <hyperlink ref="A309" r:id="rId307" display="https://scrapsfromtheloft.com/comedy/ari-shaffir-double-negative-transcript/" xr:uid="{E44A4536-F7E6-4D67-A0B7-5014631D5DAA}"/>
-    <hyperlink ref="A310" r:id="rId308" display="https://scrapsfromtheloft.com/comedy/chris-rock-tamborine-transcript/" xr:uid="{4E1468C8-B1C2-4046-9087-0C3260215C8B}"/>
-    <hyperlink ref="A311" r:id="rId309" display="https://scrapsfromtheloft.com/comedy/fred-armisen-standup-for-drummers-transcript/" xr:uid="{F92AD68E-6761-46C0-B513-A9DB1333CBB4}"/>
-    <hyperlink ref="A312" r:id="rId310" display="https://scrapsfromtheloft.com/comedy/dana-carvey-straight-white-male-60-2016-full-transcript/" xr:uid="{F8DD9088-A4E9-49B8-B7B8-1A95A995C716}"/>
-    <hyperlink ref="A313" r:id="rId311" display="https://scrapsfromtheloft.com/comedy/eddie-izzard-stripped-2009-full-transcript/" xr:uid="{B4973F13-68C0-4827-A30C-CC2C6C9773F8}"/>
-    <hyperlink ref="A314" r:id="rId312" display="https://scrapsfromtheloft.com/comedy/todd-glass-act-happy-transcript/" xr:uid="{E48EEA56-DC1F-4F7C-81E9-03CE4BCFB06F}"/>
-    <hyperlink ref="A315" r:id="rId313" display="https://scrapsfromtheloft.com/comedy/brian-regan-standing-up-2007-full-transcript/" xr:uid="{445F7E24-1C62-4552-A3A5-A5A63F96FB09}"/>
-    <hyperlink ref="A316" r:id="rId314" display="https://scrapsfromtheloft.com/comedy/brian-regan-nunchucks-flamethrowers-transcript/" xr:uid="{6DFF6FB9-B9D1-482F-B969-2816D7854F0C}"/>
-    <hyperlink ref="A317" r:id="rId315" display="https://scrapsfromtheloft.com/comedy/katt-williams-great-america-transcript/" xr:uid="{5EAA7AB5-7411-41D5-A6EC-59517CC236A2}"/>
-    <hyperlink ref="A318" r:id="rId316" display="https://scrapsfromtheloft.com/comedy/jimmy-carr-being-funny-transcript/" xr:uid="{9D61D4FA-3C71-4296-ABC4-5A7C0F3AA22C}"/>
-    <hyperlink ref="A319" r:id="rId317" display="https://scrapsfromtheloft.com/comedy/jimmy-carr-laughing-and-joking-transcript/" xr:uid="{44699F87-6EA3-47C0-A0A3-A74490572BEC}"/>
-    <hyperlink ref="A320" r:id="rId318" display="https://scrapsfromtheloft.com/comedy/eddie-izzard-unrepeatable-transcript/" xr:uid="{E2CE7857-B8A5-495A-8524-E8F78A747742}"/>
-    <hyperlink ref="A321" r:id="rId319" display="https://scrapsfromtheloft.com/comedy/d-l-hughley-unapologetic-transcript/" xr:uid="{852FCB34-503A-4FBC-B222-3D407409F1F6}"/>
-    <hyperlink ref="A322" r:id="rId320" display="https://scrapsfromtheloft.com/comedy/bridget-everett-gynecological-wonder-2015-full-transcript/" xr:uid="{E3C95DB7-0234-443B-B4C0-2ED6D60EF665}"/>
-    <hyperlink ref="A323" r:id="rId321" display="https://scrapsfromtheloft.com/comedy/chris-rock-never-scared-2004-full-transcript/" xr:uid="{7F57ED07-253C-4E62-89B7-91945C9A35C5}"/>
-    <hyperlink ref="A324" r:id="rId322" display="https://scrapsfromtheloft.com/comedy/stewart-lee-standup-comedian-full-transcript/" xr:uid="{7CA413D9-4C43-48DE-8F82-0B6DB0D09046}"/>
-    <hyperlink ref="A325" r:id="rId323" display="https://scrapsfromtheloft.com/comedy/jimmy-carr-funny-business-transcript/" xr:uid="{F44FDC33-B12C-49B3-A302-53B5B9962FCB}"/>
-    <hyperlink ref="A326" r:id="rId324" display="https://scrapsfromtheloft.com/comedy/eddie-izzard-dress-kill-1999-full-transcript/" xr:uid="{1799C577-6E0D-435D-BA4E-C63D1E6B6AA2}"/>
-    <hyperlink ref="A327" r:id="rId325" display="https://scrapsfromtheloft.com/comedy/chris-tucker-live-2015-transcript/" xr:uid="{9705962C-C745-4E70-B0F9-D2410C38E9F6}"/>
-    <hyperlink ref="A328" r:id="rId326" display="https://scrapsfromtheloft.com/comedy/kevin-hart-what-now-2016-full-transcript/" xr:uid="{49C8E8BB-DE88-4816-8F5B-80A77A144FBE}"/>
-    <hyperlink ref="A329" r:id="rId327" display="https://scrapsfromtheloft.com/comedy/kevin-hart-let-me-explain-2013-full-transcript/" xr:uid="{6728A3F2-B8B8-49F3-993E-F2299EEDBE63}"/>
-    <hyperlink ref="A330" r:id="rId328" display="https://scrapsfromtheloft.com/comedy/tom-segura-disgraceful-2018-full-transcript/" xr:uid="{74925C1E-CBBF-4156-A164-E94FDC816691}"/>
-    <hyperlink ref="A331" r:id="rId329" display="https://scrapsfromtheloft.com/comedy/bill-hicks-live-at-laff-stop-austin-tx-and-cobbs-san-francisco-ca-1993/" xr:uid="{443BC8E2-9C89-4D61-B3CD-A6B0775DA12D}"/>
-    <hyperlink ref="A332" r:id="rId330" display="https://scrapsfromtheloft.com/comedy/michelle-wolf-nice-lady-2017-full-transcript/" xr:uid="{A9FB563A-28C2-4D2E-B9E6-6882B8A29D1D}"/>
-    <hyperlink ref="A333" r:id="rId331" display="https://scrapsfromtheloft.com/comedy/fahim-anwar-theres-no-business-like-show-business-2017-full-transcript/" xr:uid="{A4ACF17A-5799-4EA1-A5D6-5832DA2F082E}"/>
-    <hyperlink ref="A334" r:id="rId332" display="https://scrapsfromtheloft.com/comedy/ellen-degeneres-the-beginning-2000-full-transcript/" xr:uid="{819B94A7-1FF7-4C5F-B6F0-95F93DA602E7}"/>
-    <hyperlink ref="A335" r:id="rId333" display="https://scrapsfromtheloft.com/comedy/maz-jobrani-immigrant-2017-full-transcript/" xr:uid="{8E98AB6A-FF2A-455B-9E09-E5D0B448C76B}"/>
-    <hyperlink ref="A336" r:id="rId334" display="https://scrapsfromtheloft.com/comedy/todd-barry-spicy-honey-2017-full-transcript/" xr:uid="{96D3BAD4-CC6B-49EE-8743-96E175CDA1EA}"/>
-    <hyperlink ref="A337" r:id="rId335" display="https://scrapsfromtheloft.com/comedy/jerry-seinfeld-im-telling-you-for-the-last-time-full-transcript/" xr:uid="{BB009DA9-6BF7-4B66-A4B4-8A4FAF0A5ECD}"/>
-    <hyperlink ref="A338" r:id="rId336" display="https://scrapsfromtheloft.com/comedy/craig-ferguson-does-this-need-to-be-said-transcript/" xr:uid="{F2967F33-EA75-40B6-80D3-EED06F1D425B}"/>
-    <hyperlink ref="A339" r:id="rId337" display="https://scrapsfromtheloft.com/comedy/craig-ferguson-tickle-fight-2017-full-transcript/" xr:uid="{CA84D59A-2710-4FA8-8E60-A2E4F63541CD}"/>
-    <hyperlink ref="A340" r:id="rId338" display="https://scrapsfromtheloft.com/comedy/dylan-moran-like-totally-2006-full-transcript/" xr:uid="{8FCBDBC8-486B-435D-B75C-034A2B5B6D5C}"/>
-    <hyperlink ref="A341" r:id="rId339" display="https://scrapsfromtheloft.com/comedy/dave-chappelle-equanimity-2017-transcripcion-completa/" xr:uid="{E193FFC3-EFA4-46EC-9DAC-3917BE9609B5}"/>
-    <hyperlink ref="A342" r:id="rId340" display="https://scrapsfromtheloft.com/movies/dave-chappelle-bird-revelation-2017-transcripcion-completa/" xr:uid="{B53DE219-FAF7-4650-BAAB-8BA6BA784286}"/>
-    <hyperlink ref="A343" r:id="rId341" display="https://scrapsfromtheloft.com/comedy/dave-chappelle-hbo-half-hour-1998-traduzione-italiana/" xr:uid="{7BFD5986-5B8F-4FB7-B94F-D7A69F59AE68}"/>
-    <hyperlink ref="A344" r:id="rId342" display="https://scrapsfromtheloft.com/comedy/trevor-noah-live-at-the-apollo-2013-transcript/" xr:uid="{9E4D7F9D-B5EE-4AD8-BA75-6F3D99EA4D4E}"/>
-    <hyperlink ref="A345" r:id="rId343" display="https://scrapsfromtheloft.com/comedy/dave-chappelle-the-bird-revelation-2017-full-transcript/" xr:uid="{7A303C16-63D7-4DF7-A76D-C28201CF51AB}"/>
-    <hyperlink ref="A346" r:id="rId344" display="https://scrapsfromtheloft.com/comedy/dave-chappelle-equanimity-2017-full-transcript/" xr:uid="{0A4B1C2A-07EA-4255-BBAB-344E42399331}"/>
-    <hyperlink ref="A347" r:id="rId345" display="https://scrapsfromtheloft.com/comedy/craig-ferguson-im-here-to-help-2013-full-transcript/" xr:uid="{4B6BC776-7D59-4759-A34E-23E321A7BA72}"/>
-    <hyperlink ref="A348" r:id="rId346" display="https://scrapsfromtheloft.com/comedy/russell-howard-recalibrate-2017-full-transcript/" xr:uid="{A204CCF8-7621-44D1-81E9-AB2E62AB5B78}"/>
-    <hyperlink ref="A349" r:id="rId347" display="https://scrapsfromtheloft.com/comedy/whitney-cummings-i-love-2014-full-transcript/" xr:uid="{32FC1A51-50E4-469D-82E2-B20564D74BE6}"/>
-    <hyperlink ref="A350" r:id="rId348" display="https://scrapsfromtheloft.com/comedy/whitney-cummings-im-your-girlfriend-2016-full-transcript/" xr:uid="{588B7D7A-46E1-48D6-BB6B-D20D8A4A31A3}"/>
-    <hyperlink ref="A351" r:id="rId349" display="https://scrapsfromtheloft.com/comedy/sarah-millican-chatterbox-live-2011-full-transcript/" xr:uid="{2FA33E0A-9162-4B62-9A46-1CE945E05600}"/>
-    <hyperlink ref="A352" r:id="rId350" display="https://scrapsfromtheloft.com/comedy/anjelah-johnson-not-fancy-transcript/" xr:uid="{C2E4C99E-E2B5-40E8-955B-69D5D1AA16EF}"/>
-    <hyperlink ref="A353" r:id="rId351" display="https://scrapsfromtheloft.com/movies/ricky-gervais-live-2-politics-2004-full-transcript/" xr:uid="{E86CEAF3-EA16-44A4-AE3B-73F4DF51D74C}"/>
-    <hyperlink ref="A354" r:id="rId352" display="https://scrapsfromtheloft.com/comedy/russell-howard-live-dingledodies-2009-full-transcript/" xr:uid="{AF150ED4-9E6C-4591-9D1F-19577869FB61}"/>
-    <hyperlink ref="A355" r:id="rId353" display="https://scrapsfromtheloft.com/comedy/christina-pazsitzky-mother-inferior-transcript/" xr:uid="{EBB4B9EF-6638-49F0-B589-D8A2678A4E16}"/>
-    <hyperlink ref="A356" r:id="rId354" display="https://scrapsfromtheloft.com/comedy/jack-whitehall-at-large-2017-full-transcript/" xr:uid="{B903D090-9F8B-4A66-A822-F08B716EE1AF}"/>
-    <hyperlink ref="A357" r:id="rId355" display="https://scrapsfromtheloft.com/comedy/cristela-alonzo-lower-classy-2017-full-transcript/" xr:uid="{8AE8B85C-088E-4F3D-BCC0-846130A89619}"/>
-    <hyperlink ref="A358" r:id="rId356" display="https://scrapsfromtheloft.com/comedy/judah-friedlander-america-is-the-greatest-country-in-the-united-states-2017-full-transcript/" xr:uid="{A64F1431-9A3C-47E1-AC8A-52CA8105B29F}"/>
-    <hyperlink ref="A359" r:id="rId357" display="https://scrapsfromtheloft.com/comedy/aziz-ansari-live-in-madison-square-garden-2015-full-transcript/" xr:uid="{13EA3EAF-8146-4FC0-BA25-79D1D288FB1D}"/>
-    <hyperlink ref="A360" r:id="rId358" display="https://scrapsfromtheloft.com/comedy/aziz-ansari-buried-alive-2013-full-transcript/" xr:uid="{5ADD9A1B-66C1-4E1D-BF19-F0111011B8B4}"/>
-    <hyperlink ref="A361" r:id="rId359" display="https://scrapsfromtheloft.com/comedy/paul-mooney-piece-mind-godbless-america-transcript/" xr:uid="{FCBA18B6-B74B-43F6-826B-5D1D2C3B461B}"/>
-    <hyperlink ref="A362" r:id="rId360" display="https://scrapsfromtheloft.com/comedy/patton-oswalt-annihilation-2017-full-transcript/" xr:uid="{F0F8A7DF-51CA-4CC2-8DBB-904427AD7BCF}"/>
-    <hyperlink ref="A363" r:id="rId361" display="https://scrapsfromtheloft.com/comedy/chris-rock-kill-the-messenger-london-new-york-johannesburg-2008-movie-script/" xr:uid="{1512E18E-E3F2-4494-9D5F-F249EDCC48A7}"/>
-    <hyperlink ref="A364" r:id="rId362" display="https://scrapsfromtheloft.com/comedy/bill-maher-live-from-d-c-2014-full-transcript/" xr:uid="{1B63FFE6-1076-4213-8BAE-1C6AEAAA70F5}"/>
-    <hyperlink ref="A365" r:id="rId363" display="https://scrapsfromtheloft.com/comedy/sarah-silverman-jesus-is-magic-2005-full-transcript/" xr:uid="{667D881A-9599-4DAF-AFFB-12488F647DD6}"/>
-    <hyperlink ref="A366" r:id="rId364" display="https://scrapsfromtheloft.com/comedy/sarah-silverman-we-are-miracles-2013-full-transcript/" xr:uid="{3FB07B42-06E3-4DF7-A709-32B301F25FAA}"/>
-    <hyperlink ref="A367" r:id="rId365" display="https://scrapsfromtheloft.com/comedy/pablo-francisco-ouch-live-san-jose-2006-full-transcript/" xr:uid="{FAD1DE1E-01DE-4098-8DC9-5AC5A47EC6CE}"/>
-    <hyperlink ref="A368" r:id="rId366" display="https://scrapsfromtheloft.com/comedy/bill-maher-but-im-not-wrong-2010-full-transcript/" xr:uid="{660221F3-B6AF-45D2-B6F9-4C7D588AF1F7}"/>
-    <hyperlink ref="A369" r:id="rId367" display="https://scrapsfromtheloft.com/comedy/russell-brand-messiah-complex-2013-full-transcript/" xr:uid="{5D100F7A-59EA-4557-A367-457F7CEADC2B}"/>
-    <hyperlink ref="A370" r:id="rId368" display="https://scrapsfromtheloft.com/comedy/chris-rock-bigger-blacker-1999-full-transcript/" xr:uid="{2FF8BD4A-BAA3-41B0-BAE5-3029842FC524}"/>
-    <hyperlink ref="A371" r:id="rId369" display="https://scrapsfromtheloft.com/comedy/gabriel-iglesias-hot-and-fluffy-2007-full-transcript/" xr:uid="{99828007-4F7B-45E4-B824-DF14943599F4}"/>
-    <hyperlink ref="A372" r:id="rId370" display="https://scrapsfromtheloft.com/comedy/gabriel-iglesias-im-not-fat-im-fluffy-2009-full-transcript/" xr:uid="{0C9CAD15-5D28-4D87-8E1A-AEEF4FE6594E}"/>
-    <hyperlink ref="A373" r:id="rId371" display="https://scrapsfromtheloft.com/comedy/gabriel-iglesias-im-sorry-for-what-i-said-when-i-was-hungry-2016-full-transcript/" xr:uid="{9A7C450A-C6A9-445A-8831-3CDACD0470E7}"/>
-    <hyperlink ref="A374" r:id="rId372" display="https://scrapsfromtheloft.com/comedy/george-carlin-pro-life-abortion-and-the-sanctity-of-life/" xr:uid="{C74D6FD4-6C91-4055-8A7C-D083C8482E8D}"/>
-    <hyperlink ref="A375" r:id="rId373" display="https://scrapsfromtheloft.com/comedy/richard-pryors-monologue-saturday-night-live-1975/" xr:uid="{685C2801-0B0D-4229-BBB6-EFB4EA6F6FDE}"/>
-    <hyperlink ref="A376" r:id="rId374" display="https://scrapsfromtheloft.com/comedy/rory-scovel-tries-stand-up-for-the-first-time-a-netflix-special/" xr:uid="{5C66D822-3C40-4D70-BD9A-4FD7726237AA}"/>
-    <hyperlink ref="A377" r:id="rId375" display="https://scrapsfromtheloft.com/comedy/lisa-lampanelli-back-to-the-drawing-board-2015-full-transcript/" xr:uid="{45EB51D5-18D8-4B61-8F0A-C08E994A6B8E}"/>
-    <hyperlink ref="A378" r:id="rId376" display="https://scrapsfromtheloft.com/comedy/comedy-central-presents-dave-attell-1999-full-transcript/" xr:uid="{860A8A5D-8759-403D-A380-9290D1408EF7}"/>
-    <hyperlink ref="A379" r:id="rId377" display="https://scrapsfromtheloft.com/comedy/erik-griffin-the-ugly-truth-2017-full-transcript/" xr:uid="{EABD20C5-FFB1-4E3C-8E2D-0F296F6D5B88}"/>
-    <hyperlink ref="A380" r:id="rId378" display="https://scrapsfromtheloft.com/comedy/chris-rocks-monologue-saturday-night-live-1996/" xr:uid="{F5AE0BA1-F91A-4455-B2B8-DFAFA18CCBB1}"/>
-    <hyperlink ref="A381" r:id="rId379" display="https://scrapsfromtheloft.com/comedy/jen-kirkman-just-keep-livin-2017-full-transcript/" xr:uid="{3C7A03EC-E626-482B-9D9B-2DA81E2E8F4D}"/>
-    <hyperlink ref="A382" r:id="rId380" display="https://scrapsfromtheloft.com/comedy/comedy-central-presents-daniel-tosh-2003-full-transcript/" xr:uid="{5110A35A-BE5F-4270-ACF1-CAA9724920A9}"/>
-    <hyperlink ref="A383" r:id="rId381" display="https://scrapsfromtheloft.com/comedy/george-carlin-religion-is-bullshit/" xr:uid="{D3F6A12D-F52F-4BFE-A704-D5E75264651D}"/>
-    <hyperlink ref="A384" r:id="rId382" display="https://scrapsfromtheloft.com/comedy/saturday-night-news-with-george-carlin-11-10-1984-transcript/" xr:uid="{BF1046CF-C48B-4AD1-8A8D-7F5470EEDE3B}"/>
-    <hyperlink ref="A385" r:id="rId383" display="https://scrapsfromtheloft.com/comedy/jim-jefferies-e-il-controllo-della-armi-in-america/" xr:uid="{D06F6EC6-66B9-4346-902B-80EF045873A6}"/>
-    <hyperlink ref="A386" r:id="rId384" display="https://scrapsfromtheloft.com/comedy/daniel-tosh-completely-serious-2007-full-transcript/" xr:uid="{61BE62B5-B917-456B-80FA-928DBABC7A15}"/>
-    <hyperlink ref="A387" r:id="rId385" display="https://scrapsfromtheloft.com/comedy/al-madrigal-why-is-the-rabbit-crying-2013-full-transcript/" xr:uid="{5DAC12C8-57CC-42D2-BC93-B00DB2A318E5}"/>
-    <hyperlink ref="A388" r:id="rId386" display="https://scrapsfromtheloft.com/comedy/neal-brennan-3-mics-2017-full-transcript/" xr:uid="{C1590D7F-099D-4439-9770-908CB2D5169C}"/>
-    <hyperlink ref="A389" r:id="rId387" display="https://scrapsfromtheloft.com/comedy/norm-macdonald-one-night-stand-1991/" xr:uid="{783AF5AE-573B-4FC0-A9D0-924E16B176CC}"/>
-    <hyperlink ref="A390" r:id="rId388" display="https://scrapsfromtheloft.com/comedy/john-mulaney-new-in-town-2012-full-transcript/" xr:uid="{C5875B2E-14F2-479F-AB7C-D687C4E565A9}"/>
-    <hyperlink ref="A391" r:id="rId389" display="https://scrapsfromtheloft.com/comedy/donald-glover-weirdo-transcript/" xr:uid="{5DC154C1-60BE-48E4-BB59-C72ED858DCE3}"/>
-    <hyperlink ref="A392" r:id="rId390" display="https://scrapsfromtheloft.com/comedy/ali-wong-baby-cobra-2016-full-transcript/" xr:uid="{1F40108F-861C-48EA-B60B-6C1EF7CD8A06}"/>
-    <hyperlink ref="A393" r:id="rId391" display="https://scrapsfromtheloft.com/comedy/norm-macdonald-hitlers-dog-gossip-trickery-2017-full-transcript/" xr:uid="{76C61EA1-97CB-4EB2-B0F7-86564191CD3A}"/>
-    <hyperlink ref="A394" r:id="rId392" display="https://scrapsfromtheloft.com/comedy/daniel-tosh-people-pleaser-2016-full-transcript/" xr:uid="{2DD4BB57-AB44-4D06-B156-ADF1A0438BE6}"/>
-    <hyperlink ref="A395" r:id="rId393" display="https://scrapsfromtheloft.com/comedy/marc-maron-more-later-2015-full-transcript/" xr:uid="{7E784723-47FB-4590-B86C-96ED6EDAD4B3}"/>
-    <hyperlink ref="A396" r:id="rId394" display="https://scrapsfromtheloft.com/comedy/dylan-moran-off-the-hook-2015-full-transcript/" xr:uid="{CBEAED70-4043-4D58-B320-40712C2B9C2F}"/>
-    <hyperlink ref="A397" r:id="rId395" display="https://scrapsfromtheloft.com/comedy/richard-pryor-live-and-smokin-1971-full-transcript/" xr:uid="{6D619A27-EF0B-4B00-BEE2-CDBB202C52E7}"/>
-    <hyperlink ref="A398" r:id="rId396" display="https://scrapsfromtheloft.com/movies/richard-pryor-here-and-now-1983/" xr:uid="{03FED81A-65DE-4DEE-AF80-1ABAD3D76D0A}"/>
-    <hyperlink ref="A399" r:id="rId397" display="https://scrapsfromtheloft.com/comedy/bill-burr-i-2008-testo-italiano-completo/" xr:uid="{9BAB76F7-7BB5-4D79-A1C2-15CEF3282C40}"/>
-    <hyperlink ref="A400" r:id="rId398" display="https://scrapsfromtheloft.com/movies/amy-schumer-mostly-sex-stuff-2012-full-transcript/" xr:uid="{6D56C838-9BD6-419D-9EC0-B41B90E95222}"/>
-    <hyperlink ref="A401" r:id="rId399" display="https://scrapsfromtheloft.com/comedy/jim-jefferies-alcoholocaust-2010-full-transcript/" xr:uid="{99C055C2-2095-45E0-BDF3-E61531DC469E}"/>
-    <hyperlink ref="A402" r:id="rId400" display="https://scrapsfromtheloft.com/movies/amy-schumer-live-apollo-2015-full-transcript/" xr:uid="{AC0B489C-87A9-4A37-A78C-26042120C4E0}"/>
-    <hyperlink ref="A403" r:id="rId401" display="https://scrapsfromtheloft.com/comedy/kevin-hart-seriously-funny-2010-full-transcript/" xr:uid="{AE7A32EB-F468-403E-B039-2EF8EC747F21}"/>
-    <hyperlink ref="A404" r:id="rId402" display="https://scrapsfromtheloft.com/comedy/hannibal-buress-comedy-camisado-2016-full-transcript/" xr:uid="{8AD18EEC-E969-4A45-80B5-520D6B17ACF8}"/>
-    <hyperlink ref="A405" r:id="rId403" display="https://scrapsfromtheloft.com/comedy/neal-brennan-women-and-black-dudes-transcript/" xr:uid="{45E25AC2-AA33-43C6-9F36-38AED1922C42}"/>
-    <hyperlink ref="A406" r:id="rId404" display="https://scrapsfromtheloft.com/comedy/nick-offerman-american-ham-2014-full-transcript/" xr:uid="{DDB69AFF-0D53-4EC9-8528-7755E435E3DC}"/>
-    <hyperlink ref="A407" r:id="rId405" display="https://scrapsfromtheloft.com/comedy/aziz-ansari-intimate-moments-sensual-evening-2010-full-transcript/" xr:uid="{F9974FBE-F1E5-4758-9E6A-94A13DAC2E80}"/>
-    <hyperlink ref="A408" r:id="rId406" display="https://scrapsfromtheloft.com/comedy/big-jay-oakerson-live-webster-hall-2016-full-transcript/" xr:uid="{EC4904A4-4BC3-4C2A-8924-685A2DC9FB3F}"/>
-    <hyperlink ref="A409" r:id="rId407" display="https://scrapsfromtheloft.com/comedy/lenny-bruce-berkeley-concert-1965-full-transcript/" xr:uid="{B84BFD44-5A06-491E-B7DA-1AEEAC2020C5}"/>
-    <hyperlink ref="A410" r:id="rId408" display="https://scrapsfromtheloft.com/comedy/doug-stanhope-no-refunds-2007-trascrizione-italiana/" xr:uid="{062B8D9B-BAF7-4410-9C9D-8520DD389CAC}"/>
-    <hyperlink ref="A411" r:id="rId409" display="https://scrapsfromtheloft.com/comedy/george-carlin-at-usc-1977-full-transcript/" xr:uid="{12B49538-F949-435F-A4B3-65F47B68FAF1}"/>
-    <hyperlink ref="A412" r:id="rId410" display="https://scrapsfromtheloft.com/comedy/jim-norton-mouthful-shame-transcript/" xr:uid="{DF4DEECA-DFBF-4EF6-A8D2-89B6163FD100}"/>
-    <hyperlink ref="A413" r:id="rId411" display="https://scrapsfromtheloft.com/comedy/michael-che-matters-transcript/" xr:uid="{3AC0F6CB-888E-428A-8E35-4DE6BAF287C7}"/>
-    <hyperlink ref="A414" r:id="rId412" display="https://scrapsfromtheloft.com/comedy/joe-rogan-triggered-2016-full-transcript/" xr:uid="{0BFE7F16-6112-43F1-A920-E37809D3A8A9}"/>
-    <hyperlink ref="A415" r:id="rId413" display="https://scrapsfromtheloft.com/comedy/trevor-noah-lost-translation-2015-full-transcript/" xr:uid="{0B578DB3-B37C-4F43-AC04-DEB576819DA5}"/>
-    <hyperlink ref="A416" r:id="rId414" display="https://scrapsfromtheloft.com/comedy/maria-bamford-old-baby-2017-full-transcript/" xr:uid="{5E8E36E9-07A3-462E-9278-2F6378ACD71E}"/>
-    <hyperlink ref="A417" r:id="rId415" display="https://scrapsfromtheloft.com/comedy/bo-burnham-what-transcript/" xr:uid="{AE2144FF-F24F-41F2-A968-CCBD7B67429E}"/>
-    <hyperlink ref="A418" r:id="rId416" display="https://scrapsfromtheloft.com/comedy/bo-burnham-make-happy-2016-full-transcript/" xr:uid="{B2713393-E87B-49C2-8512-F7F3EF26691A}"/>
-    <hyperlink ref="A419" r:id="rId417" display="https://scrapsfromtheloft.com/comedy/anthony-jeselnik-caligula-2013-full-transcript/" xr:uid="{135689C0-21CB-44E3-8996-CA9AF0F17076}"/>
-    <hyperlink ref="A420" r:id="rId418" display="https://scrapsfromtheloft.com/comedy/anthony-jeselnik-thoughts-prayers-2015-full-transcript/" xr:uid="{E79F2024-7A6B-419A-B891-5F184CF2177D}"/>
-    <hyperlink ref="A421" r:id="rId419" display="https://scrapsfromtheloft.com/comedy/john-mulaney-comeback-kid-2015-full-transcript/" xr:uid="{C5D8CE2F-AF50-4B97-9269-F25B4DDDCE44}"/>
-    <hyperlink ref="A422" r:id="rId420" display="https://scrapsfromtheloft.com/comedy/bill-hicks-revelations-1993-full-transcript/" xr:uid="{6A41967C-3B2A-4381-8A23-A74C6D0890CA}"/>
-    <hyperlink ref="A423" r:id="rId421" display="https://scrapsfromtheloft.com/comedy/lewis-black-black-future-2016-full-transcript/" xr:uid="{C756C6FC-B6B6-4F74-B19F-697985FA240A}"/>
-    <hyperlink ref="A424" r:id="rId422" display="https://scrapsfromtheloft.com/comedy/doug-stanhope-turning-gun-2012-transcript/" xr:uid="{22C9345C-248C-4D86-90F7-644013E0C300}"/>
-    <hyperlink ref="A425" r:id="rId423" display="https://scrapsfromtheloft.com/comedy/doug-stanhope-deadbeat-hero-2004-transcript/" xr:uid="{65328E0C-FA0A-4C0B-9941-DC520E0F272F}"/>
-    <hyperlink ref="A426" r:id="rId424" display="https://scrapsfromtheloft.com/comedy/jim-jefferies-contraband-2008-full-transcript/" xr:uid="{59A14800-2CBF-4DBD-B2F4-AFFFDEB06100}"/>
-    <hyperlink ref="A427" r:id="rId425" display="https://scrapsfromtheloft.com/comedy/mike-birbiglia-thank-god-jokes-2017-full-transcript/" xr:uid="{9D8B6073-982C-4936-92A8-B7F74E654229}"/>
-    <hyperlink ref="A428" r:id="rId426" display="https://scrapsfromtheloft.com/comedy/sarah-silverman-a-speck-of-dust-2017/" xr:uid="{CF2F767E-DB0F-4B15-9256-92F8C914C950}"/>
-    <hyperlink ref="A429" r:id="rId427" display="https://scrapsfromtheloft.com/comedy/george-carlin-playing-head-1986-full-transcript/" xr:uid="{6D843DE4-AC61-4324-91E4-C958775D7106}"/>
-    <hyperlink ref="A430" r:id="rId428" display="https://scrapsfromtheloft.com/comedy/george-carlin-1978-full-transcript/" xr:uid="{9D262801-A40A-4043-A42B-5BC855AB2723}"/>
-    <hyperlink ref="A431" r:id="rId429" display="https://scrapsfromtheloft.com/comedy/mitch-hedberg-comedy-central-special1999-full-transcript/" xr:uid="{857345E0-AB1A-4A73-B0FA-7A56EC37B033}"/>
-    <hyperlink ref="A432" r:id="rId430" display="https://scrapsfromtheloft.com/comedy/tom-segura-completely-normal-2014-full-transcript/" xr:uid="{925227BE-202B-4820-BAB9-1679EE3E259E}"/>
-    <hyperlink ref="A433" r:id="rId431" display="https://scrapsfromtheloft.com/comedy/george-carlin-carlin-campus-1984-full-transcript/" xr:uid="{CB32320F-853C-4E34-8C4C-FC8D9F7D74C3}"/>
-    <hyperlink ref="A434" r:id="rId432" display="https://scrapsfromtheloft.com/comedy/louis-c-k-live-at-the-beacon-theatre-2011-full-transcript/" xr:uid="{E3FE5A81-F91E-4D89-84CA-899192EF28AA}"/>
-    <hyperlink ref="A435" r:id="rId433" display="https://scrapsfromtheloft.com/comedy/ricky-gervais-england-2-2010-full-transcript/" xr:uid="{6E9A4494-2EC0-4A9A-9735-E49421BB2FCC}"/>
-    <hyperlink ref="A436" r:id="rId434" display="https://scrapsfromtheloft.com/comedy/amy-schumer-leather-special-2017-full-transcript/" xr:uid="{4BBE7954-4037-4621-862A-67111A7D286E}"/>
-    <hyperlink ref="A437" r:id="rId435" display="https://scrapsfromtheloft.com/comedy/jim-gaffigan-cinco-2017-full-transcript/" xr:uid="{8789260B-B720-4683-A3F1-E43BB97C0CBC}"/>
-    <hyperlink ref="A438" r:id="rId436" display="https://scrapsfromtheloft.com/comedy/jim-jefferies-i-swear-god-2009-full-transcript/" xr:uid="{D2F6658D-6D48-4EF4-BC09-BC1C368AF683}"/>
-    <hyperlink ref="A439" r:id="rId437" display="https://scrapsfromtheloft.com/comedy/louis-c-k-hilarious-2010-full-transcript/" xr:uid="{E47C6DBC-5220-436E-9EFC-8D13F8B20B66}"/>
-    <hyperlink ref="A440" r:id="rId438" display="https://scrapsfromtheloft.com/comedy/louis-c-k-shameless-2007-full-transcript/" xr:uid="{4E2FBE99-27CA-48B6-AC4E-7DDF22C77997}"/>
-    <hyperlink ref="A441" r:id="rId439" display="https://scrapsfromtheloft.com/comedy/bill-burr-im-sorry-feel-way-2014-full-transcript/" xr:uid="{96A7C660-FD88-4092-9533-00C100ABDF9F}"/>
-    <hyperlink ref="A442" r:id="rId440" display="https://scrapsfromtheloft.com/comedy/bill-burr-people-2012-full-transcript/" xr:uid="{67FF97FC-8FBB-4149-A0DD-731D13C977A4}"/>
-    <hyperlink ref="A443" r:id="rId441" display="https://scrapsfromtheloft.com/comedy/dave-chappelle-worth-2004-full-transcript/" xr:uid="{58E49691-5232-4995-A89A-D4580077F616}"/>
-    <hyperlink ref="A444" r:id="rId442" display="https://scrapsfromtheloft.com/comedy/dave-chappelle-killin-softly-2000-full-transcript/" xr:uid="{BFD91A7E-6520-4658-9435-AC2D1AC86123}"/>
-    <hyperlink ref="A445" r:id="rId443" display="https://scrapsfromtheloft.com/comedy/eddie-griffin-can-tell-em-i-said-transcript/" xr:uid="{760B74AE-6473-48BA-8DFB-EC7B02235782}"/>
-    <hyperlink ref="A446" r:id="rId444" display="https://scrapsfromtheloft.com/comedy/bill-burr-walk-way-2017-full-transcript/" xr:uid="{976AF3E2-C400-4042-9929-5BBC9AF8464B}"/>
-    <hyperlink ref="A447" r:id="rId445" display="https://scrapsfromtheloft.com/comedy/louis-ck-oh-my-god-full-transcript/" xr:uid="{73D79FB6-C8C4-4705-B544-F82AF76FB5AE}"/>
-    <hyperlink ref="A448" r:id="rId446" display="https://scrapsfromtheloft.com/comedy/louis-c-k-live-at-the-comedy-store-2015-transcript/" xr:uid="{AAA6CD50-3FFA-4581-8A9E-B834D434CEDA}"/>
-    <hyperlink ref="A449" r:id="rId447" display="https://scrapsfromtheloft.com/comedy/bill-hicks-relentless-1992-transcript/" xr:uid="{09FF7DDA-FF83-4316-A1E7-E682BC5DF708}"/>
-    <hyperlink ref="A450" r:id="rId448" display="https://scrapsfromtheloft.com/comedy/hasan-minhaj-white-house-correspondents-dinner-transcript/" xr:uid="{4EAEFEC6-5C59-4D76-8558-27C6B53B05D8}"/>
-    <hyperlink ref="A451" r:id="rId449" display="https://scrapsfromtheloft.com/comedy/daniel-tosh-happy-thoughts-transcript/" xr:uid="{DB7C35FE-BA61-4019-BF0F-F197C2F391A8}"/>
-    <hyperlink ref="A452" r:id="rId450" display="https://scrapsfromtheloft.com/comedy/patrice-oneal-elephant-in-the-room-2011-full-transcript/" xr:uid="{5B613BE4-4715-4178-8FFD-FB1FD10593DD}"/>
-    <hyperlink ref="A453" r:id="rId451" display="https://scrapsfromtheloft.com/comedy/katt-williams-live-2006-full-transcript/" xr:uid="{1AC2B586-766C-43D2-A24A-F07F5FDDCC54}"/>
-    <hyperlink ref="A454" r:id="rId452" display="https://scrapsfromtheloft.com/comedy/richard-pryor-live-concert-1979-full-transcript/" xr:uid="{8A370BA8-AA6F-4DC9-8CE4-9186163B9AF5}"/>
-    <hyperlink ref="A455" r:id="rId453" display="https://scrapsfromtheloft.com/comedy/richard-pryor-live-sunset-strip-1982-full-transcript/" xr:uid="{823116FC-B024-4026-B906-9C90958DB384}"/>
-    <hyperlink ref="A456" r:id="rId454" display="https://scrapsfromtheloft.com/comedy/george-carlin-seven-words-you-can-never-say-on-television/" xr:uid="{11DDEAA4-747B-412D-86BE-C95662CB5F13}"/>
-    <hyperlink ref="A457" r:id="rId455" display="https://scrapsfromtheloft.com/comedy/trevor-noah-afraid-dark-2017-full-transcript/" xr:uid="{36C7CC4C-A217-4E63-A455-63718D731197}"/>
-    <hyperlink ref="A458" r:id="rId456" display="https://scrapsfromtheloft.com/comedy/jim-jefferies-bare-2014-full-transcript/" xr:uid="{CC87369A-6A84-40AB-BE5D-D9132777A6B0}"/>
-    <hyperlink ref="A459" r:id="rId457" display="https://scrapsfromtheloft.com/comedy/dave-chappelle-deep-heart-texas-2017-full-transcript/" xr:uid="{42B3BA21-7F9C-411F-BDF6-F1E7ED7086E3}"/>
-    <hyperlink ref="A460" r:id="rId458" display="https://scrapsfromtheloft.com/comedy/tom-segura-mostly-stories-2016-full-transcript/" xr:uid="{617D29B0-5EC3-441A-9326-5C5AC6C92D69}"/>
-    <hyperlink ref="A461" r:id="rId459" display="https://scrapsfromtheloft.com/comedy/bill-burr-let-it-go-2010-full-transcript/" xr:uid="{A668F282-3C9D-41B4-B836-F7A86B147E60}"/>
-    <hyperlink ref="A462" r:id="rId460" display="https://scrapsfromtheloft.com/comedy/george-carlin-jamming-new-york-testo-italiano-completo/" xr:uid="{5B2E6B8C-DAFC-4BC1-9BC7-A3651811BBC3}"/>
-    <hyperlink ref="A463" r:id="rId461" display="https://scrapsfromtheloft.com/comedy/george-carlin-diseased-1999-testo-italiano-completo/" xr:uid="{DED2FA93-4C67-45E0-AF28-5BA6D547139D}"/>
-    <hyperlink ref="A464" r:id="rId462" display="https://scrapsfromtheloft.com/comedy/george-carlin-bad-2008-testo-italiano-completo/" xr:uid="{01609E28-E18B-4D89-BB16-8F8FA18EE461}"/>
-    <hyperlink ref="A465" r:id="rId463" display="https://scrapsfromtheloft.com/comedy/jim-jefferies-freedumb-2016-full-transcript/" xr:uid="{2F7DFF56-2F12-4630-BFC1-BDFEC387D6AC}"/>
-    <hyperlink ref="A466" r:id="rId464" display="https://scrapsfromtheloft.com/comedy/eddie-murphy-delirious-full-transcript/" xr:uid="{8847A120-0F0A-448D-A807-E956CC519E8C}"/>
-    <hyperlink ref="A467" r:id="rId465" display="https://scrapsfromtheloft.com/comedy/dave-chappelle-age-spin-2017-full-transcript/" xr:uid="{4BC8FFCD-9C6F-4C8E-A365-721DE32C0815}"/>
-    <hyperlink ref="A468" r:id="rId466" display="https://scrapsfromtheloft.com/comedy/george-carlin-back-town-1996-full-transcript/" xr:uid="{FC2E21C7-2076-48EA-8EBD-E49602DC4ED2}"/>
-    <hyperlink ref="A469" r:id="rId467" display="https://scrapsfromtheloft.com/comedy/seth-meyers-2011-white-house-correspondents-dinner-transcript/" xr:uid="{BDFFF244-CA5B-4DE0-B519-B765B516BB52}"/>
-    <hyperlink ref="A470" r:id="rId468" display="https://scrapsfromtheloft.com/comedy/louis-c-k-2017-full-transcript/" xr:uid="{327BD52E-54FF-46B0-A103-A519FDDBC596}"/>
-    <hyperlink ref="A471" r:id="rId469" display="https://scrapsfromtheloft.com/comedy/george-carlin-jamming-new-york-1992-full-transcript/" xr:uid="{A1A63194-040C-4649-820B-1EDD044CBE89}"/>
-    <hyperlink ref="A472" r:id="rId470" display="https://scrapsfromtheloft.com/comedy/jim-jefferies-gun-control-full-transcript/" xr:uid="{8E4EEC0B-06EB-4DD3-8001-98D29C1AA1CE}"/>
-    <hyperlink ref="A473" r:id="rId471" display="https://scrapsfromtheloft.com/comedy/reggie-watts-spatial-transcript/" xr:uid="{500DDC1D-EC71-441B-B053-9DB21BE42395}"/>
-    <hyperlink ref="A474" r:id="rId472" display="https://scrapsfromtheloft.com/comedy/george-carlin-complaints-grievances/" xr:uid="{E74E04DB-7E9B-4F98-8C5B-E5F9A12B3D09}"/>
-    <hyperlink ref="A475" r:id="rId473" display="https://scrapsfromtheloft.com/comedy/george-carlin-its-bad-for-ya/" xr:uid="{9AB3C2A7-B991-4877-8765-5258F6B45122}"/>
+    <hyperlink ref="A2" r:id="rId1" display="https://scrapsfromtheloft.com/comedy/pete-holmes-i-am-not-for-everyone-transcript/" xr:uid="{5A1D765B-06A2-49FE-BDA4-2A5B993608A1}"/>
+    <hyperlink ref="A3" r:id="rId2" display="https://scrapsfromtheloft.com/comedy/jeff-dunham-im-with-cupid-transcript/" xr:uid="{B0B29DFB-ABDE-4008-8EA5-1D27FE82B09B}"/>
+    <hyperlink ref="A4" r:id="rId3" display="https://scrapsfromtheloft.com/comedy/taylor-tomlinson-have-it-all-transcript/" xr:uid="{103F827F-24EC-4689-9102-48B055EF2FDD}"/>
+    <hyperlink ref="A5" r:id="rId4" display="https://scrapsfromtheloft.com/comedy/kevin-bridges-overdue-catch-up-transcript/" xr:uid="{A7F568A5-11B6-46D3-B2D9-7C87DA717B0A}"/>
+    <hyperlink ref="A6" r:id="rId5" display="https://scrapsfromtheloft.com/comedy/jacqueline-novak-get-on-your-knees-transcript/" xr:uid="{7692E464-8943-4D84-BA2B-5363B730D1C1}"/>
+    <hyperlink ref="A7" r:id="rId6" display="https://scrapsfromtheloft.com/comedy/kelsey-cook-the-hustler-transcript/" xr:uid="{9693B817-5A06-444C-82D3-BBAC48918F51}"/>
+    <hyperlink ref="A8" r:id="rId7" display="https://scrapsfromtheloft.com/comedy/dylan-moran-yeah-yeah-2011-transcript/" xr:uid="{51C0208E-82FD-4991-8787-A7270417625A}"/>
+    <hyperlink ref="A9" r:id="rId8" display="https://scrapsfromtheloft.com/comedy/dusty-slay-workin-man-transcript/" xr:uid="{B6E212AE-B1D2-45ED-A04A-3FCB565E9B1A}"/>
+    <hyperlink ref="A10" r:id="rId9" display="https://scrapsfromtheloft.com/comedy/jack-whitehall-settle-down-transcript/" xr:uid="{26C5255C-0209-41E5-B84E-FB020AE7AB14}"/>
+    <hyperlink ref="A11" r:id="rId10" display="https://scrapsfromtheloft.com/comedy/dylan-moran-what-it-is-transcript/" xr:uid="{99F33C3C-7B79-42F9-B96E-7A881B9E13F8}"/>
+    <hyperlink ref="A12" r:id="rId11" display="https://scrapsfromtheloft.com/comedy/kevin-james-irregardless-transcript/" xr:uid="{F48C2FB9-816C-40EC-97C0-279F70009A5C}"/>
+    <hyperlink ref="A13" r:id="rId12" display="https://scrapsfromtheloft.com/comedy/pete-davidson-turbo-fonzarelli-transcript/" xr:uid="{5CE31BAE-8266-47A7-945A-9514347478FE}"/>
+    <hyperlink ref="A14" r:id="rId13" display="https://scrapsfromtheloft.com/comedy/david-nihill-cultural-appreciation-transcript/" xr:uid="{1940523D-A103-423C-982F-4408D8A68B61}"/>
+    <hyperlink ref="A15" r:id="rId14" display="https://scrapsfromtheloft.com/comedy/matt-rife-matthew-steven-rife-transcript/" xr:uid="{D51A4658-261A-46B4-9F25-46142BEF6822}"/>
+    <hyperlink ref="A16" r:id="rId15" display="https://scrapsfromtheloft.com/comedy/shane-gillis-live-in-austin-transcript/" xr:uid="{1D73F476-BE79-4BC3-92AF-9A8F66F2A4FF}"/>
+    <hyperlink ref="A17" r:id="rId16" display="https://scrapsfromtheloft.com/comedy/lewis-black-tragically-i-need-you-transcript/" xr:uid="{EA61EA08-68B7-46DD-83B7-7D4B1F3E4B7B}"/>
+    <hyperlink ref="A18" r:id="rId17" display="https://scrapsfromtheloft.com/comedy/stavros-halkias-live-at-the-lodge-room-transcript/" xr:uid="{582622BF-6C06-4DBC-A8B0-37B7F6C2CE3C}"/>
+    <hyperlink ref="A19" r:id="rId18" display="https://scrapsfromtheloft.com/comedy/george-carlin-im-glad-im-dead-transcript/" xr:uid="{02F33CE5-BA29-4A86-B762-870B1F6EEF9F}"/>
+    <hyperlink ref="A20" r:id="rId19" display="https://scrapsfromtheloft.com/comedy/leanne-morgan-im-every-woman-transcript/" xr:uid="{4427E684-5AD4-4694-BF68-0AEE8840C6E9}"/>
+    <hyperlink ref="A21" r:id="rId20" display="https://scrapsfromtheloft.com/comedy/louis-ck-at-the-dolby-transcript/" xr:uid="{6FA7854F-995C-4C0C-983E-1A1D07543902}"/>
+    <hyperlink ref="A22" r:id="rId21" display="https://scrapsfromtheloft.com/comedy/roseanne-barr-cancel-this-transcript/" xr:uid="{B56BFF6C-BC17-4945-9A51-407389636B4F}"/>
+    <hyperlink ref="A23" r:id="rId22" display="https://scrapsfromtheloft.com/comedy/sammy-obeid-martyr-in-safe-space-transcript/" xr:uid="{E053EB31-A7E0-4BAC-94BC-CFA67D54C679}"/>
+    <hyperlink ref="A24" r:id="rId23" display="https://scrapsfromtheloft.com/comedy/sammy-obeid-where-is-bethlehem-transcript/" xr:uid="{0781BE37-A90C-4EFF-B6AB-BD942D928BE1}"/>
+    <hyperlink ref="A25" r:id="rId24" display="https://scrapsfromtheloft.com/comedy/sammy-obeid-palestine-censorship/" xr:uid="{A0E040FC-4C5A-42B1-92EE-E14DFA88EA17}"/>
+    <hyperlink ref="A26" r:id="rId25" display="https://scrapsfromtheloft.com/comedy/sammy-obeid-on-palestine-transcript/" xr:uid="{569C38DA-EC81-45C9-9D13-5D49CD798BA6}"/>
+    <hyperlink ref="A27" r:id="rId26" display="https://scrapsfromtheloft.com/comedy/dave-chappelle-the-dreamer-transcript/" xr:uid="{27D0EDF7-371E-4081-8012-1149BC40FD17}"/>
+    <hyperlink ref="A28" r:id="rId27" display="https://scrapsfromtheloft.com/comedy/gary-gulman-the-great-depresh-transcript/" xr:uid="{AB838C74-6B13-4A97-8594-550D7EC88590}"/>
+    <hyperlink ref="A29" r:id="rId28" display="https://scrapsfromtheloft.com/comedy/ricky-gervais-armageddon-transcript/" xr:uid="{CF928857-29C4-448A-89DB-6DDF81E06B1F}"/>
+    <hyperlink ref="A30" r:id="rId29" display="https://scrapsfromtheloft.com/comedy/gary-gulman-its-about-time-transcript/" xr:uid="{E589B5B6-FA85-42C2-8699-5091A348A3D4}"/>
+    <hyperlink ref="A31" r:id="rId30" display="https://scrapsfromtheloft.com/comedy/gary-gulman-born-on-3rd-base-transcript/" xr:uid="{CC303E0C-EBB7-4052-896A-EC5BFBF5EBC6}"/>
+    <hyperlink ref="A32" r:id="rId31" display="https://scrapsfromtheloft.com/comedy/trevor-noah-where-was-i-transcript/" xr:uid="{33A79624-DC03-411A-97C5-17B2085CF5B8}"/>
+    <hyperlink ref="A33" r:id="rId32" display="https://scrapsfromtheloft.com/comedy/maria-bamford-special-special-special-transcript/" xr:uid="{B9DAB39D-FD11-4D40-AD2D-32D6127E1EC4}"/>
+    <hyperlink ref="A34" r:id="rId33" display="https://scrapsfromtheloft.com/comedy/david-cross-making-america-great-again-transcript/" xr:uid="{EF0290DD-065D-4037-B470-2160A6C12B3B}"/>
+    <hyperlink ref="A35" r:id="rId34" display="https://scrapsfromtheloft.com/comedy/matt-rife-natural-selection-transcript/" xr:uid="{320771BD-7579-4BF6-9F7F-979102D48CA1}"/>
+    <hyperlink ref="A36" r:id="rId35" display="https://scrapsfromtheloft.com/comedy/mike-birbiglia-old-man-and-pool-transcript/" xr:uid="{E99853AA-59BE-4441-A5B0-C320A0FDABF5}"/>
+    <hyperlink ref="A37" r:id="rId36" display="https://scrapsfromtheloft.com/comedy/beth-stelling-girl-daddy-transcript/" xr:uid="{275BD693-9A5A-4FB9-B2B9-537E1F490AD1}"/>
+    <hyperlink ref="A38" r:id="rId37" display="https://scrapsfromtheloft.com/comedy/beth-stelling-if-you-didnt-want-me-then-transcript/" xr:uid="{72F3D415-3E9A-4990-BDA5-181C8D678160}"/>
+    <hyperlink ref="A39" r:id="rId38" display="https://scrapsfromtheloft.com/comedy/michelle-wolf-its-great-to-be-here-transcript/" xr:uid="{44AB3F1A-BBB5-4C8B-94D4-815367BC2688}"/>
+    <hyperlink ref="A40" r:id="rId39" display="https://scrapsfromtheloft.com/comedy/andrew-santino-home-field-advantage-transcript/" xr:uid="{0270D451-5285-49E4-8C4B-837684C2EC71}"/>
+    <hyperlink ref="A41" r:id="rId40" display="https://scrapsfromtheloft.com/comedy/shane-gillis-beautiful-dogs-transcript/" xr:uid="{56ACA4F0-CFA1-497D-834C-901B1AF627D2}"/>
+    <hyperlink ref="A42" r:id="rId41" display="https://scrapsfromtheloft.com/comedy/andrew-santino-cheeseburger-transcript/" xr:uid="{A43D24A2-35FA-407F-B732-16F165F13022}"/>
+    <hyperlink ref="A43" r:id="rId42" display="https://scrapsfromtheloft.com/comedy/jared-freid-37-and-single-transcript/" xr:uid="{3EECE32C-5C51-42C4-85D7-D886F0D7959D}"/>
+    <hyperlink ref="A44" r:id="rId43" display="https://scrapsfromtheloft.com/comedy/jim-gaffigan-dark-pale-transcript/" xr:uid="{95D28C6D-D32C-465C-AB48-B07BB786CE3C}"/>
+    <hyperlink ref="A45" r:id="rId44" display="https://scrapsfromtheloft.com/comedy/jim-gaffigan-obsessed-transcript/" xr:uid="{71868F17-B803-43BD-BC70-C708FEB639E3}"/>
+    <hyperlink ref="A46" r:id="rId45" display="https://scrapsfromtheloft.com/comedy/mark-normand-soup-to-nuts-transcript/" xr:uid="{658766F7-447D-4C30-8CF9-11BC39E4A0F0}"/>
+    <hyperlink ref="A47" r:id="rId46" display="https://scrapsfromtheloft.com/comedy/tom-segura-sledgehammer-transcript/" xr:uid="{130B2024-145A-451E-97A1-0802F0C7956D}"/>
+    <hyperlink ref="A48" r:id="rId47" display="https://scrapsfromtheloft.com/comedy/eddie-izzard-force-majeure-live-transcript/" xr:uid="{F3441139-8832-4351-AA7E-9D2B0DD5FFDC}"/>
+    <hyperlink ref="A49" r:id="rId48" display="https://scrapsfromtheloft.com/comedy/marlon-wayans-you-know-what-it-is-transcript/" xr:uid="{138144C1-6447-4473-BECA-FD472F1189AC}"/>
+    <hyperlink ref="A50" r:id="rId49" display="https://scrapsfromtheloft.com/comedy/kyle-kinane-whiskey-icarus-transcript/" xr:uid="{E7270BCC-027B-4611-8931-FCF01FF6C861}"/>
+    <hyperlink ref="A51" r:id="rId50" display="https://scrapsfromtheloft.com/comedy/kyle-kinane-loose-in-chicago-transcript/" xr:uid="{20A7F931-8E28-4282-BC06-AC6144F259DC}"/>
+    <hyperlink ref="A52" r:id="rId51" display="https://scrapsfromtheloft.com/comedy/mae-martin-sap-transcript/" xr:uid="{8CB7D3C9-4EA1-41C0-B0B7-1CEBE17E1B66}"/>
+    <hyperlink ref="A53" r:id="rId52" display="https://scrapsfromtheloft.com/comedy/amy-schumer-emergency-contact-transcript/" xr:uid="{23C89BD9-C383-4ED2-8C5A-B4EF9E232564}"/>
+    <hyperlink ref="A54" r:id="rId53" display="https://scrapsfromtheloft.com/comedy/wanda-sykes-im-an-entertainer-transcript/" xr:uid="{5879064C-47CD-43B0-91C1-EA1F1B1DCB19}"/>
+    <hyperlink ref="A55" r:id="rId54" display="https://scrapsfromtheloft.com/comedy/john-mulaney-baby-j-transcript/" xr:uid="{01979D08-EE3E-4054-B8DD-E0C091F9300F}"/>
+    <hyperlink ref="A56" r:id="rId55" display="https://scrapsfromtheloft.com/comedy/kathleen-madigan-hunting-bigfoot-transcript/" xr:uid="{5241BA9A-2293-48AF-8CC0-49D7E9C26709}"/>
+    <hyperlink ref="A57" r:id="rId56" display="https://scrapsfromtheloft.com/comedy/marc-maron-from-bleak-to-dark-transcript/" xr:uid="{003AD07F-770F-45EF-8F2F-643268147328}"/>
+    <hyperlink ref="A58" r:id="rId57" display="https://scrapsfromtheloft.com/comedy/bert-kreischer-razzle-dazzle-transcript/" xr:uid="{A0DC67F6-22C8-42CF-80BA-CBC6A2A5DD78}"/>
+    <hyperlink ref="A59" r:id="rId58" display="https://scrapsfromtheloft.com/comedy/chris-rock-selective-outrage-transcript/" xr:uid="{E76CD361-0D9B-4D87-88FC-C28102BDA6D7}"/>
+    <hyperlink ref="A60" r:id="rId59" display="https://scrapsfromtheloft.com/comedy/marc-maron-thinky-pain-transcript/" xr:uid="{B7C6A84F-1BC8-46ED-9505-768A8411E813}"/>
+    <hyperlink ref="A61" r:id="rId60" display="https://scrapsfromtheloft.com/comedy/chelsea-handler-evolution-transcript/" xr:uid="{119F2563-F9C6-4204-9AF9-750553FA1FDE}"/>
+    <hyperlink ref="A62" r:id="rId61" display="https://scrapsfromtheloft.com/comedy/tom-papa-what-a-day-transcript/" xr:uid="{F588BA02-5EBF-4767-84C4-94B8C2AF9983}"/>
+    <hyperlink ref="A63" r:id="rId62" display="https://scrapsfromtheloft.com/comedy/jim-jefferies-high-n-dry-transcript/" xr:uid="{7B8E60CD-6566-4020-A48C-0BF3A94DC8C1}"/>
+    <hyperlink ref="A64" r:id="rId63" display="https://scrapsfromtheloft.com/comedy/dave-chappelle-monologue-snl-2022-transcript/" xr:uid="{1434AA6F-7A8D-4AB9-94EC-8938E743419F}"/>
+    <hyperlink ref="A65" r:id="rId64" display="https://scrapsfromtheloft.com/comedy/dave-chappelle-whats-in-a-name-transcript/" xr:uid="{4A67C691-3641-4E69-B582-E07CE3B96A42}"/>
+    <hyperlink ref="A66" r:id="rId65" display="https://scrapsfromtheloft.com/comedy/iliza-shlesinger-hot-forever-transcript/" xr:uid="{4C4E5619-DCCB-46B3-9AF3-F32F199A27BB}"/>
+    <hyperlink ref="A67" r:id="rId66" display="https://scrapsfromtheloft.com/comedy/gabriel-iglesias-stadium-fluffy-transcript/" xr:uid="{2CC29002-1846-4602-8A65-DF109AA92D44}"/>
+    <hyperlink ref="A68" r:id="rId67" display="https://scrapsfromtheloft.com/comedy/fortune-feimster-good-fortune-transcript/" xr:uid="{43348BEB-168B-4CF2-9EE5-7A9B05FB23AB}"/>
+    <hyperlink ref="A69" r:id="rId68" display="https://scrapsfromtheloft.com/comedy/deon-cole-charleens-boy-transcript/" xr:uid="{0E3EEF81-2D90-4CC4-8DFA-1B2B2658E1EE}"/>
+    <hyperlink ref="A70" r:id="rId69" display="https://scrapsfromtheloft.com/comedy/neal-brennan-blocks-transcript/" xr:uid="{2F0E5B77-96E9-4B57-A570-1FA3CFF70D15}"/>
+    <hyperlink ref="A71" r:id="rId70" display="https://scrapsfromtheloft.com/comedy/trevor-noah-i-wish-you-would-transcript/" xr:uid="{C9E739FB-B0D0-43AF-AC88-FF5CDA6E8E6A}"/>
+    <hyperlink ref="A72" r:id="rId71" display="https://scrapsfromtheloft.com/comedy/whitney-cummings-jokes-transcript/" xr:uid="{398274B3-82FC-4F71-82F7-31B73230A375}"/>
+    <hyperlink ref="A73" r:id="rId72" display="https://scrapsfromtheloft.com/comedy/kate-berlant-cinnamon-in-the-wind-transcript/" xr:uid="{01A6C34F-B8F2-4224-849B-4836DC21374E}"/>
+    <hyperlink ref="A74" r:id="rId73" display="https://scrapsfromtheloft.com/comedy/patton-oswalt-we-all-scream-transcript/" xr:uid="{8659D14A-3BFC-49B1-BAB4-C9FD2B303DDD}"/>
+    <hyperlink ref="A75" r:id="rId74" display="https://scrapsfromtheloft.com/comedy/orny-adams-more-than-loud-transcript/" xr:uid="{458CF1FB-F993-4CE5-AA95-A166A91CC5D6}"/>
+    <hyperlink ref="A76" r:id="rId75" display="https://scrapsfromtheloft.com/comedy/bill-burr-live-at-red-rocks-transcript/" xr:uid="{EAE8F4AB-FC97-4213-A775-0AF1FB9B8881}"/>
+    <hyperlink ref="A77" r:id="rId76" display="https://scrapsfromtheloft.com/comedy/jon-stewart-acceptance-speech-2022-mark-twain-prize/" xr:uid="{5C98BD8C-D047-45A7-9CFF-2A8502F7FEBE}"/>
+    <hyperlink ref="A78" r:id="rId77" display="https://scrapsfromtheloft.com/comedy/pete-davidson-presents-the-best-friends-transcript/" xr:uid="{0DB4D68D-4E58-4780-850C-08264CEDE938}"/>
+    <hyperlink ref="A79" r:id="rId78" display="https://scrapsfromtheloft.com/comedy/amy-schumer-presents-parental-advisory-transcript/" xr:uid="{2F5F84A9-0A0B-416B-9002-CAF9DCE1ECA7}"/>
+    <hyperlink ref="A80" r:id="rId79" display="https://scrapsfromtheloft.com/comedy/bill-burr-presents-friends-who-kill-transcript/" xr:uid="{52452733-0AE7-4A32-9594-A28586828AA9}"/>
+    <hyperlink ref="A81" r:id="rId80" display="https://scrapsfromtheloft.com/comedy/norm-macdonald-nothing-special-transcript/" xr:uid="{0706AF62-2CB6-4A95-B943-0EC5B22DD9EA}"/>
+    <hyperlink ref="A82" r:id="rId81" display="https://scrapsfromtheloft.com/comedy/ricky-gervais-supernature-transcript/" xr:uid="{E3A2A904-F047-46D8-9396-9DCD252020B5}"/>
+    <hyperlink ref="A83" r:id="rId82" display="https://scrapsfromtheloft.com/comedy/mike-epps-under-rated-never-faded-x-rated-transcript/" xr:uid="{A9C7B963-8628-454B-B657-FE4AEC724CF9}"/>
+    <hyperlink ref="A84" r:id="rId83" display="https://scrapsfromtheloft.com/comedy/mike-epps-dont-take-it-personal-transcript/" xr:uid="{0B25DD54-D623-405B-B02B-47A2F2A5E75D}"/>
+    <hyperlink ref="A85" r:id="rId84" display="https://scrapsfromtheloft.com/comedy/catherine-cohen-the-twist-she-gorgeous-transcript/" xr:uid="{5DDA4DEF-1630-4A86-A0A3-7C94EF765733}"/>
+    <hyperlink ref="A86" r:id="rId85" display="https://scrapsfromtheloft.com/comedy/mike-epps-indiana-mike-transcript/" xr:uid="{313AEE6C-EEA2-4ECF-B028-CF35244A44C6}"/>
+    <hyperlink ref="A87" r:id="rId86" display="https://scrapsfromtheloft.com/comedy/jerrod-carmichael-rothaniel-transcript/" xr:uid="{1B68785C-E27A-4DCA-8883-654EF9D3E358}"/>
+    <hyperlink ref="A88" r:id="rId87" display="https://scrapsfromtheloft.com/comedy/taylor-tomlinson-look-at-you-transcript/" xr:uid="{19633DE2-5841-4790-BA8C-17E6FAD75ADF}"/>
+    <hyperlink ref="A89" r:id="rId88" display="https://scrapsfromtheloft.com/comedy/taylor-tomlinson-quarter-life-crisis-transcript/" xr:uid="{CC3384BF-D97D-4D34-899F-678F1EF333CB}"/>
+    <hyperlink ref="A90" r:id="rId89" display="https://scrapsfromtheloft.com/comedy/moses-storm-trash-white-transcript/" xr:uid="{BCDC121A-FF2F-481C-9B92-7AD0FD7BA71D}"/>
+    <hyperlink ref="A91" r:id="rId90" display="https://scrapsfromtheloft.com/comedy/trevor-noah-white-house-correspondents-dinner-2022-transcript/" xr:uid="{9D20C3B0-17BB-4BC9-8993-53A8A1DA84DE}"/>
+    <hyperlink ref="A92" r:id="rId91" display="https://scrapsfromtheloft.com/comedy/ali-wong-don-wong-transcript/" xr:uid="{56987CA9-BC60-4B45-A639-835DDBE72193}"/>
+    <hyperlink ref="A93" r:id="rId92" display="https://scrapsfromtheloft.com/comedy/aziz-ansari-nightclub-comedian-transcript/" xr:uid="{620C4C02-D013-4B79-B80C-455B2F224801}"/>
+    <hyperlink ref="A94" r:id="rId93" display="https://scrapsfromtheloft.com/comedy/jim-gaffigan-comedy-monster-transcript/" xr:uid="{0804EE60-73FF-4C1E-9C60-53F788C57527}"/>
+    <hyperlink ref="A95" r:id="rId94" display="https://scrapsfromtheloft.com/comedy/louis-c-k-sorry-transcript/" xr:uid="{8D8A75CD-2960-4788-A201-CD7447A9CD8F}"/>
+    <hyperlink ref="A96" r:id="rId95" display="https://scrapsfromtheloft.com/comedy/drew-michael-drew-michael-2018-transcript/" xr:uid="{4E30AA5B-9642-4AF8-AEB1-C8951B3CBB72}"/>
+    <hyperlink ref="A97" r:id="rId96" display="https://scrapsfromtheloft.com/comedy/drew-michael-red-blue-green-transcript/" xr:uid="{A2C28084-BED3-4165-9E9B-2925D053355D}"/>
+    <hyperlink ref="A98" r:id="rId97" display="https://scrapsfromtheloft.com/comedy/mo-amer-mohammed-in-texas-transcript/" xr:uid="{3B8B17E7-1A29-4A30-A30F-A9CF54157D33}"/>
+    <hyperlink ref="A99" r:id="rId98" display="https://scrapsfromtheloft.com/comedy/dave-chappelle-the-closer-transcript/" xr:uid="{6FB89A96-DB6D-4D0A-9D11-346EB139A59C}"/>
+    <hyperlink ref="A100" r:id="rId99" display="https://scrapsfromtheloft.com/comedy/kathleen-madigan-bothering-jesus-transcript/" xr:uid="{D0801BB9-5BCC-435F-A99A-9ABB068695F2}"/>
+    <hyperlink ref="A101" r:id="rId100" display="https://scrapsfromtheloft.com/comedy/kathleen-madigan-madigan-again-transcript/" xr:uid="{5C618F8D-BEC1-479B-AE27-E83EAFAB95A0}"/>
+    <hyperlink ref="A102" r:id="rId101" display="https://scrapsfromtheloft.com/comedy/phil-wang-philly-philly-wang-wang-transcript/" xr:uid="{635ED003-0DDA-4E5F-B1D7-D896AD1E1C45}"/>
+    <hyperlink ref="A103" r:id="rId102" display="https://scrapsfromtheloft.com/comedy/dave-chappelle-846-transcript/" xr:uid="{C32677AD-48A3-43C4-B4F2-63EC1DB51B60}"/>
+    <hyperlink ref="A104" r:id="rId103" display="https://scrapsfromtheloft.com/comedy/tom-papa-youre-doing-great-transcript/" xr:uid="{4E7B839C-41F1-4FDA-AC46-504B073D9084}"/>
+    <hyperlink ref="A105" r:id="rId104" display="https://scrapsfromtheloft.com/comedy/tom-papa-human-mule-transcript/" xr:uid="{66275D45-FD4E-4902-8FA9-AD456D2D8A9F}"/>
+    <hyperlink ref="A106" r:id="rId105" display="https://scrapsfromtheloft.com/comedy/tom-papa-freaked-out-transcript/" xr:uid="{AD8A8B62-366D-4448-84FC-E735BB187BE4}"/>
+    <hyperlink ref="A107" r:id="rId106" display="https://scrapsfromtheloft.com/comedy/bo-burnham-inside-transcript/" xr:uid="{2C64B8C6-4EFA-46E4-87EF-0BC25CFB5C36}"/>
+    <hyperlink ref="A108" r:id="rId107" display="https://scrapsfromtheloft.com/comedy/tig-notaro-boyish-girl-interrupted-transcript/" xr:uid="{9F74A07F-BCCB-488B-A6FA-6AE219CE3DDD}"/>
+    <hyperlink ref="A109" r:id="rId108" display="https://scrapsfromtheloft.com/comedy/joe-list-i-hate-myself-transcript/" xr:uid="{4A517A92-43EA-4378-856F-8823824B9454}"/>
+    <hyperlink ref="A110" r:id="rId109" display="https://scrapsfromtheloft.com/comedy/nate-bargatze-greatest-average-american-transcript/" xr:uid="{808DE029-55A6-496A-B3E1-37E70E354777}"/>
+    <hyperlink ref="A111" r:id="rId110" display="https://scrapsfromtheloft.com/comedy/brian-regan-on-the-rocks-transcript/" xr:uid="{143C3DFB-426C-4F4F-A8F1-B8796327CD77}"/>
+    <hyperlink ref="A112" r:id="rId111" display="https://scrapsfromtheloft.com/comedy/george-carlin-politically-correct-language/" xr:uid="{6D7B449C-8EC2-493D-83E9-1CC0B3A40661}"/>
+    <hyperlink ref="A113" r:id="rId112" display="https://scrapsfromtheloft.com/comedy/doug-stanhope-beer-hall-putsch-transcript/" xr:uid="{903A1195-357E-4307-A44B-38CF6A47EAF0}"/>
+    <hyperlink ref="A114" r:id="rId113" display="https://scrapsfromtheloft.com/comedy/chris-rock-total-blackout-the-tamborine-extended-cut-transcript/" xr:uid="{0AAED6DC-BC35-49BB-AB60-59E767B7F9D8}"/>
+    <hyperlink ref="A115" r:id="rId114" display="https://scrapsfromtheloft.com/comedy/george-carlin-life-worth-losing-transcript/" xr:uid="{61A8D5B7-44AA-473D-85F6-F7666220CC0A}"/>
+    <hyperlink ref="A116" r:id="rId115" display="https://scrapsfromtheloft.com/comedy/sarah-cooper-everythings-fine-transcript/" xr:uid="{58DF5534-8D8C-4558-9DEE-5EA3E08A70A8}"/>
+    <hyperlink ref="A117" r:id="rId116" display="https://scrapsfromtheloft.com/comedy/bo-burnham-words-words-words-transcript/" xr:uid="{4F62E633-E1A8-40EA-8945-63F6054122FE}"/>
+    <hyperlink ref="A118" r:id="rId117" display="https://scrapsfromtheloft.com/comedy/vir-das-outside-in-the-lockdown-special-transcript/" xr:uid="{3D63A592-1E13-42CC-B427-F21C20AE678C}"/>
+    <hyperlink ref="A119" r:id="rId118" display="https://scrapsfromtheloft.com/comedy/larry-the-cable-guy-remain-seated-transcript/" xr:uid="{A38CE093-B7CA-4776-896A-C505283E53E6}"/>
+    <hyperlink ref="A120" r:id="rId119" display="https://scrapsfromtheloft.com/comedy/craig-ferguson-just-being-honest-transcript/" xr:uid="{3C3F8D19-FF85-43BF-9D50-75D654EFBC33}"/>
+    <hyperlink ref="A121" r:id="rId120" display="https://scrapsfromtheloft.com/comedy/kevin-hart-zero-fks-given-2020-transcript/" xr:uid="{2662A13A-09C0-4000-A057-74A9E1942F5E}"/>
+    <hyperlink ref="A122" r:id="rId121" display="https://scrapsfromtheloft.com/comedy/sam-morril-i-got-this-2020-transcript/" xr:uid="{E2C4D97E-8D52-4FA7-89C7-093232B6E00A}"/>
+    <hyperlink ref="A123" r:id="rId122" display="https://scrapsfromtheloft.com/comedy/dave-chappelle-snl-monologue-2020-transcript/" xr:uid="{D3215B21-C8F6-4FF0-8FA9-306D44A360AA}"/>
+    <hyperlink ref="A124" r:id="rId123" display="https://scrapsfromtheloft.com/comedy/chris-rock-snl-monologue-2020-transcript/" xr:uid="{C6E9E2F5-6BE0-42AE-BF4A-09C9B4DBAF0B}"/>
+    <hyperlink ref="A125" r:id="rId124" display="https://scrapsfromtheloft.com/comedy/bill-burr-snl-monologue-2020-transcript/" xr:uid="{57E57DDF-3C15-46ED-945A-393A6BE85F66}"/>
+    <hyperlink ref="A126" r:id="rId125" display="https://scrapsfromtheloft.com/comedy/john-mulaney-snl-monologue-2020-transcript/" xr:uid="{E1A1DC93-219F-49FC-871D-F7FB8CD66980}"/>
+    <hyperlink ref="A127" r:id="rId126" display="https://scrapsfromtheloft.com/comedy/ronny-chieng-asian-comedian-destroys-america-transcript/" xr:uid="{79E6A364-575E-4B13-9A0C-AC977AD8FBB6}"/>
+    <hyperlink ref="A128" r:id="rId127" display="https://scrapsfromtheloft.com/comedy/craig-ferguson-a-wee-bit-o-revolution-transcript/" xr:uid="{A33111DD-B534-4938-B617-DEEAB3312E8A}"/>
+    <hyperlink ref="A129" r:id="rId128" display="https://scrapsfromtheloft.com/comedy/michael-mcintyre-showman-transcript/" xr:uid="{46EF93DF-25B1-467A-9CDA-EE85B73271F2}"/>
+    <hyperlink ref="A130" r:id="rId129" display="https://scrapsfromtheloft.com/comedy/rob-schneider-asian-momma-mexican-kids-transcript/" xr:uid="{69DE029C-2DC8-4EA0-AA94-105521863FC5}"/>
+    <hyperlink ref="A131" r:id="rId130" display="https://scrapsfromtheloft.com/comedy/sam-jay-3-in-the-morning-transcript/" xr:uid="{D3A50ECE-A607-4DCC-8C23-48F472C3AE4D}"/>
+    <hyperlink ref="A132" r:id="rId131" display="https://scrapsfromtheloft.com/comedy/jack-whitehall-im-only-joking-transcript/" xr:uid="{02167311-F9B8-4B2C-9697-2F0CBB595180}"/>
+    <hyperlink ref="A133" r:id="rId132" display="https://scrapsfromtheloft.com/comedy/urzila-carlson-overqualified-loser-transcript/" xr:uid="{77F892BA-0DB3-444B-AD36-69602E309037}"/>
+    <hyperlink ref="A134" r:id="rId133" display="https://scrapsfromtheloft.com/comedy/george-lopez-well-do-it-for-half-transcript/" xr:uid="{04142243-8610-447A-A81A-67C99FE7D179}"/>
+    <hyperlink ref="A135" r:id="rId134" display="https://scrapsfromtheloft.com/comedy/jim-jefferies-intolerant-transcript/" xr:uid="{2403AEF5-D047-4F8E-9CB0-924A31826541}"/>
+    <hyperlink ref="A136" r:id="rId135" display="https://scrapsfromtheloft.com/comedy/bill-hicks-censored-david-letterman-transcript/" xr:uid="{E92E9AA6-A596-4131-BE29-7A8F022E1BD7}"/>
+    <hyperlink ref="A137" r:id="rId136" display="https://scrapsfromtheloft.com/comedy/george-carlin-doin-it-again-transcript/" xr:uid="{A2052C3A-68A7-4B9B-8617-18D6A6E99DCA}"/>
+    <hyperlink ref="A138" r:id="rId137" display="https://scrapsfromtheloft.com/comedy/eric-andre-legalize-everything-transcript/" xr:uid="{B349E504-7C7D-4255-9E5B-18D896F3B398}"/>
+    <hyperlink ref="A139" r:id="rId138" display="https://scrapsfromtheloft.com/comedy/roy-wood-jr-father-figure-transcript/" xr:uid="{F745C385-DA3C-4EB7-B472-F4E649884604}"/>
+    <hyperlink ref="A140" r:id="rId139" display="https://scrapsfromtheloft.com/comedy/dave-chappelle-hbo-comedy-half-hour-1998-transcript/" xr:uid="{02B0E273-9452-46D8-94E2-5515DE66D468}"/>
+    <hyperlink ref="A141" r:id="rId140" display="https://scrapsfromtheloft.com/comedy/mark-normand-dont-be-yourself-transcript/" xr:uid="{874620AA-BD19-4AFB-99CA-CB640B258141}"/>
+    <hyperlink ref="A142" r:id="rId141" display="https://scrapsfromtheloft.com/comedy/doug-stanhope-fear-of-an-empty-bed-transcript/" xr:uid="{89849FAA-F300-4B65-8139-BC9AC20D3BAC}"/>
+    <hyperlink ref="A143" r:id="rId142" display="https://scrapsfromtheloft.com/comedy/chris-gethard-career-suicide-transcript/" xr:uid="{9CF34735-48EA-4D73-90C2-E365CB7D864D}"/>
+    <hyperlink ref="A144" r:id="rId143" display="https://scrapsfromtheloft.com/comedy/ramy-youssef-feelings-transcript/" xr:uid="{D881A39D-B5D5-451E-BF49-D46E4CD6DF75}"/>
+    <hyperlink ref="A145" r:id="rId144" display="https://scrapsfromtheloft.com/comedy/kenny-sebastian-dont-be-that-guy-transcript/" xr:uid="{6402D41B-646C-4121-B52F-457DEB584E88}"/>
+    <hyperlink ref="A146" r:id="rId145" display="https://scrapsfromtheloft.com/comedy/billy-connolly-high-horse-tour-live-transcript/" xr:uid="{83A0F7DD-5E4D-496F-89DF-879261A2A76F}"/>
+    <hyperlink ref="A147" r:id="rId146" display="https://scrapsfromtheloft.com/comedy/hannah-gadsby-douglas-transcript/" xr:uid="{2A98E731-9133-4944-840E-496E5F5EA1B5}"/>
+    <hyperlink ref="A148" r:id="rId147" display="https://scrapsfromtheloft.com/comedy/hasan-minhaj-homecoming-king-transcript/" xr:uid="{853BBDA7-3BB3-4E00-8C5B-7515E742E665}"/>
+    <hyperlink ref="A149" r:id="rId148" display="https://scrapsfromtheloft.com/comedy/patton-oswalt-i-love-everything-transcript/" xr:uid="{B2439BB0-C739-4D83-9362-EE928DCDC194}"/>
+    <hyperlink ref="A150" r:id="rId149" display="https://scrapsfromtheloft.com/comedy/russell-peters-deported-transcript/" xr:uid="{6769E7C2-76D7-4C5C-811F-A0E8B15ADA69}"/>
+    <hyperlink ref="A151" r:id="rId150" display="https://scrapsfromtheloft.com/comedy/jimmy-o-yang-good-deal-transcript/" xr:uid="{4ABC56B4-64DD-4C7D-A2B6-C4B52021DD64}"/>
+    <hyperlink ref="A152" r:id="rId151" display="https://scrapsfromtheloft.com/comedy/jo-koy-lights-out-2012-full-transcript/" xr:uid="{0F75CFB1-80D6-4E65-9D2B-99EFA2107AAA}"/>
+    <hyperlink ref="A153" r:id="rId152" display="https://scrapsfromtheloft.com/comedy/lee-mack-going-out-live-transcript/" xr:uid="{93DA4351-9905-4F94-8183-657C2D92938E}"/>
+    <hyperlink ref="A154" r:id="rId153" display="https://scrapsfromtheloft.com/comedy/lee-mack-live-transcript/" xr:uid="{6E707677-42DA-41AE-9581-F477FC63DE1D}"/>
+    <hyperlink ref="A155" r:id="rId154" display="https://scrapsfromtheloft.com/comedy/t-j-miller-no-real-reason-transcript/" xr:uid="{B32D671A-7170-4BBB-8206-3073709D1EA3}"/>
+    <hyperlink ref="A156" r:id="rId155" display="https://scrapsfromtheloft.com/comedy/jerry-seinfeld-23-hours-to-kill-transcript/" xr:uid="{48231A52-58A3-4CD4-BDCC-1C8BDE6FAFD0}"/>
+    <hyperlink ref="A157" r:id="rId156" display="https://scrapsfromtheloft.com/comedy/bill-burr-late-show-with-david-letterman-2010/" xr:uid="{D06B706C-B279-40FF-81C3-02C7ED2FC9B1}"/>
+    <hyperlink ref="A158" r:id="rId157" display="https://scrapsfromtheloft.com/comedy/sincerely-louis-ck-transcript/" xr:uid="{24C12A27-C13E-440A-8D4B-4690AF28F35F}"/>
+    <hyperlink ref="A159" r:id="rId158" display="https://scrapsfromtheloft.com/comedy/jim-norton-american-degenerate-transcript/" xr:uid="{3A62081B-BD0B-4DDA-A7ED-F33649777CE0}"/>
+    <hyperlink ref="A160" r:id="rId159" display="https://scrapsfromtheloft.com/comedy/jim-norton-monster-rain-transcript/" xr:uid="{A14B89C2-19C9-4329-9BEF-26EF09BAAE07}"/>
+    <hyperlink ref="A161" r:id="rId160" display="https://scrapsfromtheloft.com/comedy/maria-bamford-weakness-is-the-brand-transcript/" xr:uid="{FFDD023F-D592-4A42-B0AC-C551414ACCF1}"/>
+    <hyperlink ref="A162" r:id="rId161" display="https://scrapsfromtheloft.com/comedy/dave-allen-first-day-at-school-transcript/" xr:uid="{525AFA60-60AC-4B16-B9D3-906AD7990B63}"/>
+    <hyperlink ref="A163" r:id="rId162" display="https://scrapsfromtheloft.com/comedy/chris-d-elia-white-male-black-comic-transcript/" xr:uid="{48325F99-6C3E-4992-B977-3E1503986B50}"/>
+    <hyperlink ref="A164" r:id="rId163" display="https://scrapsfromtheloft.com/comedy/chris-d-elia-man-on-fire-transcript/" xr:uid="{8D5C7C1C-1F52-4922-8E5F-599ED344139A}"/>
+    <hyperlink ref="A165" r:id="rId164" display="https://scrapsfromtheloft.com/comedy/george-carlin-indian-drill-sergeant-transcript/" xr:uid="{428637A9-12B3-47D0-9E05-C6BD2984E4C0}"/>
+    <hyperlink ref="A166" r:id="rId165" display="https://scrapsfromtheloft.com/comedy/tom-segura-ball-hog-transcript/" xr:uid="{3DF8548C-5E87-4A37-BC5A-16E3107CE840}"/>
+    <hyperlink ref="A167" r:id="rId166" display="https://scrapsfromtheloft.com/comedy/bert-kreischer-hey-big-boy-transcript/" xr:uid="{6BC8D29B-3490-40CD-9E06-B1724F2C6818}"/>
+    <hyperlink ref="A168" r:id="rId167" display="https://scrapsfromtheloft.com/comedy/bert-kreischer-fighting-a-bear-transcript/" xr:uid="{DABAFA02-E493-48C8-9CC8-3BA9582AE0D0}"/>
+    <hyperlink ref="A169" r:id="rId168" display="https://scrapsfromtheloft.com/comedy/marc-maron-end-times-fun-transcript/" xr:uid="{60E40130-2DD6-47D2-91E8-669BCC6D489A}"/>
+    <hyperlink ref="A170" r:id="rId169" display="https://scrapsfromtheloft.com/comedy/pete-davidson-smd-transcript/" xr:uid="{0E71D953-8185-40C5-B70C-6EBCCCB6FB51}"/>
+    <hyperlink ref="A171" r:id="rId170" display="https://scrapsfromtheloft.com/comedy/pete-davidson-alive-from-new-york-transcript/" xr:uid="{A6EF7B36-CA7F-4FEB-B1C1-5352C9113941}"/>
+    <hyperlink ref="A172" r:id="rId171" display="https://scrapsfromtheloft.com/comedy/amanda-seales-i-be-knowin-transcript/" xr:uid="{C2E35E00-738E-4FA1-99A3-F2BE812250E7}"/>
+    <hyperlink ref="A173" r:id="rId172" display="https://scrapsfromtheloft.com/comedy/stewart-lee-carpet-remnant-world-transcript/" xr:uid="{32143994-4CEA-416F-9AF2-E67C478EC48B}"/>
+    <hyperlink ref="A174" r:id="rId173" display="https://scrapsfromtheloft.com/comedy/stewart-lee-content-provider-transcript/" xr:uid="{ECAC06A7-7766-44B4-BE13-1BC276D79FF7}"/>
+    <hyperlink ref="A175" r:id="rId174" display="https://scrapsfromtheloft.com/comedy/sara-pascoe-ladsladslads-2019-full-transcript/" xr:uid="{9F5930FE-603D-41BB-AD15-ED29C17B22A9}"/>
+    <hyperlink ref="A176" r:id="rId175" display="https://scrapsfromtheloft.com/comedy/dan-soder-son-of-a-gary-transcript/" xr:uid="{E8FC0CEF-0EA6-4431-A525-4A10A7198501}"/>
+    <hyperlink ref="A177" r:id="rId176" display="https://scrapsfromtheloft.com/comedy/jim-gaffigan-quality-time-transcript/" xr:uid="{8371EE7A-6B57-4BC1-9980-C605E4DE5237}"/>
+    <hyperlink ref="A178" r:id="rId177" display="https://scrapsfromtheloft.com/comedy/dave-chappelle-acceptance-speech-2019-mark-twain-prize/" xr:uid="{FFC097E6-0790-4272-8817-49ABC04C1F59}"/>
+    <hyperlink ref="A179" r:id="rId178" display="https://scrapsfromtheloft.com/comedy/ricky-gervais-2020-golden-globes-monologue-transcript/" xr:uid="{A20AA465-EB98-455A-9462-1ED6F1C5AF13}"/>
+    <hyperlink ref="A180" r:id="rId179" display="https://scrapsfromtheloft.com/comedy/kevin-bridges-whole-different-story-transcript/" xr:uid="{F69CDC9E-520D-4D78-9CD8-AFFB155DA0D9}"/>
+    <hyperlink ref="A181" r:id="rId180" display="https://scrapsfromtheloft.com/comedy/kevin-bridges-story-so-far-live-glasgow-transcript/" xr:uid="{65FE2A4C-7DB8-421F-AD57-B0BD3A1D6C55}"/>
+    <hyperlink ref="A182" r:id="rId181" display="https://scrapsfromtheloft.com/comedy/kevin-bridges-the-story-continues-transcript/" xr:uid="{386A9112-D3F8-4C1D-8C4D-703CCD1A11BC}"/>
+    <hyperlink ref="A183" r:id="rId182" display="https://scrapsfromtheloft.com/comedy/andy-woodhull-youll-always-be-late-transcript/" xr:uid="{0B40AAC3-70CA-48A6-9591-272F99E0F057}"/>
+    <hyperlink ref="A184" r:id="rId183" display="https://scrapsfromtheloft.com/comedy/michelle-wolf-joke-show-transcript/" xr:uid="{CA12813D-E949-486A-A186-267FB683E3F1}"/>
+    <hyperlink ref="A185" r:id="rId184" display="https://scrapsfromtheloft.com/comedy/tiffany-haddish-black-mitzvah-transcript/" xr:uid="{669178C5-F85A-4BDE-9915-7FD09E85E865}"/>
+    <hyperlink ref="A186" r:id="rId185" display="https://scrapsfromtheloft.com/comedy/mike-birbiglia-the-new-one-transcript/" xr:uid="{D01E8F51-586D-4C80-94E8-DD207F1F851E}"/>
+    <hyperlink ref="A187" r:id="rId186" display="https://scrapsfromtheloft.com/comedy/iliza-shlesinger-unveiled-transcript/" xr:uid="{7B02D1D5-C8EC-46D8-8A3E-DA506B513204}"/>
+    <hyperlink ref="A188" r:id="rId187" display="https://scrapsfromtheloft.com/comedy/seth-meyers-lobby-baby-transcript/" xr:uid="{FDAC246E-7F9E-4D3D-8859-83840D7DC992}"/>
+    <hyperlink ref="A189" r:id="rId188" display="https://scrapsfromtheloft.com/comedy/arsenio-hall-smart-and-classy-transcript/" xr:uid="{B96D4084-124A-4A0C-BA78-EAB12E3D5BA0}"/>
+    <hyperlink ref="A190" r:id="rId189" display="https://scrapsfromtheloft.com/comedy/sebastian-maniscalco-tonight-show-starring-jimmy-fallon-transcript/" xr:uid="{32829CD6-F948-47CB-9D73-2838E402B0D2}"/>
+    <hyperlink ref="A191" r:id="rId190" display="https://scrapsfromtheloft.com/comedy/nikki-glaser-bangin-transcript/" xr:uid="{06B477EE-CD33-4E59-B806-AE6D84EE8169}"/>
+    <hyperlink ref="A192" r:id="rId191" display="https://scrapsfromtheloft.com/comedy/ryan-hamilton-stand-up-the-tonight-show-starring-jimmy-fallon-transcript/" xr:uid="{2ABE238D-E04E-4A99-8BA2-5B76306DBA42}"/>
+    <hyperlink ref="A193" r:id="rId192" display="https://scrapsfromtheloft.com/comedy/mark-normand-stand-up-tonight-show-starring-jimmy-fallon/" xr:uid="{FC723AB0-2B6E-4332-9A31-1960C9203EC7}"/>
+    <hyperlink ref="A194" r:id="rId193" display="https://scrapsfromtheloft.com/comedy/george-carlin-dumb-americans-transcript/" xr:uid="{BC20C34D-9791-41DB-A64E-E34A2AC9CE79}"/>
+    <hyperlink ref="A195" r:id="rId194" display="https://scrapsfromtheloft.com/comedy/bill-burr-paper-tiger-transcript/" xr:uid="{F31FD261-2770-4AE9-8114-48EF34A99559}"/>
+    <hyperlink ref="A196" r:id="rId195" display="https://scrapsfromtheloft.com/comedy/dave-chappelle-sticks-stones-epilogue-punchline-transcript/" xr:uid="{9587C9E8-1B85-4766-9E5B-595A53BAE814}"/>
+    <hyperlink ref="A197" r:id="rId196" display="https://scrapsfromtheloft.com/comedy/brazil-corruption-amazon-hasan-minhaj/" xr:uid="{42730A73-8E69-43AD-B0FC-45B84227C65B}"/>
+    <hyperlink ref="A198" r:id="rId197" display="https://scrapsfromtheloft.com/comedy/dave-chappelle-sticks-stones-transcript/" xr:uid="{E96C77B4-E21E-4270-8126-6210DEE0F843}"/>
+    <hyperlink ref="A199" r:id="rId198" display="https://scrapsfromtheloft.com/comedy/emily-heller-ice-thickeners-transcript/" xr:uid="{84B7CFA5-AE2C-43E2-B87E-494593BC0F00}"/>
+    <hyperlink ref="A200" r:id="rId199" display="https://scrapsfromtheloft.com/comedy/david-cross-oh-come-on-transcript/" xr:uid="{5E9F50A2-B89A-476A-94F8-8B4930879449}"/>
+    <hyperlink ref="A201" r:id="rId200" display="https://scrapsfromtheloft.com/comedy/kevin-hart-gun-compartment-transcript/" xr:uid="{63B59384-DF87-4DF6-954E-96F71B98044F}"/>
+    <hyperlink ref="A202" r:id="rId201" display="https://scrapsfromtheloft.com/comedy/whitney-cummings-can-i-touch-it-transcript/" xr:uid="{27387D58-FFE9-4BAE-B223-57DAE6F99B15}"/>
+    <hyperlink ref="A203" r:id="rId202" display="https://scrapsfromtheloft.com/comedy/eddie-griffin-bible-negro-version-transcript/" xr:uid="{6A4A76CD-0777-4ADC-A9FF-C7AF3F6496C1}"/>
+    <hyperlink ref="A204" r:id="rId203" display="https://scrapsfromtheloft.com/comedy/tom-segura-overdoses-this-is-not-happening-transcript/" xr:uid="{57F57310-AD30-4AE4-AAC3-2F99929FE243}"/>
+    <hyperlink ref="A205" r:id="rId204" display="https://scrapsfromtheloft.com/comedy/aziz-ansari-right-now-transcript/" xr:uid="{FC3D1EFC-18F9-4D8E-8577-B1A7BF87E5F3}"/>
+    <hyperlink ref="A206" r:id="rId205" display="https://scrapsfromtheloft.com/comedy/ralphie-may-filthy-animal-tour-transcript/" xr:uid="{426E5086-58EC-433A-8F66-501025AEE4CE}"/>
+    <hyperlink ref="A207" r:id="rId206" display="https://scrapsfromtheloft.com/comedy/mike-epps-only-one-mike-transcript/" xr:uid="{D84672F7-727D-4ADD-BDF8-820FAA54F96D}"/>
+    <hyperlink ref="A208" r:id="rId207" display="https://scrapsfromtheloft.com/comedy/adam-devine-best-time-of-our-lives-transcript/" xr:uid="{3D84A67A-FBFD-4B2A-948A-309D2B26AF1C}"/>
+    <hyperlink ref="A209" r:id="rId208" display="https://scrapsfromtheloft.com/comedy/jo-koy-live-from-seattle-transcript/" xr:uid="{AB071FC9-B7D1-49F5-A658-94E2FA0A274B}"/>
+    <hyperlink ref="A210" r:id="rId209" display="https://scrapsfromtheloft.com/comedy/jo-ko-comin-in-hot-transcript/" xr:uid="{F5864EAC-0F41-42CA-83C8-46064E4AD8B9}"/>
+    <hyperlink ref="A211" r:id="rId210" display="https://scrapsfromtheloft.com/comedy/the-standups-gina-yashere-2018-transcript/" xr:uid="{1BACB788-FA07-48B1-BDDE-788713F13F96}"/>
+    <hyperlink ref="A212" r:id="rId211" display="https://scrapsfromtheloft.com/comedy/wanda-sykes-not-normal-transcript/" xr:uid="{27227C81-1FAA-460A-8C05-B40B4209FABE}"/>
+    <hyperlink ref="A213" r:id="rId212" display="https://scrapsfromtheloft.com/comedy/doug-stanhope-babies-and-abortion/" xr:uid="{B1145A4A-62C5-4F54-9CC2-035B01DA816B}"/>
+    <hyperlink ref="A214" r:id="rId213" display="https://scrapsfromtheloft.com/comedy/cedric-the-entertainer-live-from-the-ville-transcript/" xr:uid="{AEBEF49F-5CB8-48C0-B204-7A72DFFC0217}"/>
+    <hyperlink ref="A215" r:id="rId214" display="https://scrapsfromtheloft.com/comedy/eddie-murphy-raw-transcript/" xr:uid="{D5BCD62D-A493-4FBA-85D6-CDAA64A62D12}"/>
+    <hyperlink ref="A216" r:id="rId215" display="https://scrapsfromtheloft.com/comedy/colin-quinn-the-new-york-story-transcript/" xr:uid="{79C2D788-C5F9-486F-AB3D-092E77D1BD69}"/>
+    <hyperlink ref="A217" r:id="rId216" display="https://scrapsfromtheloft.com/comedy/demetri-martin-live-at-the-time-transcript/" xr:uid="{A13A0B01-455B-46F5-90B7-609A01773337}"/>
+    <hyperlink ref="A218" r:id="rId217" display="https://scrapsfromtheloft.com/comedy/george-carlin-what-am-i-doing-in-new-jersey-transcript/" xr:uid="{34AA16DC-314C-4424-8515-AAC49D1418E2}"/>
+    <hyperlink ref="A219" r:id="rId218" display="https://scrapsfromtheloft.com/comedy/chelsea-peretti-one-of-the-greats-transcript/" xr:uid="{63206FEE-EBD0-4D61-A526-4D03243B0AA1}"/>
+    <hyperlink ref="A220" r:id="rId219" display="https://scrapsfromtheloft.com/comedy/anthony-jeselnik-fire-in-the-maternity-ward-transcript/" xr:uid="{E010D904-CDB7-4A28-9282-6866A1A012CD}"/>
+    <hyperlink ref="A221" r:id="rId220" display="https://scrapsfromtheloft.com/comedy/roy-wood-jr-no-one-loves-you-transcript/" xr:uid="{0673BC99-1DB8-44AF-B75A-3CB30177BF23}"/>
+    <hyperlink ref="A222" r:id="rId221" display="https://scrapsfromtheloft.com/comedy/robin-williams-weapons-of-self-destruction-transcript/" xr:uid="{2790B4EC-7544-42CC-B32A-FB805A4460B8}"/>
+    <hyperlink ref="A223" r:id="rId222" display="https://scrapsfromtheloft.com/comedy/robin-williams-live-on-broadway-2002-full-transcript/" xr:uid="{CA143D91-3D85-4995-994C-1F89AFC229D2}"/>
+    <hyperlink ref="A224" r:id="rId223" display="https://scrapsfromtheloft.com/comedy/jimmy-carr-the-best-of-ultimate-gold-greatest-hits-transcript/" xr:uid="{C6E45C70-8BC1-4ADF-881C-350C421F9EC6}"/>
+    <hyperlink ref="A225" r:id="rId224" display="https://scrapsfromtheloft.com/comedy/nate-bargatze-the-tennessee-kid-transcript/" xr:uid="{2303AF80-BE3B-4A66-8266-45FF547E7605}"/>
+    <hyperlink ref="A226" r:id="rId225" display="https://scrapsfromtheloft.com/comedy/w-kamau-bell-private-school-negro-transcript/" xr:uid="{B1D664E6-C631-4E44-8E88-8333BD10D74F}"/>
+    <hyperlink ref="A227" r:id="rId226" display="https://scrapsfromtheloft.com/comedy/kevin-hart-irresponsible-transcript/" xr:uid="{FAF7CA67-39DD-4FF2-AF5C-2DC41FA3B3DF}"/>
+    <hyperlink ref="A228" r:id="rId227" display="https://scrapsfromtheloft.com/comedy/nate-bargatze-full-time-magic-transcript/" xr:uid="{F1865610-16FF-4C38-8825-3E81AA17E28F}"/>
+    <hyperlink ref="A229" r:id="rId228" display="https://scrapsfromtheloft.com/comedy/amy-schumer-growing-transcript/" xr:uid="{10824422-A151-4B41-95F5-2F4A7BE40864}"/>
+    <hyperlink ref="A230" r:id="rId229" display="https://scrapsfromtheloft.com/comedy/ricky-gervais-2011-golden-globes-opening-monologue/" xr:uid="{226632C0-A2AD-444C-A9E6-50F40784F47E}"/>
+    <hyperlink ref="A231" r:id="rId230" display="https://scrapsfromtheloft.com/comedy/ricky-gervais-2016-golden-globes-opening-monologue/" xr:uid="{9CFC712A-D11B-46D9-B19B-E113D314747E}"/>
+    <hyperlink ref="A232" r:id="rId231" display="https://scrapsfromtheloft.com/comedy/enissa-amani-ehrenwort-2018-full-transcript/" xr:uid="{4297CB80-4999-4CB8-80F9-46443EAC890B}"/>
+    <hyperlink ref="A233" r:id="rId232" display="https://scrapsfromtheloft.com/comedy/ken-jeong-you-complete-me-ho-transcript/" xr:uid="{43A04EDA-2169-4F8E-91B9-17936FBFEA22}"/>
+    <hyperlink ref="A234" r:id="rId233" display="https://scrapsfromtheloft.com/comedy/ray-romano-right-here-around-the-corner-transcript/" xr:uid="{ACE60299-EB0B-4B9C-B22F-5D62DB6A630D}"/>
+    <hyperlink ref="A235" r:id="rId234" display="https://scrapsfromtheloft.com/comedy/gabriel-fluffy-iglesias-one-show-fits-all-transcript/" xr:uid="{54FC58CE-3E94-4E97-8D3A-A634B7F301C4}"/>
+    <hyperlink ref="A236" r:id="rId235" display="https://scrapsfromtheloft.com/comedy/sebastian-maniscalco-stay-hungry-transcript/" xr:uid="{E2148CF7-A2BF-43C3-8724-A55BDDAE46B0}"/>
+    <hyperlink ref="A237" r:id="rId236" display="https://scrapsfromtheloft.com/comedy/latin-history-for-morons-john-leguizamo-transcript/" xr:uid="{A69E4AF9-43D1-4197-BEA6-4A0D7563A557}"/>
+    <hyperlink ref="A238" r:id="rId237" display="https://scrapsfromtheloft.com/comedy/sebastian-maniscalco-arent-you-embarrassed-transcript/" xr:uid="{8A8DD5E8-B4B3-48CC-927D-51986E41212A}"/>
+    <hyperlink ref="A239" r:id="rId238" display="https://scrapsfromtheloft.com/comedy/sebastian-maniscalco-whats-wrong-with-people-transcript/" xr:uid="{211FEBB0-AC42-4859-8F78-60FEF7FAF4EB}"/>
+    <hyperlink ref="A240" r:id="rId239" display="https://scrapsfromtheloft.com/comedy/oh-hello-on-broadway-transcript/" xr:uid="{E2E30995-FA6F-4665-BE81-9EF0C6B14326}"/>
+    <hyperlink ref="A241" r:id="rId240" display="https://scrapsfromtheloft.com/comedy/ellen-degeneres-relatable-transcript/" xr:uid="{2CA97D97-35B7-4837-BE20-BBBD4C21D463}"/>
+    <hyperlink ref="A242" r:id="rId241" display="https://scrapsfromtheloft.com/comedy/pete-holmes-dirty-clean-transcript/" xr:uid="{21E9B9E3-10E6-4E6D-84C1-B5A96D3B76D0}"/>
+    <hyperlink ref="A243" r:id="rId242" display="https://scrapsfromtheloft.com/comedy/vir-das-losing-it-transcript/" xr:uid="{339B00D9-82B3-4EE9-98E4-521AAF275D4A}"/>
+    <hyperlink ref="A244" r:id="rId243" display="https://scrapsfromtheloft.com/comedy/volker-pispers-about-usa-2004-transcript/" xr:uid="{9117F30F-0DC9-4095-B63A-214A112EB80A}"/>
+    <hyperlink ref="A245" r:id="rId244" display="https://scrapsfromtheloft.com/comedy/trevor-noah-son-of-patricia-transcript/" xr:uid="{47C2271A-DF16-46F3-8F2A-CCCBA3FCCBE5}"/>
+    <hyperlink ref="A246" r:id="rId245" display="https://scrapsfromtheloft.com/comedy/jeff-foxworthy-larry-the-cable-guy-weve-been-thinking-transcript/" xr:uid="{9FB458B3-A488-4B6A-9C5E-EE0AC6189A5C}"/>
+    <hyperlink ref="A247" r:id="rId246" display="https://scrapsfromtheloft.com/comedy/adam-sandler-100-fresh-transcript/" xr:uid="{C95AE3F6-49BE-4978-B286-EA8BB44A1445}"/>
+    <hyperlink ref="A248" r:id="rId247" display="https://scrapsfromtheloft.com/comedy/jeff-foxworthy-totally-committed-transcript/" xr:uid="{48DB69AE-831D-4337-BB08-CD92563F5D03}"/>
+    <hyperlink ref="A249" r:id="rId248" display="https://scrapsfromtheloft.com/comedy/ron-white-if-you-quit-listening-ill-shutup-transcript/" xr:uid="{597AEA37-E878-4B8C-BE73-C028EFA61242}"/>
+    <hyperlink ref="A250" r:id="rId249" display="https://scrapsfromtheloft.com/comedy/carlin-at-carnegie-transcript/" xr:uid="{78B51715-B2FA-46BB-8DC7-E59115D57905}"/>
+    <hyperlink ref="A251" r:id="rId250" display="https://scrapsfromtheloft.com/comedy/comedy-central-presents-tom-segura-s15e01-transcript/" xr:uid="{3D354D13-C56D-4517-B827-9C71C0282184}"/>
+    <hyperlink ref="A252" r:id="rId251" display="https://scrapsfromtheloft.com/comedy/mo-amer-the-vagabond-transcript/" xr:uid="{2BD833F7-C400-4801-B94E-0A3D98145D34}"/>
+    <hyperlink ref="A253" r:id="rId252" display="https://scrapsfromtheloft.com/comedy/joe-mandes-award-winning-comedy-special-transcript/" xr:uid="{895BC373-F9B5-4D5B-B664-1D3DD6C3BE96}"/>
+    <hyperlink ref="A254" r:id="rId253" display="https://scrapsfromtheloft.com/comedy/henry-rollins-keep-talking-pal-transcript/" xr:uid="{BB3D6EED-8405-4795-956A-F4B208D7853A}"/>
+    <hyperlink ref="A255" r:id="rId254" display="https://scrapsfromtheloft.com/comedy/george-carlin-saturday-night-live-monologue1975-s01e01/" xr:uid="{EB500B4D-8FDC-4DA4-85E9-4153AEA33B03}"/>
+    <hyperlink ref="A256" r:id="rId255" display="https://scrapsfromtheloft.com/comedy/joe-rogan-strange-times-transcript/" xr:uid="{99621B67-D273-40C3-84E5-A9245AC1798A}"/>
+    <hyperlink ref="A257" r:id="rId256" display="https://scrapsfromtheloft.com/comedy/louis-ck-snl-monologue-s38e06-2012-transcript/" xr:uid="{476D347E-E860-423E-8D17-173F311370D2}"/>
+    <hyperlink ref="A258" r:id="rId257" display="https://scrapsfromtheloft.com/comedy/louis-c-k-snl-monologue-march-29-2014-full-transcript/" xr:uid="{ABE33F0E-67B0-42AE-8BE7-281F12985544}"/>
+    <hyperlink ref="A259" r:id="rId258" display="https://scrapsfromtheloft.com/comedy/sarah-silvermans-monologue-saturday-night-live-2014-transcript/" xr:uid="{77825692-807E-464B-82AD-4D0732B2F304}"/>
+    <hyperlink ref="A260" r:id="rId259" display="https://scrapsfromtheloft.com/comedy/louis-c-k-snl-monologue-2015-transcript/" xr:uid="{CAD2B358-1A2D-47EA-B9DD-EE584A7ECF66}"/>
+    <hyperlink ref="A261" r:id="rId260" display="https://scrapsfromtheloft.com/comedy/john-mulaney-snl-monologue-2018-transcript/" xr:uid="{4943C0D0-9651-4679-83DD-610D8E261A90}"/>
+    <hyperlink ref="A262" r:id="rId261" display="https://scrapsfromtheloft.com/comedy/david-chappelles-snl-monologue-2016-transcript/" xr:uid="{292497D1-C8EF-43BF-9B0A-42F006CDD67F}"/>
+    <hyperlink ref="A263" r:id="rId262" display="https://scrapsfromtheloft.com/comedy/d-l-hughley-contrarian-transcript/" xr:uid="{47488665-E446-4F0B-9333-93029992429E}"/>
+    <hyperlink ref="A264" r:id="rId263" display="https://scrapsfromtheloft.com/comedy/iliza-shlesinger-freezing-hot-transcript/" xr:uid="{31D9CF2B-827D-41EF-A342-A3C61724E59F}"/>
+    <hyperlink ref="A265" r:id="rId264" display="https://scrapsfromtheloft.com/comedy/iliza-shlesinger-war-paint-transcript/" xr:uid="{E98F38BC-7D70-4A11-860E-665EABB01DE0}"/>
+    <hyperlink ref="A266" r:id="rId265" display="https://scrapsfromtheloft.com/comedy/bert-kreischer-secret-time-transcript/" xr:uid="{760D9FF4-DC5E-475C-8B6C-65B53BA5E670}"/>
+    <hyperlink ref="A267" r:id="rId266" display="https://scrapsfromtheloft.com/comedy/dick-gregory-speech-st-johns-baptist-church-may-20-1963/" xr:uid="{0E70A489-CA2C-45B6-9FAE-0F3DE552C425}"/>
+    <hyperlink ref="A268" r:id="rId267" display="https://scrapsfromtheloft.com/comedy/demetri-martin-overthinker-transcript/" xr:uid="{DF1B4884-EB2E-4935-B154-6D71D4DBF99F}"/>
+    <hyperlink ref="A269" r:id="rId268" display="https://scrapsfromtheloft.com/comedy/bill-maher-live-from-oklahoma-2018-full-transcript/" xr:uid="{AFA939A5-26EF-4AD3-825F-12445DB20EE4}"/>
+    <hyperlink ref="A270" r:id="rId269" display="https://scrapsfromtheloft.com/comedy/rowan-atkinson-live-1992-transcript/" xr:uid="{4924B6CD-7377-46EF-A4A6-26F450D2CB10}"/>
+    <hyperlink ref="A271" r:id="rId270" display="https://scrapsfromtheloft.com/comedy/iliza-shlesinger-confirmed-kills-transcript/" xr:uid="{40236CFB-E00E-4266-AA15-CDDBFBDD63B9}"/>
+    <hyperlink ref="A272" r:id="rId271" display="https://scrapsfromtheloft.com/comedy/iliza-shlesinger-elder-millennial-2018-full-transcript/" xr:uid="{3C2F2AB5-8935-42AB-B33E-2D982E4B5B37}"/>
+    <hyperlink ref="A273" r:id="rId272" display="https://scrapsfromtheloft.com/comedy/jim-gaffigan-noble-ape-full-transcript/" xr:uid="{05266F29-6721-4909-912C-5A0EBCAAAFD6}"/>
+    <hyperlink ref="A274" r:id="rId273" display="https://scrapsfromtheloft.com/comedy/jim-norton-contextually-inadequate-full-transcript/" xr:uid="{090AC489-A932-4F8D-9C04-AD0D2C808BD9}"/>
+    <hyperlink ref="A275" r:id="rId274" display="https://scrapsfromtheloft.com/comedy/hannah-gadsby-nanette-transcript/" xr:uid="{7CF8ECCD-62DC-4134-8EF1-811B83073365}"/>
+    <hyperlink ref="A276" r:id="rId275" display="https://scrapsfromtheloft.com/comedy/brad-williams-daddy-issues-transcript/" xr:uid="{0A70C933-C92A-420E-B28B-02C90EBA660E}"/>
+    <hyperlink ref="A277" r:id="rId276" display="https://scrapsfromtheloft.com/comedy/deray-davis-how-to-act-black-transcript/" xr:uid="{0BA44745-4B42-4312-AE4C-8100547A4245}"/>
+    <hyperlink ref="A278" r:id="rId277" display="https://scrapsfromtheloft.com/comedy/ricky-gervais-live-iv-science-transcript/" xr:uid="{FDE2B252-1119-437E-80BC-8194BCEB841B}"/>
+    <hyperlink ref="A279" r:id="rId278" display="https://scrapsfromtheloft.com/comedy/jim-jefferies-this-is-me-now-transcript/" xr:uid="{2A5F4BEE-4CC7-4CCE-8592-844931E30759}"/>
+    <hyperlink ref="A280" r:id="rId279" display="https://scrapsfromtheloft.com/comedy/louis-c-k-chewed-up-transcript/" xr:uid="{D6E0180B-B898-4B06-BE4B-BDCBFB8C5F08}"/>
+    <hyperlink ref="A281" r:id="rId280" display="https://scrapsfromtheloft.com/comedy/bill-burr-the-philadelphia-incident-2006-transcript/" xr:uid="{DD662BF0-A782-4222-8C19-A2D52C8C6875}"/>
+    <hyperlink ref="A282" r:id="rId281" display="https://scrapsfromtheloft.com/comedy/russell-peters-outsourced-transcript/" xr:uid="{C4961752-EBBF-4FC8-A91F-DE472B532001}"/>
+    <hyperlink ref="A283" r:id="rId282" display="https://scrapsfromtheloft.com/comedy/russell-peters-almost-famous-2016-full-transcript/" xr:uid="{F6CE82C2-A3DD-428D-A7B5-D4473023CBF4}"/>
+    <hyperlink ref="A284" r:id="rId283" display="https://scrapsfromtheloft.com/comedy/ron-white-a-little-unprofessional-transcript/" xr:uid="{B46CFEAC-040B-4D79-B6CF-BA6996F96121}"/>
+    <hyperlink ref="A285" r:id="rId284" display="https://scrapsfromtheloft.com/comedy/michael-mcintyre-hello-wembley-transcript/" xr:uid="{B322ADAD-DEF5-43E4-A93A-D3F58F5E310F}"/>
+    <hyperlink ref="A286" r:id="rId285" display="https://scrapsfromtheloft.com/comedy/kevin-smith-silent-but-deadly-transcript/" xr:uid="{3B0992C5-0459-4209-A125-98056290AD31}"/>
+    <hyperlink ref="A287" r:id="rId286" display="https://scrapsfromtheloft.com/comedy/kevin-james-never-dont-give-up-full-transcript/" xr:uid="{EFCDA39C-7770-4080-82E5-1F5E0C9F9443}"/>
+    <hyperlink ref="A288" r:id="rId287" display="https://scrapsfromtheloft.com/comedy/trevor-noah-royal-wedding-2018/" xr:uid="{EC9866D0-6A33-416D-AC69-2DF5A851C015}"/>
+    <hyperlink ref="A289" r:id="rId288" display="https://scrapsfromtheloft.com/comedy/brent-morin-im-brent-morin-2015-full-transcript/" xr:uid="{7EB78E10-DC27-4707-AF18-CC3C0E8AD169}"/>
+    <hyperlink ref="A290" r:id="rId289" display="https://scrapsfromtheloft.com/comedy/nikki-glaser-perfect-2016-full-transcript/" xr:uid="{C539AB73-4C65-4970-AA45-52FAF851DD2A}"/>
+    <hyperlink ref="A291" r:id="rId290" display="https://scrapsfromtheloft.com/comedy/doug-stanhope-on-nationalism/" xr:uid="{F71E6699-A49B-42E7-B408-3C3653276008}"/>
+    <hyperlink ref="A292" r:id="rId291" display="https://scrapsfromtheloft.com/comedy/ali-wong-hard-knock-wife-transcript/" xr:uid="{50634716-CAFF-4807-A6D0-EF245604B58D}"/>
+    <hyperlink ref="A293" r:id="rId292" display="https://scrapsfromtheloft.com/comedy/kavin-jay-everybody-calm-down-full-transcript/" xr:uid="{2C25A5FA-58C1-4651-814F-0159D2F64E4D}"/>
+    <hyperlink ref="A294" r:id="rId293" display="https://scrapsfromtheloft.com/comedy/john-mulaney-kid-gorgeous-at-radio-city-full-transcript/" xr:uid="{5382F369-01E1-4321-B1A4-F88303F47DEC}"/>
+    <hyperlink ref="A295" r:id="rId294" display="https://scrapsfromtheloft.com/comedy/eddie-griffin-undeniable-2018-full-transcript/" xr:uid="{DED80B03-C04A-4C09-AAA0-323928B641FB}"/>
+    <hyperlink ref="A296" r:id="rId295" display="https://scrapsfromtheloft.com/comedy/greg-davies-you-magnificent-beast-full-transcript/" xr:uid="{EDB7394E-FDFC-4BBD-8604-E0E295F2C157}"/>
+    <hyperlink ref="A297" r:id="rId296" display="https://scrapsfromtheloft.com/comedy/comedy-central-patton-oswalt-1999-full-transcript/" xr:uid="{44E93FDA-F210-4D6C-B5A3-C147671A11EA}"/>
+    <hyperlink ref="A298" r:id="rId297" display="https://scrapsfromtheloft.com/comedy/george-carlin-you-are-all-diseased-transcript/" xr:uid="{E353F09A-7803-4746-B3FF-E52D97711899}"/>
+    <hyperlink ref="A299" r:id="rId298" display="https://scrapsfromtheloft.com/comedy/ricky-gervais-2012-golden-globes-opening-monologue/" xr:uid="{4895119E-D2C7-49E7-8AD6-EB8628111A92}"/>
+    <hyperlink ref="A300" r:id="rId299" display="https://scrapsfromtheloft.com/comedy/marlon-wayans-wokeish-transcript/" xr:uid="{A409FB5A-6E2F-40DF-988A-EAC8A61AE25C}"/>
+    <hyperlink ref="A301" r:id="rId300" display="https://scrapsfromtheloft.com/comedy/ricky-gervais-humanity-transcript/" xr:uid="{BCEF0668-5422-43AE-9A93-DFBA261BB4BA}"/>
+    <hyperlink ref="A302" r:id="rId301" display="https://scrapsfromtheloft.com/comedy/adel-karam-live-from-beirut-transcript/" xr:uid="{33C407C0-D8CF-41A6-A5BD-425F15E25416}"/>
+    <hyperlink ref="A303" r:id="rId302" display="https://scrapsfromtheloft.com/comedy/stewart-lee-90s-comedian-2006-full-transcript/" xr:uid="{5F52CD72-8715-4897-A842-C813A3867A45}"/>
+    <hyperlink ref="A304" r:id="rId303" display="https://scrapsfromtheloft.com/comedy/mike-birbiglia-my-girlfriends-boyfriend-2013-full-transcript/" xr:uid="{039A4450-5DC2-4887-BD39-6C1E4D02BED1}"/>
+    <hyperlink ref="A305" r:id="rId304" display="https://scrapsfromtheloft.com/comedy/dave-attell-road-work-transcript/" xr:uid="{6FFA399A-4F3F-4519-91A6-DC7B5409CAB9}"/>
+    <hyperlink ref="A306" r:id="rId305" display="https://scrapsfromtheloft.com/comedy/eddie-izzard-glorious-1997-full-transcript/" xr:uid="{EB503DCF-7F44-4657-A3D5-A6BFE1B27BE5}"/>
+    <hyperlink ref="A307" r:id="rId306" display="https://scrapsfromtheloft.com/comedy/chris-rock-bring-pain-transcript/" xr:uid="{04FA5472-9842-4A8C-9395-EBA7557AF5A7}"/>
+    <hyperlink ref="A308" r:id="rId307" display="https://scrapsfromtheloft.com/comedy/ari-shaffir-double-negative-transcript/" xr:uid="{E44A4536-F7E6-4D67-A0B7-5014631D5DAA}"/>
+    <hyperlink ref="A309" r:id="rId308" display="https://scrapsfromtheloft.com/comedy/chris-rock-tamborine-transcript/" xr:uid="{4E1468C8-B1C2-4046-9087-0C3260215C8B}"/>
+    <hyperlink ref="A310" r:id="rId309" display="https://scrapsfromtheloft.com/comedy/fred-armisen-standup-for-drummers-transcript/" xr:uid="{F92AD68E-6761-46C0-B513-A9DB1333CBB4}"/>
+    <hyperlink ref="A311" r:id="rId310" display="https://scrapsfromtheloft.com/comedy/dana-carvey-straight-white-male-60-2016-full-transcript/" xr:uid="{F8DD9088-A4E9-49B8-B7B8-1A95A995C716}"/>
+    <hyperlink ref="A312" r:id="rId311" display="https://scrapsfromtheloft.com/comedy/eddie-izzard-stripped-2009-full-transcript/" xr:uid="{B4973F13-68C0-4827-A30C-CC2C6C9773F8}"/>
+    <hyperlink ref="A313" r:id="rId312" display="https://scrapsfromtheloft.com/comedy/todd-glass-act-happy-transcript/" xr:uid="{E48EEA56-DC1F-4F7C-81E9-03CE4BCFB06F}"/>
+    <hyperlink ref="A314" r:id="rId313" display="https://scrapsfromtheloft.com/comedy/brian-regan-standing-up-2007-full-transcript/" xr:uid="{445F7E24-1C62-4552-A3A5-A5A63F96FB09}"/>
+    <hyperlink ref="A315" r:id="rId314" display="https://scrapsfromtheloft.com/comedy/brian-regan-nunchucks-flamethrowers-transcript/" xr:uid="{6DFF6FB9-B9D1-482F-B969-2816D7854F0C}"/>
+    <hyperlink ref="A316" r:id="rId315" display="https://scrapsfromtheloft.com/comedy/katt-williams-great-america-transcript/" xr:uid="{5EAA7AB5-7411-41D5-A6EC-59517CC236A2}"/>
+    <hyperlink ref="A317" r:id="rId316" display="https://scrapsfromtheloft.com/comedy/jimmy-carr-being-funny-transcript/" xr:uid="{9D61D4FA-3C71-4296-ABC4-5A7C0F3AA22C}"/>
+    <hyperlink ref="A318" r:id="rId317" display="https://scrapsfromtheloft.com/comedy/jimmy-carr-laughing-and-joking-transcript/" xr:uid="{44699F87-6EA3-47C0-A0A3-A74490572BEC}"/>
+    <hyperlink ref="A319" r:id="rId318" display="https://scrapsfromtheloft.com/comedy/eddie-izzard-unrepeatable-transcript/" xr:uid="{E2CE7857-B8A5-495A-8524-E8F78A747742}"/>
+    <hyperlink ref="A320" r:id="rId319" display="https://scrapsfromtheloft.com/comedy/d-l-hughley-unapologetic-transcript/" xr:uid="{852FCB34-503A-4FBC-B222-3D407409F1F6}"/>
+    <hyperlink ref="A321" r:id="rId320" display="https://scrapsfromtheloft.com/comedy/bridget-everett-gynecological-wonder-2015-full-transcript/" xr:uid="{E3C95DB7-0234-443B-B4C0-2ED6D60EF665}"/>
+    <hyperlink ref="A322" r:id="rId321" display="https://scrapsfromtheloft.com/comedy/chris-rock-never-scared-2004-full-transcript/" xr:uid="{7F57ED07-253C-4E62-89B7-91945C9A35C5}"/>
+    <hyperlink ref="A323" r:id="rId322" display="https://scrapsfromtheloft.com/comedy/stewart-lee-standup-comedian-full-transcript/" xr:uid="{7CA413D9-4C43-48DE-8F82-0B6DB0D09046}"/>
+    <hyperlink ref="A324" r:id="rId323" display="https://scrapsfromtheloft.com/comedy/jimmy-carr-funny-business-transcript/" xr:uid="{F44FDC33-B12C-49B3-A302-53B5B9962FCB}"/>
+    <hyperlink ref="A325" r:id="rId324" display="https://scrapsfromtheloft.com/comedy/eddie-izzard-dress-kill-1999-full-transcript/" xr:uid="{1799C577-6E0D-435D-BA4E-C63D1E6B6AA2}"/>
+    <hyperlink ref="A326" r:id="rId325" display="https://scrapsfromtheloft.com/comedy/chris-tucker-live-2015-transcript/" xr:uid="{9705962C-C745-4E70-B0F9-D2410C38E9F6}"/>
+    <hyperlink ref="A327" r:id="rId326" display="https://scrapsfromtheloft.com/comedy/kevin-hart-what-now-2016-full-transcript/" xr:uid="{49C8E8BB-DE88-4816-8F5B-80A77A144FBE}"/>
+    <hyperlink ref="A328" r:id="rId327" display="https://scrapsfromtheloft.com/comedy/kevin-hart-let-me-explain-2013-full-transcript/" xr:uid="{6728A3F2-B8B8-49F3-993E-F2299EEDBE63}"/>
+    <hyperlink ref="A329" r:id="rId328" display="https://scrapsfromtheloft.com/comedy/tom-segura-disgraceful-2018-full-transcript/" xr:uid="{74925C1E-CBBF-4156-A164-E94FDC816691}"/>
+    <hyperlink ref="A330" r:id="rId329" display="https://scrapsfromtheloft.com/comedy/bill-hicks-live-at-laff-stop-austin-tx-and-cobbs-san-francisco-ca-1993/" xr:uid="{443BC8E2-9C89-4D61-B3CD-A6B0775DA12D}"/>
+    <hyperlink ref="A331" r:id="rId330" display="https://scrapsfromtheloft.com/comedy/michelle-wolf-nice-lady-2017-full-transcript/" xr:uid="{A9FB563A-28C2-4D2E-B9E6-6882B8A29D1D}"/>
+    <hyperlink ref="A332" r:id="rId331" display="https://scrapsfromtheloft.com/comedy/fahim-anwar-theres-no-business-like-show-business-2017-full-transcript/" xr:uid="{A4ACF17A-5799-4EA1-A5D6-5832DA2F082E}"/>
+    <hyperlink ref="A333" r:id="rId332" display="https://scrapsfromtheloft.com/comedy/ellen-degeneres-the-beginning-2000-full-transcript/" xr:uid="{819B94A7-1FF7-4C5F-B6F0-95F93DA602E7}"/>
+    <hyperlink ref="A334" r:id="rId333" display="https://scrapsfromtheloft.com/comedy/maz-jobrani-immigrant-2017-full-transcript/" xr:uid="{8E98AB6A-FF2A-455B-9E09-E5D0B448C76B}"/>
+    <hyperlink ref="A335" r:id="rId334" display="https://scrapsfromtheloft.com/comedy/todd-barry-spicy-honey-2017-full-transcript/" xr:uid="{96D3BAD4-CC6B-49EE-8743-96E175CDA1EA}"/>
+    <hyperlink ref="A336" r:id="rId335" display="https://scrapsfromtheloft.com/comedy/jerry-seinfeld-im-telling-you-for-the-last-time-full-transcript/" xr:uid="{BB009DA9-6BF7-4B66-A4B4-8A4FAF0A5ECD}"/>
+    <hyperlink ref="A337" r:id="rId336" display="https://scrapsfromtheloft.com/comedy/craig-ferguson-does-this-need-to-be-said-transcript/" xr:uid="{F2967F33-EA75-40B6-80D3-EED06F1D425B}"/>
+    <hyperlink ref="A338" r:id="rId337" display="https://scrapsfromtheloft.com/comedy/craig-ferguson-tickle-fight-2017-full-transcript/" xr:uid="{CA84D59A-2710-4FA8-8E60-A2E4F63541CD}"/>
+    <hyperlink ref="A339" r:id="rId338" display="https://scrapsfromtheloft.com/comedy/dylan-moran-like-totally-2006-full-transcript/" xr:uid="{8FCBDBC8-486B-435D-B75C-034A2B5B6D5C}"/>
+    <hyperlink ref="A340" r:id="rId339" display="https://scrapsfromtheloft.com/comedy/dave-chappelle-equanimity-2017-transcripcion-completa/" xr:uid="{E193FFC3-EFA4-46EC-9DAC-3917BE9609B5}"/>
+    <hyperlink ref="A341" r:id="rId340" display="https://scrapsfromtheloft.com/movies/dave-chappelle-bird-revelation-2017-transcripcion-completa/" xr:uid="{B53DE219-FAF7-4650-BAAB-8BA6BA784286}"/>
+    <hyperlink ref="A342" r:id="rId341" display="https://scrapsfromtheloft.com/comedy/dave-chappelle-hbo-half-hour-1998-traduzione-italiana/" xr:uid="{7BFD5986-5B8F-4FB7-B94F-D7A69F59AE68}"/>
+    <hyperlink ref="A343" r:id="rId342" display="https://scrapsfromtheloft.com/comedy/trevor-noah-live-at-the-apollo-2013-transcript/" xr:uid="{9E4D7F9D-B5EE-4AD8-BA75-6F3D99EA4D4E}"/>
+    <hyperlink ref="A344" r:id="rId343" display="https://scrapsfromtheloft.com/comedy/dave-chappelle-the-bird-revelation-2017-full-transcript/" xr:uid="{7A303C16-63D7-4DF7-A76D-C28201CF51AB}"/>
+    <hyperlink ref="A345" r:id="rId344" display="https://scrapsfromtheloft.com/comedy/dave-chappelle-equanimity-2017-full-transcript/" xr:uid="{0A4B1C2A-07EA-4255-BBAB-344E42399331}"/>
+    <hyperlink ref="A346" r:id="rId345" display="https://scrapsfromtheloft.com/comedy/craig-ferguson-im-here-to-help-2013-full-transcript/" xr:uid="{4B6BC776-7D59-4759-A34E-23E321A7BA72}"/>
+    <hyperlink ref="A347" r:id="rId346" display="https://scrapsfromtheloft.com/comedy/russell-howard-recalibrate-2017-full-transcript/" xr:uid="{A204CCF8-7621-44D1-81E9-AB2E62AB5B78}"/>
+    <hyperlink ref="A348" r:id="rId347" display="https://scrapsfromtheloft.com/comedy/whitney-cummings-i-love-2014-full-transcript/" xr:uid="{32FC1A51-50E4-469D-82E2-B20564D74BE6}"/>
+    <hyperlink ref="A349" r:id="rId348" display="https://scrapsfromtheloft.com/comedy/whitney-cummings-im-your-girlfriend-2016-full-transcript/" xr:uid="{588B7D7A-46E1-48D6-BB6B-D20D8A4A31A3}"/>
+    <hyperlink ref="A350" r:id="rId349" display="https://scrapsfromtheloft.com/comedy/sarah-millican-chatterbox-live-2011-full-transcript/" xr:uid="{2FA33E0A-9162-4B62-9A46-1CE945E05600}"/>
+    <hyperlink ref="A351" r:id="rId350" display="https://scrapsfromtheloft.com/comedy/anjelah-johnson-not-fancy-transcript/" xr:uid="{C2E4C99E-E2B5-40E8-955B-69D5D1AA16EF}"/>
+    <hyperlink ref="A352" r:id="rId351" display="https://scrapsfromtheloft.com/movies/ricky-gervais-live-2-politics-2004-full-transcript/" xr:uid="{E86CEAF3-EA16-44A4-AE3B-73F4DF51D74C}"/>
+    <hyperlink ref="A353" r:id="rId352" display="https://scrapsfromtheloft.com/comedy/russell-howard-live-dingledodies-2009-full-transcript/" xr:uid="{AF150ED4-9E6C-4591-9D1F-19577869FB61}"/>
+    <hyperlink ref="A354" r:id="rId353" display="https://scrapsfromtheloft.com/comedy/christina-pazsitzky-mother-inferior-transcript/" xr:uid="{EBB4B9EF-6638-49F0-B589-D8A2678A4E16}"/>
+    <hyperlink ref="A355" r:id="rId354" display="https://scrapsfromtheloft.com/comedy/jack-whitehall-at-large-2017-full-transcript/" xr:uid="{B903D090-9F8B-4A66-A822-F08B716EE1AF}"/>
+    <hyperlink ref="A356" r:id="rId355" display="https://scrapsfromtheloft.com/comedy/cristela-alonzo-lower-classy-2017-full-transcript/" xr:uid="{8AE8B85C-088E-4F3D-BCC0-846130A89619}"/>
+    <hyperlink ref="A357" r:id="rId356" display="https://scrapsfromtheloft.com/comedy/judah-friedlander-america-is-the-greatest-country-in-the-united-states-2017-full-transcript/" xr:uid="{A64F1431-9A3C-47E1-AC8A-52CA8105B29F}"/>
+    <hyperlink ref="A358" r:id="rId357" display="https://scrapsfromtheloft.com/comedy/aziz-ansari-live-in-madison-square-garden-2015-full-transcript/" xr:uid="{13EA3EAF-8146-4FC0-BA25-79D1D288FB1D}"/>
+    <hyperlink ref="A359" r:id="rId358" display="https://scrapsfromtheloft.com/comedy/aziz-ansari-buried-alive-2013-full-transcript/" xr:uid="{5ADD9A1B-66C1-4E1D-BF19-F0111011B8B4}"/>
+    <hyperlink ref="A360" r:id="rId359" display="https://scrapsfromtheloft.com/comedy/paul-mooney-piece-mind-godbless-america-transcript/" xr:uid="{FCBA18B6-B74B-43F6-826B-5D1D2C3B461B}"/>
+    <hyperlink ref="A361" r:id="rId360" display="https://scrapsfromtheloft.com/comedy/patton-oswalt-annihilation-2017-full-transcript/" xr:uid="{F0F8A7DF-51CA-4CC2-8DBB-904427AD7BCF}"/>
+    <hyperlink ref="A362" r:id="rId361" display="https://scrapsfromtheloft.com/comedy/chris-rock-kill-the-messenger-london-new-york-johannesburg-2008-movie-script/" xr:uid="{1512E18E-E3F2-4494-9D5F-F249EDCC48A7}"/>
+    <hyperlink ref="A363" r:id="rId362" display="https://scrapsfromtheloft.com/comedy/bill-maher-live-from-d-c-2014-full-transcript/" xr:uid="{1B63FFE6-1076-4213-8BAE-1C6AEAAA70F5}"/>
+    <hyperlink ref="A364" r:id="rId363" display="https://scrapsfromtheloft.com/comedy/sarah-silverman-jesus-is-magic-2005-full-transcript/" xr:uid="{667D881A-9599-4DAF-AFFB-12488F647DD6}"/>
+    <hyperlink ref="A365" r:id="rId364" display="https://scrapsfromtheloft.com/comedy/sarah-silverman-we-are-miracles-2013-full-transcript/" xr:uid="{3FB07B42-06E3-4DF7-A709-32B301F25FAA}"/>
+    <hyperlink ref="A366" r:id="rId365" display="https://scrapsfromtheloft.com/comedy/pablo-francisco-ouch-live-san-jose-2006-full-transcript/" xr:uid="{FAD1DE1E-01DE-4098-8DC9-5AC5A47EC6CE}"/>
+    <hyperlink ref="A367" r:id="rId366" display="https://scrapsfromtheloft.com/comedy/bill-maher-but-im-not-wrong-2010-full-transcript/" xr:uid="{660221F3-B6AF-45D2-B6F9-4C7D588AF1F7}"/>
+    <hyperlink ref="A368" r:id="rId367" display="https://scrapsfromtheloft.com/comedy/russell-brand-messiah-complex-2013-full-transcript/" xr:uid="{5D100F7A-59EA-4557-A367-457F7CEADC2B}"/>
+    <hyperlink ref="A369" r:id="rId368" display="https://scrapsfromtheloft.com/comedy/chris-rock-bigger-blacker-1999-full-transcript/" xr:uid="{2FF8BD4A-BAA3-41B0-BAE5-3029842FC524}"/>
+    <hyperlink ref="A370" r:id="rId369" display="https://scrapsfromtheloft.com/comedy/gabriel-iglesias-hot-and-fluffy-2007-full-transcript/" xr:uid="{99828007-4F7B-45E4-B824-DF14943599F4}"/>
+    <hyperlink ref="A371" r:id="rId370" display="https://scrapsfromtheloft.com/comedy/gabriel-iglesias-im-not-fat-im-fluffy-2009-full-transcript/" xr:uid="{0C9CAD15-5D28-4D87-8E1A-AEEF4FE6594E}"/>
+    <hyperlink ref="A372" r:id="rId371" display="https://scrapsfromtheloft.com/comedy/gabriel-iglesias-im-sorry-for-what-i-said-when-i-was-hungry-2016-full-transcript/" xr:uid="{9A7C450A-C6A9-445A-8831-3CDACD0470E7}"/>
+    <hyperlink ref="A373" r:id="rId372" display="https://scrapsfromtheloft.com/comedy/george-carlin-pro-life-abortion-and-the-sanctity-of-life/" xr:uid="{C74D6FD4-6C91-4055-8A7C-D083C8482E8D}"/>
+    <hyperlink ref="A374" r:id="rId373" display="https://scrapsfromtheloft.com/comedy/richard-pryors-monologue-saturday-night-live-1975/" xr:uid="{685C2801-0B0D-4229-BBB6-EFB4EA6F6FDE}"/>
+    <hyperlink ref="A375" r:id="rId374" display="https://scrapsfromtheloft.com/comedy/rory-scovel-tries-stand-up-for-the-first-time-a-netflix-special/" xr:uid="{5C66D822-3C40-4D70-BD9A-4FD7726237AA}"/>
+    <hyperlink ref="A376" r:id="rId375" display="https://scrapsfromtheloft.com/comedy/lisa-lampanelli-back-to-the-drawing-board-2015-full-transcript/" xr:uid="{45EB51D5-18D8-4B61-8F0A-C08E994A6B8E}"/>
+    <hyperlink ref="A377" r:id="rId376" display="https://scrapsfromtheloft.com/comedy/comedy-central-presents-dave-attell-1999-full-transcript/" xr:uid="{860A8A5D-8759-403D-A380-9290D1408EF7}"/>
+    <hyperlink ref="A378" r:id="rId377" display="https://scrapsfromtheloft.com/comedy/erik-griffin-the-ugly-truth-2017-full-transcript/" xr:uid="{EABD20C5-FFB1-4E3C-8E2D-0F296F6D5B88}"/>
+    <hyperlink ref="A379" r:id="rId378" display="https://scrapsfromtheloft.com/comedy/chris-rocks-monologue-saturday-night-live-1996/" xr:uid="{F5AE0BA1-F91A-4455-B2B8-DFAFA18CCBB1}"/>
+    <hyperlink ref="A380" r:id="rId379" display="https://scrapsfromtheloft.com/comedy/jen-kirkman-just-keep-livin-2017-full-transcript/" xr:uid="{3C7A03EC-E626-482B-9D9B-2DA81E2E8F4D}"/>
+    <hyperlink ref="A381" r:id="rId380" display="https://scrapsfromtheloft.com/comedy/comedy-central-presents-daniel-tosh-2003-full-transcript/" xr:uid="{5110A35A-BE5F-4270-ACF1-CAA9724920A9}"/>
+    <hyperlink ref="A382" r:id="rId381" display="https://scrapsfromtheloft.com/comedy/george-carlin-religion-is-bullshit/" xr:uid="{D3F6A12D-F52F-4BFE-A704-D5E75264651D}"/>
+    <hyperlink ref="A383" r:id="rId382" display="https://scrapsfromtheloft.com/comedy/saturday-night-news-with-george-carlin-11-10-1984-transcript/" xr:uid="{BF1046CF-C48B-4AD1-8A8D-7F5470EEDE3B}"/>
+    <hyperlink ref="A384" r:id="rId383" display="https://scrapsfromtheloft.com/comedy/jim-jefferies-e-il-controllo-della-armi-in-america/" xr:uid="{D06F6EC6-66B9-4346-902B-80EF045873A6}"/>
+    <hyperlink ref="A385" r:id="rId384" display="https://scrapsfromtheloft.com/comedy/daniel-tosh-completely-serious-2007-full-transcript/" xr:uid="{61BE62B5-B917-456B-80FA-928DBABC7A15}"/>
+    <hyperlink ref="A386" r:id="rId385" display="https://scrapsfromtheloft.com/comedy/al-madrigal-why-is-the-rabbit-crying-2013-full-transcript/" xr:uid="{5DAC12C8-57CC-42D2-BC93-B00DB2A318E5}"/>
+    <hyperlink ref="A387" r:id="rId386" display="https://scrapsfromtheloft.com/comedy/neal-brennan-3-mics-2017-full-transcript/" xr:uid="{C1590D7F-099D-4439-9770-908CB2D5169C}"/>
+    <hyperlink ref="A388" r:id="rId387" display="https://scrapsfromtheloft.com/comedy/norm-macdonald-one-night-stand-1991/" xr:uid="{783AF5AE-573B-4FC0-A9D0-924E16B176CC}"/>
+    <hyperlink ref="A389" r:id="rId388" display="https://scrapsfromtheloft.com/comedy/john-mulaney-new-in-town-2012-full-transcript/" xr:uid="{C5875B2E-14F2-479F-AB7C-D687C4E565A9}"/>
+    <hyperlink ref="A390" r:id="rId389" display="https://scrapsfromtheloft.com/comedy/donald-glover-weirdo-transcript/" xr:uid="{5DC154C1-60BE-48E4-BB59-C72ED858DCE3}"/>
+    <hyperlink ref="A391" r:id="rId390" display="https://scrapsfromtheloft.com/comedy/ali-wong-baby-cobra-2016-full-transcript/" xr:uid="{1F40108F-861C-48EA-B60B-6C1EF7CD8A06}"/>
+    <hyperlink ref="A392" r:id="rId391" display="https://scrapsfromtheloft.com/comedy/norm-macdonald-hitlers-dog-gossip-trickery-2017-full-transcript/" xr:uid="{76C61EA1-97CB-4EB2-B0F7-86564191CD3A}"/>
+    <hyperlink ref="A393" r:id="rId392" display="https://scrapsfromtheloft.com/comedy/daniel-tosh-people-pleaser-2016-full-transcript/" xr:uid="{2DD4BB57-AB44-4D06-B156-ADF1A0438BE6}"/>
+    <hyperlink ref="A394" r:id="rId393" display="https://scrapsfromtheloft.com/comedy/marc-maron-more-later-2015-full-transcript/" xr:uid="{7E784723-47FB-4590-B86C-96ED6EDAD4B3}"/>
+    <hyperlink ref="A395" r:id="rId394" display="https://scrapsfromtheloft.com/comedy/dylan-moran-off-the-hook-2015-full-transcript/" xr:uid="{CBEAED70-4043-4D58-B320-40712C2B9C2F}"/>
+    <hyperlink ref="A396" r:id="rId395" display="https://scrapsfromtheloft.com/comedy/richard-pryor-live-and-smokin-1971-full-transcript/" xr:uid="{6D619A27-EF0B-4B00-BEE2-CDBB202C52E7}"/>
+    <hyperlink ref="A397" r:id="rId396" display="https://scrapsfromtheloft.com/movies/richard-pryor-here-and-now-1983/" xr:uid="{03FED81A-65DE-4DEE-AF80-1ABAD3D76D0A}"/>
+    <hyperlink ref="A398" r:id="rId397" display="https://scrapsfromtheloft.com/comedy/bill-burr-i-2008-testo-italiano-completo/" xr:uid="{9BAB76F7-7BB5-4D79-A1C2-15CEF3282C40}"/>
+    <hyperlink ref="A399" r:id="rId398" display="https://scrapsfromtheloft.com/movies/amy-schumer-mostly-sex-stuff-2012-full-transcript/" xr:uid="{6D56C838-9BD6-419D-9EC0-B41B90E95222}"/>
+    <hyperlink ref="A400" r:id="rId399" display="https://scrapsfromtheloft.com/comedy/jim-jefferies-alcoholocaust-2010-full-transcript/" xr:uid="{99C055C2-2095-45E0-BDF3-E61531DC469E}"/>
+    <hyperlink ref="A401" r:id="rId400" display="https://scrapsfromtheloft.com/movies/amy-schumer-live-apollo-2015-full-transcript/" xr:uid="{AC0B489C-87A9-4A37-A78C-26042120C4E0}"/>
+    <hyperlink ref="A402" r:id="rId401" display="https://scrapsfromtheloft.com/comedy/kevin-hart-seriously-funny-2010-full-transcript/" xr:uid="{AE7A32EB-F468-403E-B039-2EF8EC747F21}"/>
+    <hyperlink ref="A403" r:id="rId402" display="https://scrapsfromtheloft.com/comedy/hannibal-buress-comedy-camisado-2016-full-transcript/" xr:uid="{8AD18EEC-E969-4A45-80B5-520D6B17ACF8}"/>
+    <hyperlink ref="A404" r:id="rId403" display="https://scrapsfromtheloft.com/comedy/neal-brennan-women-and-black-dudes-transcript/" xr:uid="{45E25AC2-AA33-43C6-9F36-38AED1922C42}"/>
+    <hyperlink ref="A405" r:id="rId404" display="https://scrapsfromtheloft.com/comedy/nick-offerman-american-ham-2014-full-transcript/" xr:uid="{DDB69AFF-0D53-4EC9-8528-7755E435E3DC}"/>
+    <hyperlink ref="A406" r:id="rId405" display="https://scrapsfromtheloft.com/comedy/aziz-ansari-intimate-moments-sensual-evening-2010-full-transcript/" xr:uid="{F9974FBE-F1E5-4758-9E6A-94A13DAC2E80}"/>
+    <hyperlink ref="A407" r:id="rId406" display="https://scrapsfromtheloft.com/comedy/big-jay-oakerson-live-webster-hall-2016-full-transcript/" xr:uid="{EC4904A4-4BC3-4C2A-8924-685A2DC9FB3F}"/>
+    <hyperlink ref="A408" r:id="rId407" display="https://scrapsfromtheloft.com/comedy/lenny-bruce-berkeley-concert-1965-full-transcript/" xr:uid="{B84BFD44-5A06-491E-B7DA-1AEEAC2020C5}"/>
+    <hyperlink ref="A409" r:id="rId408" display="https://scrapsfromtheloft.com/comedy/doug-stanhope-no-refunds-2007-trascrizione-italiana/" xr:uid="{062B8D9B-BAF7-4410-9C9D-8520DD389CAC}"/>
+    <hyperlink ref="A410" r:id="rId409" display="https://scrapsfromtheloft.com/comedy/george-carlin-at-usc-1977-full-transcript/" xr:uid="{12B49538-F949-435F-A4B3-65F47B68FAF1}"/>
+    <hyperlink ref="A411" r:id="rId410" display="https://scrapsfromtheloft.com/comedy/jim-norton-mouthful-shame-transcript/" xr:uid="{DF4DEECA-DFBF-4EF6-A8D2-89B6163FD100}"/>
+    <hyperlink ref="A412" r:id="rId411" display="https://scrapsfromtheloft.com/comedy/michael-che-matters-transcript/" xr:uid="{3AC0F6CB-888E-428A-8E35-4DE6BAF287C7}"/>
+    <hyperlink ref="A413" r:id="rId412" display="https://scrapsfromtheloft.com/comedy/joe-rogan-triggered-2016-full-transcript/" xr:uid="{0BFE7F16-6112-43F1-A920-E37809D3A8A9}"/>
+    <hyperlink ref="A414" r:id="rId413" display="https://scrapsfromtheloft.com/comedy/trevor-noah-lost-translation-2015-full-transcript/" xr:uid="{0B578DB3-B37C-4F43-AC04-DEB576819DA5}"/>
+    <hyperlink ref="A415" r:id="rId414" display="https://scrapsfromtheloft.com/comedy/maria-bamford-old-baby-2017-full-transcript/" xr:uid="{5E8E36E9-07A3-462E-9278-2F6378ACD71E}"/>
+    <hyperlink ref="A416" r:id="rId415" display="https://scrapsfromtheloft.com/comedy/bo-burnham-what-transcript/" xr:uid="{AE2144FF-F24F-41F2-A968-CCBD7B67429E}"/>
+    <hyperlink ref="A417" r:id="rId416" display="https://scrapsfromtheloft.com/comedy/bo-burnham-make-happy-2016-full-transcript/" xr:uid="{B2713393-E87B-49C2-8512-F7F3EF26691A}"/>
+    <hyperlink ref="A418" r:id="rId417" display="https://scrapsfromtheloft.com/comedy/anthony-jeselnik-caligula-2013-full-transcript/" xr:uid="{135689C0-21CB-44E3-8996-CA9AF0F17076}"/>
+    <hyperlink ref="A419" r:id="rId418" display="https://scrapsfromtheloft.com/comedy/anthony-jeselnik-thoughts-prayers-2015-full-transcript/" xr:uid="{E79F2024-7A6B-419A-B891-5F184CF2177D}"/>
+    <hyperlink ref="A420" r:id="rId419" display="https://scrapsfromtheloft.com/comedy/john-mulaney-comeback-kid-2015-full-transcript/" xr:uid="{C5D8CE2F-AF50-4B97-9269-F25B4DDDCE44}"/>
+    <hyperlink ref="A421" r:id="rId420" display="https://scrapsfromtheloft.com/comedy/bill-hicks-revelations-1993-full-transcript/" xr:uid="{6A41967C-3B2A-4381-8A23-A74C6D0890CA}"/>
+    <hyperlink ref="A422" r:id="rId421" display="https://scrapsfromtheloft.com/comedy/lewis-black-black-future-2016-full-transcript/" xr:uid="{C756C6FC-B6B6-4F74-B19F-697985FA240A}"/>
+    <hyperlink ref="A423" r:id="rId422" display="https://scrapsfromtheloft.com/comedy/doug-stanhope-turning-gun-2012-transcript/" xr:uid="{22C9345C-248C-4D86-90F7-644013E0C300}"/>
+    <hyperlink ref="A424" r:id="rId423" display="https://scrapsfromtheloft.com/comedy/doug-stanhope-deadbeat-hero-2004-transcript/" xr:uid="{65328E0C-FA0A-4C0B-9941-DC520E0F272F}"/>
+    <hyperlink ref="A425" r:id="rId424" display="https://scrapsfromtheloft.com/comedy/jim-jefferies-contraband-2008-full-transcript/" xr:uid="{59A14800-2CBF-4DBD-B2F4-AFFFDEB06100}"/>
+    <hyperlink ref="A426" r:id="rId425" display="https://scrapsfromtheloft.com/comedy/mike-birbiglia-thank-god-jokes-2017-full-transcript/" xr:uid="{9D8B6073-982C-4936-92A8-B7F74E654229}"/>
+    <hyperlink ref="A427" r:id="rId426" display="https://scrapsfromtheloft.com/comedy/sarah-silverman-a-speck-of-dust-2017/" xr:uid="{CF2F767E-DB0F-4B15-9256-92F8C914C950}"/>
+    <hyperlink ref="A428" r:id="rId427" display="https://scrapsfromtheloft.com/comedy/george-carlin-playing-head-1986-full-transcript/" xr:uid="{6D843DE4-AC61-4324-91E4-C958775D7106}"/>
+    <hyperlink ref="A429" r:id="rId428" display="https://scrapsfromtheloft.com/comedy/george-carlin-1978-full-transcript/" xr:uid="{9D262801-A40A-4043-A42B-5BC855AB2723}"/>
+    <hyperlink ref="A430" r:id="rId429" display="https://scrapsfromtheloft.com/comedy/mitch-hedberg-comedy-central-special1999-full-transcript/" xr:uid="{857345E0-AB1A-4A73-B0FA-7A56EC37B033}"/>
+    <hyperlink ref="A431" r:id="rId430" display="https://scrapsfromtheloft.com/comedy/tom-segura-completely-normal-2014-full-transcript/" xr:uid="{925227BE-202B-4820-BAB9-1679EE3E259E}"/>
+    <hyperlink ref="A432" r:id="rId431" display="https://scrapsfromtheloft.com/comedy/george-carlin-carlin-campus-1984-full-transcript/" xr:uid="{CB32320F-853C-4E34-8C4C-FC8D9F7D74C3}"/>
+    <hyperlink ref="A433" r:id="rId432" display="https://scrapsfromtheloft.com/comedy/louis-c-k-live-at-the-beacon-theatre-2011-full-transcript/" xr:uid="{E3FE5A81-F91E-4D89-84CA-899192EF28AA}"/>
+    <hyperlink ref="A434" r:id="rId433" display="https://scrapsfromtheloft.com/comedy/ricky-gervais-england-2-2010-full-transcript/" xr:uid="{6E9A4494-2EC0-4A9A-9735-E49421BB2FCC}"/>
+    <hyperlink ref="A435" r:id="rId434" display="https://scrapsfromtheloft.com/comedy/amy-schumer-leather-special-2017-full-transcript/" xr:uid="{4BBE7954-4037-4621-862A-67111A7D286E}"/>
+    <hyperlink ref="A436" r:id="rId435" display="https://scrapsfromtheloft.com/comedy/jim-gaffigan-cinco-2017-full-transcript/" xr:uid="{8789260B-B720-4683-A3F1-E43BB97C0CBC}"/>
+    <hyperlink ref="A437" r:id="rId436" display="https://scrapsfromtheloft.com/comedy/jim-jefferies-i-swear-god-2009-full-transcript/" xr:uid="{D2F6658D-6D48-4EF4-BC09-BC1C368AF683}"/>
+    <hyperlink ref="A438" r:id="rId437" display="https://scrapsfromtheloft.com/comedy/louis-c-k-hilarious-2010-full-transcript/" xr:uid="{E47C6DBC-5220-436E-9EFC-8D13F8B20B66}"/>
+    <hyperlink ref="A439" r:id="rId438" display="https://scrapsfromtheloft.com/comedy/louis-c-k-shameless-2007-full-transcript/" xr:uid="{4E2FBE99-27CA-48B6-AC4E-7DDF22C77997}"/>
+    <hyperlink ref="A440" r:id="rId439" display="https://scrapsfromtheloft.com/comedy/bill-burr-im-sorry-feel-way-2014-full-transcript/" xr:uid="{96A7C660-FD88-4092-9533-00C100ABDF9F}"/>
+    <hyperlink ref="A441" r:id="rId440" display="https://scrapsfromtheloft.com/comedy/bill-burr-people-2012-full-transcript/" xr:uid="{67FF97FC-8FBB-4149-A0DD-731D13C977A4}"/>
+    <hyperlink ref="A442" r:id="rId441" display="https://scrapsfromtheloft.com/comedy/dave-chappelle-worth-2004-full-transcript/" xr:uid="{58E49691-5232-4995-A89A-D4580077F616}"/>
+    <hyperlink ref="A443" r:id="rId442" display="https://scrapsfromtheloft.com/comedy/dave-chappelle-killin-softly-2000-full-transcript/" xr:uid="{BFD91A7E-6520-4658-9435-AC2D1AC86123}"/>
+    <hyperlink ref="A444" r:id="rId443" display="https://scrapsfromtheloft.com/comedy/eddie-griffin-can-tell-em-i-said-transcript/" xr:uid="{760B74AE-6473-48BA-8DFB-EC7B02235782}"/>
+    <hyperlink ref="A445" r:id="rId444" display="https://scrapsfromtheloft.com/comedy/bill-burr-walk-way-2017-full-transcript/" xr:uid="{976AF3E2-C400-4042-9929-5BBC9AF8464B}"/>
+    <hyperlink ref="A446" r:id="rId445" display="https://scrapsfromtheloft.com/comedy/louis-ck-oh-my-god-full-transcript/" xr:uid="{73D79FB6-C8C4-4705-B544-F82AF76FB5AE}"/>
+    <hyperlink ref="A447" r:id="rId446" display="https://scrapsfromtheloft.com/comedy/louis-c-k-live-at-the-comedy-store-2015-transcript/" xr:uid="{AAA6CD50-3FFA-4581-8A9E-B834D434CEDA}"/>
+    <hyperlink ref="A448" r:id="rId447" display="https://scrapsfromtheloft.com/comedy/bill-hicks-relentless-1992-transcript/" xr:uid="{09FF7DDA-FF83-4316-A1E7-E682BC5DF708}"/>
+    <hyperlink ref="A449" r:id="rId448" display="https://scrapsfromtheloft.com/comedy/hasan-minhaj-white-house-correspondents-dinner-transcript/" xr:uid="{4EAEFEC6-5C59-4D76-8558-27C6B53B05D8}"/>
+    <hyperlink ref="A450" r:id="rId449" display="https://scrapsfromtheloft.com/comedy/daniel-tosh-happy-thoughts-transcript/" xr:uid="{DB7C35FE-BA61-4019-BF0F-F197C2F391A8}"/>
+    <hyperlink ref="A451" r:id="rId450" display="https://scrapsfromtheloft.com/comedy/patrice-oneal-elephant-in-the-room-2011-full-transcript/" xr:uid="{5B613BE4-4715-4178-8FFD-FB1FD10593DD}"/>
+    <hyperlink ref="A452" r:id="rId451" display="https://scrapsfromtheloft.com/comedy/katt-williams-live-2006-full-transcript/" xr:uid="{1AC2B586-766C-43D2-A24A-F07F5FDDCC54}"/>
+    <hyperlink ref="A453" r:id="rId452" display="https://scrapsfromtheloft.com/comedy/richard-pryor-live-concert-1979-full-transcript/" xr:uid="{8A370BA8-AA6F-4DC9-8CE4-9186163B9AF5}"/>
+    <hyperlink ref="A454" r:id="rId453" display="https://scrapsfromtheloft.com/comedy/richard-pryor-live-sunset-strip-1982-full-transcript/" xr:uid="{823116FC-B024-4026-B906-9C90958DB384}"/>
+    <hyperlink ref="A455" r:id="rId454" display="https://scrapsfromtheloft.com/comedy/george-carlin-seven-words-you-can-never-say-on-television/" xr:uid="{11DDEAA4-747B-412D-86BE-C95662CB5F13}"/>
+    <hyperlink ref="A456" r:id="rId455" display="https://scrapsfromtheloft.com/comedy/trevor-noah-afraid-dark-2017-full-transcript/" xr:uid="{36C7CC4C-A217-4E63-A455-63718D731197}"/>
+    <hyperlink ref="A457" r:id="rId456" display="https://scrapsfromtheloft.com/comedy/jim-jefferies-bare-2014-full-transcript/" xr:uid="{CC87369A-6A84-40AB-BE5D-D9132777A6B0}"/>
+    <hyperlink ref="A458" r:id="rId457" display="https://scrapsfromtheloft.com/comedy/dave-chappelle-deep-heart-texas-2017-full-transcript/" xr:uid="{42B3BA21-7F9C-411F-BDF6-F1E7ED7086E3}"/>
+    <hyperlink ref="A459" r:id="rId458" display="https://scrapsfromtheloft.com/comedy/tom-segura-mostly-stories-2016-full-transcript/" xr:uid="{617D29B0-5EC3-441A-9326-5C5AC6C92D69}"/>
+    <hyperlink ref="A460" r:id="rId459" display="https://scrapsfromtheloft.com/comedy/bill-burr-let-it-go-2010-full-transcript/" xr:uid="{A668F282-3C9D-41B4-B836-F7A86B147E60}"/>
+    <hyperlink ref="A461" r:id="rId460" display="https://scrapsfromtheloft.com/comedy/george-carlin-jamming-new-york-testo-italiano-completo/" xr:uid="{5B2E6B8C-DAFC-4BC1-9BC7-A3651811BBC3}"/>
+    <hyperlink ref="A462" r:id="rId461" display="https://scrapsfromtheloft.com/comedy/george-carlin-diseased-1999-testo-italiano-completo/" xr:uid="{DED2FA93-4C67-45E0-AF28-5BA6D547139D}"/>
+    <hyperlink ref="A463" r:id="rId462" display="https://scrapsfromtheloft.com/comedy/george-carlin-bad-2008-testo-italiano-completo/" xr:uid="{01609E28-E18B-4D89-BB16-8F8FA18EE461}"/>
+    <hyperlink ref="A464" r:id="rId463" display="https://scrapsfromtheloft.com/comedy/jim-jefferies-freedumb-2016-full-transcript/" xr:uid="{2F7DFF56-2F12-4630-BFC1-BDFEC387D6AC}"/>
+    <hyperlink ref="A465" r:id="rId464" display="https://scrapsfromtheloft.com/comedy/eddie-murphy-delirious-full-transcript/" xr:uid="{8847A120-0F0A-448D-A807-E956CC519E8C}"/>
+    <hyperlink ref="A466" r:id="rId465" display="https://scrapsfromtheloft.com/comedy/dave-chappelle-age-spin-2017-full-transcript/" xr:uid="{4BC8FFCD-9C6F-4C8E-A365-721DE32C0815}"/>
+    <hyperlink ref="A467" r:id="rId466" display="https://scrapsfromtheloft.com/comedy/george-carlin-back-town-1996-full-transcript/" xr:uid="{FC2E21C7-2076-48EA-8EBD-E49602DC4ED2}"/>
+    <hyperlink ref="A468" r:id="rId467" display="https://scrapsfromtheloft.com/comedy/seth-meyers-2011-white-house-correspondents-dinner-transcript/" xr:uid="{BDFFF244-CA5B-4DE0-B519-B765B516BB52}"/>
+    <hyperlink ref="A469" r:id="rId468" display="https://scrapsfromtheloft.com/comedy/louis-c-k-2017-full-transcript/" xr:uid="{327BD52E-54FF-46B0-A103-A519FDDBC596}"/>
+    <hyperlink ref="A470" r:id="rId469" display="https://scrapsfromtheloft.com/comedy/george-carlin-jamming-new-york-1992-full-transcript/" xr:uid="{A1A63194-040C-4649-820B-1EDD044CBE89}"/>
+    <hyperlink ref="A471" r:id="rId470" display="https://scrapsfromtheloft.com/comedy/jim-jefferies-gun-control-full-transcript/" xr:uid="{8E4EEC0B-06EB-4DD3-8001-98D29C1AA1CE}"/>
+    <hyperlink ref="A472" r:id="rId471" display="https://scrapsfromtheloft.com/comedy/reggie-watts-spatial-transcript/" xr:uid="{500DDC1D-EC71-441B-B053-9DB21BE42395}"/>
+    <hyperlink ref="A473" r:id="rId472" display="https://scrapsfromtheloft.com/comedy/george-carlin-complaints-grievances/" xr:uid="{E74E04DB-7E9B-4F98-8C5B-E5F9A12B3D09}"/>
+    <hyperlink ref="A474" r:id="rId473" display="https://scrapsfromtheloft.com/comedy/george-carlin-its-bad-for-ya/" xr:uid="{9AB3C2A7-B991-4877-8765-5258F6B45122}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>